<commit_message>
Stuff has been done
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>data</t>
   </si>
@@ -577,6 +577,9 @@
   <si>
     <t>Average</t>
   </si>
+  <si>
+    <t>Theoretical model</t>
+  </si>
 </sst>
 </file>
 
@@ -588,7 +591,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,8 +708,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,6 +830,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1185,7 +1208,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1214,8 +1237,28 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1544,9 +1587,6 @@
     <xf numFmtId="1" fontId="0" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="18" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="18" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1601,8 +1641,17 @@
     <xf numFmtId="11" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="48">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1617,6 +1666,16 @@
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1630,6 +1689,16 @@
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1984,40 +2053,49 @@
                   <c:v>0.0789725165104337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0687620762056475</c:v>
+                  <c:v>0.118458774765651</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0916827682741967</c:v>
+                  <c:v>0.157945033020867</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.114603460342746</c:v>
+                  <c:v>0.197431291276084</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.137524152411295</c:v>
+                  <c:v>0.236917549531301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.160444844479844</c:v>
+                  <c:v>0.276403807786518</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.183365536548393</c:v>
+                  <c:v>0.315890066041735</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.206286228616943</c:v>
+                  <c:v>0.355376324296952</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.229206920685492</c:v>
+                  <c:v>0.394862582552169</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.252127612754041</c:v>
+                  <c:v>0.434348840807385</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.27504830482259</c:v>
+                  <c:v>0.473835099062602</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.320889688959689</c:v>
+                  <c:v>0.552807615573036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.366731073096787</c:v>
+                  <c:v>0.63178013208347</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,28 +2350,52 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0218540554791565</c:v>
+                  <c:v>0.0302049478777284</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0437081109583129</c:v>
+                  <c:v>0.0604098957554567</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0655621664374694</c:v>
+                  <c:v>0.0906148436331851</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0874162219166258</c:v>
+                  <c:v>0.120819791510913</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.109270277395782</c:v>
+                  <c:v>0.151024739388642</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.131124332874939</c:v>
+                  <c:v>0.18122968726637</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.152978388354095</c:v>
+                  <c:v>0.211434635144099</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.174832443833252</c:v>
+                  <c:v>0.241639583021827</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2366,28 +2468,52 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0173607702142703</c:v>
+                  <c:v>0.0253163423467092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0347215404285405</c:v>
+                  <c:v>0.0506326846934183</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0520823106428108</c:v>
+                  <c:v>0.0759490270401275</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.069443080857081</c:v>
+                  <c:v>0.101265369386837</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0868038510713513</c:v>
+                  <c:v>0.126581711733546</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.104164621285622</c:v>
+                  <c:v>0.151898054080255</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.121525391499892</c:v>
+                  <c:v>0.177214396426964</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.138886161714162</c:v>
+                  <c:v>0.202530738773673</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2653,43 +2779,43 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>-0.00361916191487621</c:v>
+                  <c:v>-0.0367502942882115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00901570157213013</c:v>
+                  <c:v>-0.0406809969878728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.00612721271864132</c:v>
+                  <c:v>-0.0723894774653119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0123812381205239</c:v>
+                  <c:v>-0.0952090690538621</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0230797079668508</c:v>
+                  <c:v>-0.122473105086857</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0106662666312666</c:v>
+                  <c:v>-0.105292696675407</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00330113011827293</c:v>
+                  <c:v>-0.129223399375068</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.00961956195027627</c:v>
+                  <c:v>-0.158709657630285</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0314291429077144</c:v>
+                  <c:v>-0.197084804774391</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0165720571984858</c:v>
+                  <c:v>-0.19879328525183</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0127294729551872</c:v>
+                  <c:v>-0.186057321284825</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.029110311040311</c:v>
+                  <c:v>-0.202807615573036</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0432689269032125</c:v>
+                  <c:v>-0.22178013208347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3030,25 +3156,25 @@
                   <c:v>-0.00909383676661726</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00129188904168708</c:v>
+                  <c:v>-0.0154098957554567</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0200066108819138</c:v>
+                  <c:v>-0.0450592880776296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00369488919448527</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.00927027739578229</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.0100132217638276</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.00313272275701593</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0251675561667483</c:v>
+                  <c:v>-0.0297086803998024</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>-0.0510247393886419</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>-0.0601185761552591</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>-0.0553235240329875</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>-0.041639583021827</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3387,28 +3513,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.00152811867461863</c:v>
+                  <c:v>0.00642745345782028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00583265153965163</c:v>
+                  <c:v>0.0217437958045294</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.00791768935718921</c:v>
+                  <c:v>0.0159490270401275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.00611247469847452</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.000973926706426472</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.00527573239673269</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.00985872483322515</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.0100027271747268</c:v>
+                  <c:v>0.0257098138312811</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0.038803933955768</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.0530091651913661</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.0655477297602975</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.0536418498847844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5569,14 +5695,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>691562</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>191887</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>42476</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>343646</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>53575</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>96264</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5598,15 +5724,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>691563</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>170543</xdr:rowOff>
+      <xdr:colOff>659546</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>10459</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>386336</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>32231</xdr:rowOff>
+      <xdr:colOff>354319</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>64247</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5627,16 +5753,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>691562</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>181214</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19210</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>10457</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>407680</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>42902</xdr:rowOff>
+      <xdr:colOff>429025</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>64245</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5947,22 +6073,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="2"/>
+    <col min="1" max="2" width="9.1640625" style="2"/>
+    <col min="3" max="3" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10" style="2" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" style="2"/>
-    <col min="10" max="13" width="9.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.1640625" style="2" customWidth="1"/>
     <col min="14" max="14" width="9.33203125" style="2" customWidth="1"/>
     <col min="15" max="15" width="9.1640625" style="2" customWidth="1"/>
     <col min="16" max="16" width="9.1640625" style="2"/>
-    <col min="17" max="17" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.1640625" style="2"/>
     <col min="19" max="19" width="9.1640625" style="2" customWidth="1"/>
     <col min="20" max="23" width="9.1640625" style="2"/>
@@ -6618,7 +6746,7 @@
         <f t="shared" si="2"/>
         <v>15.284715284715286</v>
       </c>
-      <c r="H9" s="123">
+      <c r="H9" s="122">
         <v>11.7</v>
       </c>
       <c r="I9" s="1"/>
@@ -6673,7 +6801,7 @@
         <f t="shared" si="2"/>
         <v>16.583416583416586</v>
       </c>
-      <c r="H10" s="123">
+      <c r="H10" s="122">
         <v>12.2</v>
       </c>
       <c r="I10" s="1"/>
@@ -6777,7 +6905,7 @@
         <f t="shared" si="2"/>
         <v>17.582417582417587</v>
       </c>
-      <c r="H11" s="123">
+      <c r="H11" s="122">
         <v>12.5</v>
       </c>
       <c r="I11" s="1"/>
@@ -6832,7 +6960,7 @@
         <f t="shared" si="2"/>
         <v>17.582417582417587</v>
       </c>
-      <c r="H12" s="123">
+      <c r="H12" s="122">
         <v>12.7</v>
       </c>
       <c r="I12" s="1"/>
@@ -6936,7 +7064,7 @@
         <f t="shared" si="2"/>
         <v>21.178821178821181</v>
       </c>
-      <c r="H13" s="123">
+      <c r="H13" s="122">
         <v>13</v>
       </c>
       <c r="I13" s="1"/>
@@ -6991,7 +7119,7 @@
         <f t="shared" si="2"/>
         <v>25.674325674325676</v>
       </c>
-      <c r="H14" s="123">
+      <c r="H14" s="122">
         <v>13.2</v>
       </c>
       <c r="I14" s="1"/>
@@ -7095,7 +7223,7 @@
         <f t="shared" si="2"/>
         <v>31.268731268731273</v>
       </c>
-      <c r="H15" s="123">
+      <c r="H15" s="122">
         <v>13.5</v>
       </c>
       <c r="I15" s="1"/>
@@ -7199,7 +7327,7 @@
         <f t="shared" si="2"/>
         <v>36.463536463536471</v>
       </c>
-      <c r="H16" s="123">
+      <c r="H16" s="122">
         <v>13.6</v>
       </c>
       <c r="I16" s="1"/>
@@ -7322,21 +7450,27 @@
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="129" t="s">
+        <v>43</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
+      <c r="Q18" s="129" t="s">
+        <v>43</v>
+      </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -7455,20 +7589,20 @@
         <v>2</v>
       </c>
       <c r="J20" s="37">
-        <f>(PI()*$X$21*$X$22*I20*$X$26^4)/(8*$X$29*$M$38*100)*10^6</f>
-        <v>2.1854055479156458E-2</v>
+        <f>(PI()*$X$21*$X$22*I20*$X$26^4)/(8*$X$29*$X$31*100)*10^6</f>
+        <v>3.0204947877728372E-2</v>
       </c>
       <c r="K20" s="45">
         <f>M4-J20</f>
-        <v>-7.4294436804534653E-4</v>
+        <v>-9.0938367666172602E-3</v>
       </c>
       <c r="L20" s="40">
         <f>K20/N4</f>
-        <v>-0.12820834726314465</v>
+        <v>-1.5693042874748002</v>
       </c>
       <c r="M20" s="42">
         <f>L20^2</f>
-        <v>1.6437380307947089E-2</v>
+        <v>2.4627159466867905</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -7476,20 +7610,20 @@
         <v>2</v>
       </c>
       <c r="Q20" s="37">
-        <f>(PI()*$X$21*$X$22*P20*$X$25^4)/(8*$X$28*$T$38*100)*10^6</f>
-        <v>1.7360770214270259E-2</v>
+        <f>(PI()*$X$21*$X$22*P20*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
+        <v>2.5316342346709167E-2</v>
       </c>
       <c r="R20" s="45">
         <f>Q20-V4</f>
-        <v>-1.5281186746186302E-3</v>
+        <v>6.4274534578202779E-3</v>
       </c>
       <c r="S20" s="40">
         <f>R20/W4</f>
-        <v>-1.9260909009469158</v>
+        <v>8.1013731636105071</v>
       </c>
       <c r="T20" s="42">
         <f>S20^2</f>
-        <v>3.7098261587105017</v>
+        <v>65.632247136068514</v>
       </c>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -7519,35 +7653,41 @@
         <v>3</v>
       </c>
       <c r="C21" s="37">
-        <f t="shared" ref="C21:C34" si="15">(PI()*$X$21*$X$22*B21*$X$27^4)/(8*$X$30*$F$38*100)*10^6</f>
-        <v>6.876207620564756E-2</v>
+        <f t="shared" ref="C21:C34" si="15">(PI()*$X$21*$X$22*B21*$X$27^4)/(8*$X$30*$X$31*100)*10^6</f>
+        <v>0.11845877476565059</v>
       </c>
       <c r="D21" s="39">
         <f t="shared" ref="D21:D30" si="16">D5-C21</f>
-        <v>9.0157015721302192E-3</v>
+        <v>-4.0680996987872808E-2</v>
       </c>
       <c r="E21" s="41">
         <f t="shared" si="14"/>
-        <v>1.3919512770480569</v>
+        <v>-6.2808163353479545</v>
       </c>
       <c r="F21" s="43">
         <f t="shared" ref="F21:F34" si="17">E21^2</f>
-        <v>1.9375283576757163</v>
+        <v>39.448653838373708</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="109"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="113"/>
+      <c r="J21" s="37">
+        <f t="shared" ref="J21:J35" si="18">(PI()*$X$21*$X$22*I21*$X$26^4)/(8*$X$29*$X$31*100)*10^6</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="117"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="112"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="109"/>
-      <c r="Q21" s="110"/>
-      <c r="R21" s="121"/>
-      <c r="S21" s="122"/>
-      <c r="T21" s="113"/>
+      <c r="Q21" s="37">
+        <f t="shared" ref="Q21:Q35" si="19">(PI()*$X$21*$X$22*P21*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="120"/>
+      <c r="S21" s="121"/>
+      <c r="T21" s="112"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="6" t="s">
@@ -7577,19 +7717,19 @@
       </c>
       <c r="C22" s="37">
         <f t="shared" si="15"/>
-        <v>9.168276827419676E-2</v>
+        <v>0.15794503302086746</v>
       </c>
       <c r="D22" s="39">
         <f t="shared" si="16"/>
-        <v>-6.127212718641209E-3</v>
+        <v>-7.2389477465311908E-2</v>
       </c>
       <c r="E22" s="41">
         <f t="shared" si="14"/>
-        <v>-0.93196687900797737</v>
+        <v>-11.010650108672287</v>
       </c>
       <c r="F22" s="43">
         <f t="shared" si="17"/>
-        <v>0.86856226356786992</v>
+        <v>121.23441581560505</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -7597,20 +7737,20 @@
         <v>4</v>
       </c>
       <c r="J22" s="37">
-        <f>(PI()*$X$21*$X$22*I22*$X$26^4)/(8*$X$29*$M$38*100)*10^6</f>
-        <v>4.3708110958312917E-2</v>
+        <f t="shared" si="18"/>
+        <v>6.0409895755456744E-2</v>
       </c>
       <c r="K22" s="47">
         <f>M6-J22</f>
-        <v>1.2918890416870818E-3</v>
+        <v>-1.5409895755456746E-2</v>
       </c>
       <c r="L22" s="41">
         <f>K22/N6</f>
-        <v>0.21262387252020912</v>
+        <v>-2.5362175890733929</v>
       </c>
       <c r="M22" s="43">
-        <f t="shared" ref="M22:M34" si="18">L22^2</f>
-        <v>4.520891116549014E-2</v>
+        <f t="shared" ref="M22:M34" si="20">L22^2</f>
+        <v>6.4323996591252532</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -7618,20 +7758,20 @@
         <v>4</v>
       </c>
       <c r="Q22" s="37">
-        <f t="shared" ref="Q22:Q34" si="19">(PI()*$X$21*$X$22*P22*$X$25^4)/(8*$X$28*$T$38*100)*10^6</f>
-        <v>3.4721540428540518E-2</v>
+        <f t="shared" si="19"/>
+        <v>5.0632684693418334E-2</v>
       </c>
       <c r="R22" s="48">
         <f>Q22-V6</f>
-        <v>5.8326515396516267E-3</v>
+        <v>2.1743795804529443E-2</v>
       </c>
       <c r="S22" s="46">
         <f>R22/W6</f>
-        <v>6.2524477467208994</v>
+        <v>23.308772375472582</v>
       </c>
       <c r="T22" s="43">
-        <f t="shared" ref="T22:T34" si="20">S22^2</f>
-        <v>39.093102825475249</v>
+        <f t="shared" ref="T22:T34" si="21">S22^2</f>
+        <v>543.2988696515938</v>
       </c>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
@@ -7662,34 +7802,40 @@
       </c>
       <c r="C23" s="37">
         <f t="shared" si="15"/>
-        <v>0.11460346034274595</v>
+        <v>0.19743129127608433</v>
       </c>
       <c r="D23" s="39">
         <f t="shared" si="16"/>
-        <v>-1.2381238120523733E-2</v>
+        <v>-9.5209069053862116E-2</v>
       </c>
       <c r="E23" s="41">
         <f t="shared" si="14"/>
-        <v>-1.8245205852868913</v>
+        <v>-14.030172483866622</v>
       </c>
       <c r="F23" s="43">
         <f t="shared" si="17"/>
-        <v>3.3288753661356205</v>
+        <v>196.8457399270481</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="109"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="118"/>
-      <c r="L23" s="112"/>
-      <c r="M23" s="113"/>
+      <c r="J23" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="117"/>
+      <c r="L23" s="111"/>
+      <c r="M23" s="112"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="109"/>
-      <c r="Q23" s="110"/>
-      <c r="R23" s="121"/>
-      <c r="S23" s="122"/>
-      <c r="T23" s="113"/>
+      <c r="Q23" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="120"/>
+      <c r="S23" s="121"/>
+      <c r="T23" s="112"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="3" t="s">
@@ -7721,19 +7867,19 @@
       </c>
       <c r="C24" s="37">
         <f t="shared" si="15"/>
-        <v>0.13752415241129512</v>
+        <v>0.23691754953130117</v>
       </c>
       <c r="D24" s="39">
         <f t="shared" si="16"/>
-        <v>-2.3079707966850674E-2</v>
+        <v>-0.12247310508685673</v>
       </c>
       <c r="E24" s="41">
         <f t="shared" si="14"/>
-        <v>-3.3240303379805227</v>
+        <v>-17.639058409235997</v>
       </c>
       <c r="F24" s="43">
         <f t="shared" si="17"/>
-        <v>11.049177687814908</v>
+        <v>311.13638156443915</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -7741,20 +7887,20 @@
         <v>6</v>
       </c>
       <c r="J24" s="37">
-        <f t="shared" ref="J24:J34" si="21">(PI()*$X$21*$X$22*I24*$X$26^4)/(8*$X$29*$M$38*100)*10^6</f>
-        <v>6.5562166437469371E-2</v>
+        <f t="shared" si="18"/>
+        <v>9.061484363318513E-2</v>
       </c>
       <c r="K24" s="47">
         <f>M8-J24</f>
-        <v>-2.0006610881913821E-2</v>
+        <v>-4.5059288077629579E-2</v>
       </c>
       <c r="L24" s="41">
         <f>K24/N8</f>
-        <v>-3.2891581843130244</v>
+        <v>-7.4079076678516476</v>
       </c>
       <c r="M24" s="43">
-        <f t="shared" si="18"/>
-        <v>10.818561561433352</v>
+        <f t="shared" si="20"/>
+        <v>54.877096015415233</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -7763,19 +7909,19 @@
       </c>
       <c r="Q24" s="37">
         <f t="shared" si="19"/>
-        <v>5.208231064281079E-2</v>
+        <v>7.5949027040127501E-2</v>
       </c>
       <c r="R24" s="48">
         <f>Q24-V8</f>
-        <v>-7.9176893571892143E-3</v>
+        <v>1.5949027040127496E-2</v>
       </c>
       <c r="S24" s="46">
         <f>R24/W8</f>
-        <v>-5.6943020616657725</v>
+        <v>11.470338562057684</v>
       </c>
       <c r="T24" s="43">
-        <f t="shared" si="20"/>
-        <v>32.425075969491068</v>
+        <f t="shared" si="21"/>
+        <v>131.56866672822753</v>
       </c>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
@@ -7818,34 +7964,40 @@
       </c>
       <c r="C25" s="37">
         <f t="shared" si="15"/>
-        <v>0.16044484447984428</v>
+        <v>0.27640380778651807</v>
       </c>
       <c r="D25" s="39">
         <f t="shared" si="16"/>
-        <v>1.0666266631266824E-2</v>
+        <v>-0.10529269667540697</v>
       </c>
       <c r="E25" s="41">
         <f t="shared" si="14"/>
-        <v>1.3865328482235673</v>
+        <v>-13.687242937518132</v>
       </c>
       <c r="F25" s="43">
         <f t="shared" si="17"/>
-        <v>1.9224733392029578</v>
+        <v>187.34061923063999</v>
       </c>
       <c r="G25" s="36"/>
       <c r="H25" s="1"/>
       <c r="I25" s="109"/>
-      <c r="J25" s="110"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="112"/>
-      <c r="M25" s="113"/>
+      <c r="J25" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="117"/>
+      <c r="L25" s="111"/>
+      <c r="M25" s="112"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="109"/>
-      <c r="Q25" s="110"/>
-      <c r="R25" s="121"/>
-      <c r="S25" s="122"/>
-      <c r="T25" s="113"/>
+      <c r="Q25" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="120"/>
+      <c r="S25" s="121"/>
+      <c r="T25" s="112"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="3" t="s">
@@ -7885,19 +8037,19 @@
       </c>
       <c r="C26" s="37">
         <f t="shared" si="15"/>
-        <v>0.18336553654839352</v>
+        <v>0.31589006604173492</v>
       </c>
       <c r="D26" s="39">
         <f t="shared" si="16"/>
-        <v>3.3011301182731545E-3</v>
+        <v>-0.12922339937506824</v>
       </c>
       <c r="E26" s="41">
         <f t="shared" si="14"/>
-        <v>0.4176784639179309</v>
+        <v>-16.35010709043663</v>
       </c>
       <c r="F26" s="43">
         <f t="shared" si="17"/>
-        <v>0.1744552992208423</v>
+        <v>267.32600186874618</v>
       </c>
       <c r="G26" s="36"/>
       <c r="H26" s="1"/>
@@ -7905,20 +8057,20 @@
         <v>8</v>
       </c>
       <c r="J26" s="37">
-        <f t="shared" si="21"/>
-        <v>8.7416221916625833E-2</v>
+        <f t="shared" si="18"/>
+        <v>0.12081979151091349</v>
       </c>
       <c r="K26" s="47">
         <f>M10-J26</f>
-        <v>3.694889194485268E-3</v>
+        <v>-2.9708680399802387E-2</v>
       </c>
       <c r="L26" s="41">
         <f>K26/N10</f>
-        <v>0.5560729243108089</v>
+        <v>-4.4710928847312132</v>
       </c>
       <c r="M26" s="43">
-        <f t="shared" si="18"/>
-        <v>0.30921709715157458</v>
+        <f t="shared" si="20"/>
+        <v>19.99067158389408</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -7927,19 +8079,19 @@
       </c>
       <c r="Q26" s="37">
         <f t="shared" si="19"/>
-        <v>6.9443080857081035E-2</v>
+        <v>0.10126536938683667</v>
       </c>
       <c r="R26" s="48">
         <f>Q26-V10</f>
-        <v>-6.112474698474521E-3</v>
+        <v>2.5709813831281111E-2</v>
       </c>
       <c r="S26" s="46">
         <f>R26/W10</f>
-        <v>-3.7596889079521199</v>
+        <v>15.813709938317631</v>
       </c>
       <c r="T26" s="43">
-        <f t="shared" si="20"/>
-        <v>14.135260684578203</v>
+        <f t="shared" si="21"/>
+        <v>250.07342201324582</v>
       </c>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
@@ -7979,34 +8131,40 @@
       </c>
       <c r="C27" s="37">
         <f t="shared" si="15"/>
-        <v>0.20628622861694271</v>
+        <v>0.35537632429695182</v>
       </c>
       <c r="D27" s="39">
         <f t="shared" si="16"/>
-        <v>-9.619561950276051E-3</v>
+        <v>-0.15870965763028516</v>
       </c>
       <c r="E27" s="41">
         <f t="shared" si="14"/>
-        <v>-1.1964639984834193</v>
+        <v>-19.740024810674072</v>
       </c>
       <c r="F27" s="43">
         <f t="shared" si="17"/>
-        <v>1.4315260996669317</v>
+        <v>389.66857952602794</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="109"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="112"/>
-      <c r="M27" s="113"/>
+      <c r="J27" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="117"/>
+      <c r="L27" s="111"/>
+      <c r="M27" s="112"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="109"/>
-      <c r="Q27" s="110"/>
-      <c r="R27" s="121"/>
-      <c r="S27" s="122"/>
-      <c r="T27" s="113"/>
+      <c r="Q27" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="120"/>
+      <c r="S27" s="121"/>
+      <c r="T27" s="112"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="10" t="s">
@@ -8044,20 +8202,20 @@
         <v>10</v>
       </c>
       <c r="C28" s="37">
-        <f>(PI()*$X$21*$X$22*B28*$X$27^4)/(8*$X$30*$F$38*100)*10^6</f>
-        <v>0.22920692068549189</v>
+        <f t="shared" si="15"/>
+        <v>0.39486258255216866</v>
       </c>
       <c r="D28" s="39">
         <f t="shared" si="16"/>
-        <v>-3.1429142907714119E-2</v>
+        <v>-0.19708480477439089</v>
       </c>
       <c r="E28" s="41">
         <f t="shared" si="14"/>
-        <v>-3.901720068252065</v>
+        <v>-24.466774044514008</v>
       </c>
       <c r="F28" s="43">
         <f t="shared" si="17"/>
-        <v>15.223419491000898</v>
+        <v>598.62303214530436</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -8065,20 +8223,20 @@
         <v>10</v>
       </c>
       <c r="J28" s="37">
-        <f t="shared" si="21"/>
-        <v>0.10927027739578229</v>
+        <f t="shared" si="18"/>
+        <v>0.15102473938864189</v>
       </c>
       <c r="K28" s="47">
         <f>M12-J28</f>
-        <v>-9.2702773957822893E-3</v>
+        <v>-5.1024739388641882E-2</v>
       </c>
       <c r="L28" s="41">
         <f>K28/N12</f>
-        <v>-1.3718260855478752</v>
+        <v>-7.5506983786124611</v>
       </c>
       <c r="M28" s="43">
-        <f t="shared" si="18"/>
-        <v>1.8819068089896063</v>
+        <f t="shared" si="20"/>
+        <v>57.013046004780847</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -8086,20 +8244,20 @@
         <v>10</v>
       </c>
       <c r="Q28" s="37">
-        <f t="shared" si="19"/>
-        <v>8.6803851071351315E-2</v>
+        <f>(PI()*$X$21*$X$22*P28*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
+        <v>0.12658171173354582</v>
       </c>
       <c r="R28" s="48">
         <f>Q28-V12</f>
-        <v>-9.7392670642647283E-4</v>
+        <v>3.8803933955768033E-2</v>
       </c>
       <c r="S28" s="46">
         <f>R28/W12</f>
-        <v>-0.53740969993041221</v>
+        <v>21.411888970377245</v>
       </c>
       <c r="T28" s="43">
-        <f t="shared" si="20"/>
-        <v>0.28880918557929569</v>
+        <f>S28^2</f>
+        <v>458.4689892797627</v>
       </c>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
@@ -8138,34 +8296,40 @@
       </c>
       <c r="C29" s="37">
         <f t="shared" si="15"/>
-        <v>0.25212761275404105</v>
+        <v>0.43434884080738551</v>
       </c>
       <c r="D29" s="39">
         <f t="shared" si="16"/>
-        <v>-1.6572057198485507E-2</v>
+        <v>-0.19879328525182996</v>
       </c>
       <c r="E29" s="41">
         <f t="shared" si="14"/>
-        <v>-1.9320842186356622</v>
+        <v>-23.176686189624011</v>
       </c>
       <c r="F29" s="43">
         <f t="shared" si="17"/>
-        <v>3.7329494279009769</v>
+        <v>537.1587827323084</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="109"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="112"/>
-      <c r="M29" s="113"/>
+      <c r="J29" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="117"/>
+      <c r="L29" s="111"/>
+      <c r="M29" s="112"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="109"/>
-      <c r="Q29" s="110"/>
-      <c r="R29" s="121"/>
-      <c r="S29" s="122"/>
-      <c r="T29" s="113"/>
+      <c r="Q29" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="120"/>
+      <c r="S29" s="121"/>
+      <c r="T29" s="112"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="27" t="s">
@@ -8203,19 +8367,19 @@
       </c>
       <c r="C30" s="37">
         <f t="shared" si="15"/>
-        <v>0.27504830482259024</v>
+        <v>0.47383509906260235</v>
       </c>
       <c r="D30" s="39">
         <f t="shared" si="16"/>
-        <v>1.2729472955187504E-2</v>
+        <v>-0.18605732128482461</v>
       </c>
       <c r="E30" s="41">
         <f t="shared" si="14"/>
-        <v>1.3668806620581271</v>
+        <v>-19.978686894096679</v>
       </c>
       <c r="F30" s="43">
         <f t="shared" si="17"/>
-        <v>1.8683627443084638</v>
+        <v>399.1479300123504</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -8223,20 +8387,20 @@
         <v>12</v>
       </c>
       <c r="J30" s="37">
-        <f t="shared" si="21"/>
-        <v>0.13112433287493874</v>
+        <f t="shared" si="18"/>
+        <v>0.18122968726637026</v>
       </c>
       <c r="K30" s="47">
         <f>M14-J30</f>
-        <v>-1.0013221763827629E-2</v>
+        <v>-6.0118576155259146E-2</v>
       </c>
       <c r="L30" s="41">
         <f>K30/N14</f>
-        <v>-1.4243985780687414</v>
+        <v>-8.5519742207661515</v>
       </c>
       <c r="M30" s="43">
-        <f t="shared" si="18"/>
-        <v>2.0289113092042523</v>
+        <f t="shared" si="20"/>
+        <v>73.136263072648831</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -8245,19 +8409,19 @@
       </c>
       <c r="Q30" s="37">
         <f t="shared" si="19"/>
-        <v>0.10416462128562158</v>
+        <v>0.151898054080255</v>
       </c>
       <c r="R30" s="48">
         <f>Q30-V14</f>
-        <v>5.2757323967326936E-3</v>
+        <v>5.3009165191366114E-2</v>
       </c>
       <c r="S30" s="46">
         <f>R30/W14</f>
-        <v>2.6609976427792033</v>
+        <v>26.737001237454084</v>
       </c>
       <c r="T30" s="43">
-        <f t="shared" si="20"/>
-        <v>7.080908454876476</v>
+        <f t="shared" si="21"/>
+        <v>714.86723517162125</v>
       </c>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
@@ -8296,24 +8460,33 @@
     <row r="31" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="109"/>
-      <c r="C31" s="110"/>
-      <c r="D31" s="111"/>
-      <c r="E31" s="112"/>
-      <c r="F31" s="113"/>
+      <c r="C31" s="37">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="110"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="112"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="109"/>
-      <c r="J31" s="110"/>
-      <c r="K31" s="118"/>
-      <c r="L31" s="112"/>
-      <c r="M31" s="113"/>
+      <c r="J31" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="117"/>
+      <c r="L31" s="111"/>
+      <c r="M31" s="112"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="109"/>
-      <c r="Q31" s="110"/>
-      <c r="R31" s="121"/>
-      <c r="S31" s="122"/>
-      <c r="T31" s="113"/>
+      <c r="Q31" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R31" s="120"/>
+      <c r="S31" s="121"/>
+      <c r="T31" s="112"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="30" t="s">
@@ -8343,19 +8516,19 @@
       </c>
       <c r="C32" s="37">
         <f t="shared" si="15"/>
-        <v>0.32088968895968856</v>
+        <v>0.55280761557303615</v>
       </c>
       <c r="D32" s="39">
         <f>D15-C32</f>
-        <v>2.9110311040311421E-2</v>
+        <v>-0.20280761557303617</v>
       </c>
       <c r="E32" s="41">
         <f>D32/E15</f>
-        <v>2.8523851170862433</v>
+        <v>-19.872182866448959</v>
       </c>
       <c r="F32" s="43">
         <f t="shared" si="17"/>
-        <v>8.1361008561751014</v>
+        <v>394.90365187758755</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -8363,20 +8536,20 @@
         <v>14</v>
       </c>
       <c r="J32" s="37">
-        <f t="shared" si="21"/>
-        <v>0.15297838835409519</v>
+        <f t="shared" si="18"/>
+        <v>0.21143463514409863</v>
       </c>
       <c r="K32" s="47">
         <f>M15-J32</f>
-        <v>3.1327227570159266E-3</v>
+        <v>-5.5323524032987514E-2</v>
       </c>
       <c r="L32" s="41">
         <f>K32/N15</f>
-        <v>0.41817439273014062</v>
+        <v>-7.3849117399150295</v>
       </c>
       <c r="M32" s="43">
-        <f t="shared" si="18"/>
-        <v>0.17486982273522189</v>
+        <f t="shared" si="20"/>
+        <v>54.536921406334827</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -8384,20 +8557,20 @@
         <v>14</v>
       </c>
       <c r="Q32" s="37">
-        <f t="shared" si="19"/>
-        <v>0.12152539149989183</v>
+        <f>(PI()*$X$21*$X$22*P32*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
+        <v>0.17721439642696415</v>
       </c>
       <c r="R32" s="48">
         <f>Q32-V15</f>
-        <v>9.8587248332251548E-3</v>
+        <v>6.5547729760297477E-2</v>
       </c>
       <c r="S32" s="46">
         <f>R32/W15</f>
-        <v>4.5238957824448169</v>
+        <v>30.078037801815391</v>
       </c>
       <c r="T32" s="43">
-        <f t="shared" si="20"/>
-        <v>20.465633050422003</v>
+        <f t="shared" si="21"/>
+        <v>904.68835800743568</v>
       </c>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
@@ -8428,24 +8601,33 @@
     <row r="33" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="109"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="111"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="113"/>
+      <c r="C33" s="37">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="110"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="112"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="109"/>
-      <c r="J33" s="110"/>
-      <c r="K33" s="118"/>
-      <c r="L33" s="112"/>
-      <c r="M33" s="113"/>
+      <c r="J33" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="117"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="112"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="109"/>
-      <c r="Q33" s="110"/>
-      <c r="R33" s="121"/>
-      <c r="S33" s="122"/>
-      <c r="T33" s="113"/>
+      <c r="Q33" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R33" s="120"/>
+      <c r="S33" s="121"/>
+      <c r="T33" s="112"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
@@ -8464,26 +8646,26 @@
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="35">
         <v>16</v>
       </c>
       <c r="C34" s="37">
         <f t="shared" si="15"/>
-        <v>0.36673107309678704</v>
+        <v>0.63178013208346984</v>
       </c>
       <c r="D34" s="39">
         <f>D16-C34</f>
-        <v>4.3268926903212934E-2</v>
+        <v>-0.22178013208346986</v>
       </c>
       <c r="E34" s="41">
         <f>D34/E16</f>
-        <v>3.9052559542947569</v>
+        <v>-20.016862985777802</v>
       </c>
       <c r="F34" s="43">
         <f t="shared" si="17"/>
-        <v>15.251024068554653</v>
+        <v>400.67480379140142</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -8491,20 +8673,20 @@
         <v>16</v>
       </c>
       <c r="J34" s="37">
-        <f t="shared" si="21"/>
-        <v>0.17483244383325167</v>
+        <f t="shared" si="18"/>
+        <v>0.24163958302182698</v>
       </c>
       <c r="K34" s="44">
         <f>M16-J34</f>
-        <v>2.5167556166748345E-2</v>
+        <v>-4.1639583021826965E-2</v>
       </c>
       <c r="L34" s="46">
         <f>K34/N16</f>
-        <v>3.1126212932760091</v>
+        <v>-5.1498147813061266</v>
       </c>
       <c r="M34" s="43">
-        <f t="shared" si="18"/>
-        <v>9.688411315355216</v>
+        <f t="shared" si="20"/>
+        <v>26.520592281759068</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -8513,19 +8695,19 @@
       </c>
       <c r="Q34" s="37">
         <f t="shared" si="19"/>
-        <v>0.13888616171416207</v>
+        <v>0.20253073877367334</v>
       </c>
       <c r="R34" s="48">
         <f>Q34-V16</f>
-        <v>-1.0002727174726833E-2</v>
+        <v>5.3641849884784432E-2</v>
       </c>
       <c r="S34" s="46">
         <f>R34/W16</f>
-        <v>-3.6307180498306915</v>
+        <v>19.470533305664606</v>
       </c>
       <c r="T34" s="43">
-        <f t="shared" si="20"/>
-        <v>13.18211355736638</v>
+        <f t="shared" si="21"/>
+        <v>379.1016672069947</v>
       </c>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
@@ -8547,28 +8729,37 @@
     </row>
     <row r="35" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="116"/>
-      <c r="D35" s="115"/>
-      <c r="E35" s="116"/>
-      <c r="F35" s="117"/>
-      <c r="G35" s="125">
+      <c r="B35" s="113"/>
+      <c r="C35" s="37">
+        <f>(PI()*$X$21*$X$22*B35*$X$27^4)/(8*$X$30*$X$31*100)*10^6</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="114"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="116"/>
+      <c r="G35" s="124">
         <f>SUM(F20:F35)</f>
-        <v>101.91199617298797</v>
+        <v>3880.4961335015951</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="114"/>
-      <c r="J35" s="116"/>
-      <c r="K35" s="119"/>
-      <c r="L35" s="120"/>
-      <c r="M35" s="117"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="118"/>
+      <c r="L35" s="119"/>
+      <c r="M35" s="116"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="114"/>
-      <c r="Q35" s="116"/>
-      <c r="R35" s="119"/>
-      <c r="S35" s="120"/>
-      <c r="T35" s="117"/>
+      <c r="P35" s="113"/>
+      <c r="Q35" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R35" s="118"/>
+      <c r="S35" s="119"/>
+      <c r="T35" s="116"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
@@ -8597,7 +8788,7 @@
       </c>
       <c r="F36" s="54">
         <f>SUM(F20:F35)/11</f>
-        <v>9.2647269248170883</v>
+        <v>352.77237577287229</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -8609,7 +8800,7 @@
       </c>
       <c r="M36" s="54">
         <f>SUM(M20:M35)/6</f>
-        <v>4.1605873677237772</v>
+        <v>49.161617661774159</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -8620,7 +8811,7 @@
       </c>
       <c r="T36" s="54">
         <f>SUM(T20:T35)/6</f>
-        <v>21.730121647749865</v>
+        <v>574.61657586582498</v>
       </c>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
@@ -8641,54 +8832,63 @@
       <c r="AI36" s="1"/>
     </row>
     <row r="37" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="126">
+      <c r="B37" s="125">
         <f>AVERAGE(B20:B35)</f>
         <v>8.2307692307692299</v>
       </c>
-      <c r="C37" s="127">
+      <c r="C37" s="126">
         <f>AVERAGE(C20:C35)</f>
-        <v>0.19120347566985371</v>
+        <v>0.26406435208176277</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="128">
+      <c r="F37" s="127">
         <f>2.15384512*10^-3</f>
         <v>2.1538451200000001E-3</v>
       </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
+      <c r="G37" s="127">
+        <f>1.47803503*10^-3</f>
+        <v>1.47803503E-3</v>
+      </c>
+      <c r="H37" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="I37" s="126">
+      <c r="I37" s="125">
         <f>AVERAGE(I20:I35)</f>
         <v>9</v>
       </c>
-      <c r="J37" s="127">
+      <c r="J37" s="126">
         <f>AVERAGE(J20:J35)</f>
-        <v>9.8343249656204057E-2</v>
+        <v>6.7961132724888851E-2</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1" t="s">
+      <c r="N37" s="127">
+        <f>2.46907554*10^-3</f>
+        <v>2.4690755399999998E-3</v>
+      </c>
+      <c r="O37" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="P37" s="126">
+      <c r="P37" s="125">
         <f>AVERAGE(P20:P35)</f>
         <v>9</v>
       </c>
-      <c r="Q37" s="127">
+      <c r="Q37" s="126">
         <f>AVERAGE(Q20:Q35)</f>
-        <v>7.8123465964216182E-2</v>
+        <v>5.6961770280095622E-2</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
+      <c r="U37" s="127">
+        <f>2.46883066*10^-3</f>
+        <v>2.4688306599999999E-3</v>
+      </c>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
@@ -8711,7 +8911,7 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="124" t="s">
+      <c r="E38" s="123" t="s">
         <v>4</v>
       </c>
       <c r="F38" s="60">
@@ -8722,7 +8922,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="124" t="s">
+      <c r="L38" s="123" t="s">
         <v>4</v>
       </c>
       <c r="M38" s="60">
@@ -8733,7 +8933,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="124" t="s">
+      <c r="S38" s="123" t="s">
         <v>4</v>
       </c>
       <c r="T38" s="60">
@@ -9390,7 +9590,7 @@
         <v>2</v>
       </c>
       <c r="C64" s="94">
-        <v>-3.6191619148762122E-3</v>
+        <v>-3.6750294288211506E-2</v>
       </c>
       <c r="F64" s="93">
         <v>2</v>
@@ -9404,7 +9604,7 @@
         <v>2</v>
       </c>
       <c r="K64" s="94">
-        <v>-1.5281186746186302E-3</v>
+        <v>6.4274534578202779E-3</v>
       </c>
       <c r="L64" s="86"/>
       <c r="M64" s="80"/>
@@ -9418,13 +9618,13 @@
         <v>3</v>
       </c>
       <c r="C65" s="94">
-        <v>9.0157015721301359E-3</v>
+        <v>-4.0680996987872808E-2</v>
       </c>
       <c r="F65" s="93">
         <v>4</v>
       </c>
       <c r="G65" s="94">
-        <v>1.2918890416870818E-3</v>
+        <v>-1.5409895755456746E-2</v>
       </c>
       <c r="H65" s="82"/>
       <c r="I65" s="84"/>
@@ -9432,7 +9632,7 @@
         <v>4</v>
       </c>
       <c r="K65" s="94">
-        <v>5.8326515396516267E-3</v>
+        <v>2.1743795804529443E-2</v>
       </c>
       <c r="L65" s="86"/>
       <c r="M65" s="80"/>
@@ -9446,13 +9646,13 @@
         <v>4</v>
       </c>
       <c r="C66" s="94">
-        <v>-6.12721271864132E-3</v>
+        <v>-7.2389477465311908E-2</v>
       </c>
       <c r="F66" s="93">
         <v>6</v>
       </c>
       <c r="G66" s="94">
-        <v>-2.0006610881913821E-2</v>
+        <v>-4.5059288077629579E-2</v>
       </c>
       <c r="H66" s="82"/>
       <c r="I66" s="84"/>
@@ -9460,7 +9660,7 @@
         <v>6</v>
       </c>
       <c r="K66" s="94">
-        <v>-7.9176893571892143E-3</v>
+        <v>1.5949027040127496E-2</v>
       </c>
       <c r="L66" s="86"/>
       <c r="M66" s="80"/>
@@ -9474,13 +9674,13 @@
         <v>5</v>
       </c>
       <c r="C67" s="94">
-        <v>-1.2381238120523871E-2</v>
+        <v>-9.5209069053862116E-2</v>
       </c>
       <c r="F67" s="93">
         <v>8</v>
       </c>
       <c r="G67" s="94">
-        <v>3.694889194485268E-3</v>
+        <v>-2.9708680399802387E-2</v>
       </c>
       <c r="H67" s="82"/>
       <c r="I67" s="84"/>
@@ -9488,7 +9688,7 @@
         <v>8</v>
       </c>
       <c r="K67" s="94">
-        <v>-6.112474698474521E-3</v>
+        <v>2.5709813831281111E-2</v>
       </c>
       <c r="L67" s="86"/>
       <c r="M67" s="80"/>
@@ -9502,21 +9702,21 @@
         <v>6</v>
       </c>
       <c r="C68" s="94">
-        <v>-2.307970796685084E-2</v>
+        <v>-0.12247310508685673</v>
       </c>
       <c r="F68" s="93">
         <v>10</v>
       </c>
-      <c r="G68" s="94">
-        <v>-9.2702773957822893E-3</v>
+      <c r="G68" s="128">
+        <v>-5.1024739388641882E-2</v>
       </c>
       <c r="H68" s="82"/>
       <c r="I68" s="84"/>
       <c r="J68" s="93">
         <v>10</v>
       </c>
-      <c r="K68" s="94">
-        <v>-9.7392670642647283E-4</v>
+      <c r="K68" s="128">
+        <v>3.8803933955768033E-2</v>
       </c>
       <c r="L68" s="86"/>
       <c r="M68" s="80"/>
@@ -9530,21 +9730,21 @@
         <v>7</v>
       </c>
       <c r="C69" s="94">
-        <v>1.066626663126663E-2</v>
+        <v>-0.10529269667540697</v>
       </c>
       <c r="F69" s="93">
         <v>12</v>
       </c>
-      <c r="G69" s="94">
-        <v>-1.0013221763827629E-2</v>
+      <c r="G69" s="128">
+        <v>-6.0118576155259146E-2</v>
       </c>
       <c r="H69" s="82"/>
       <c r="I69" s="84"/>
       <c r="J69" s="93">
         <v>12</v>
       </c>
-      <c r="K69" s="94">
-        <v>5.2757323967326936E-3</v>
+      <c r="K69" s="128">
+        <v>5.3009165191366114E-2</v>
       </c>
       <c r="L69" s="86"/>
       <c r="M69" s="80"/>
@@ -9558,21 +9758,21 @@
         <v>8</v>
       </c>
       <c r="C70" s="94">
-        <v>3.3011301182729325E-3</v>
+        <v>-0.12922339937506824</v>
       </c>
       <c r="F70" s="93">
         <v>14</v>
       </c>
-      <c r="G70" s="94">
-        <v>3.1327227570159266E-3</v>
+      <c r="G70" s="128">
+        <v>-5.5323524032987514E-2</v>
       </c>
       <c r="H70" s="82"/>
       <c r="I70" s="84"/>
       <c r="J70" s="93">
         <v>14</v>
       </c>
-      <c r="K70" s="94">
-        <v>9.8587248332251548E-3</v>
+      <c r="K70" s="128">
+        <v>6.5547729760297477E-2</v>
       </c>
       <c r="L70" s="86"/>
       <c r="M70" s="80"/>
@@ -9586,21 +9786,21 @@
         <v>9</v>
       </c>
       <c r="C71" s="94">
-        <v>-9.619561950276273E-3</v>
+        <v>-0.15870965763028516</v>
       </c>
       <c r="F71" s="93">
         <v>16</v>
       </c>
-      <c r="G71" s="94">
-        <v>2.5167556166748345E-2</v>
+      <c r="G71" s="128">
+        <v>-4.1639583021826965E-2</v>
       </c>
       <c r="H71" s="82"/>
       <c r="I71" s="84"/>
       <c r="J71" s="93">
         <v>16</v>
       </c>
-      <c r="K71" s="94">
-        <v>-1.0002727174726833E-2</v>
+      <c r="K71" s="128">
+        <v>5.3641849884784432E-2</v>
       </c>
       <c r="L71" s="86"/>
       <c r="M71" s="80"/>
@@ -9614,7 +9814,7 @@
         <v>10</v>
       </c>
       <c r="C72" s="94">
-        <v>-3.1429142907714397E-2</v>
+        <v>-0.19708480477439089</v>
       </c>
       <c r="H72" s="82"/>
       <c r="I72" s="84"/>
@@ -9630,7 +9830,7 @@
         <v>11</v>
       </c>
       <c r="C73" s="94">
-        <v>-1.6572057198485785E-2</v>
+        <v>-0.19879328525182996</v>
       </c>
       <c r="F73" s="82"/>
       <c r="G73" s="84"/>
@@ -9650,14 +9850,12 @@
         <v>12</v>
       </c>
       <c r="C74" s="94">
-        <v>1.2729472955187171E-2</v>
+        <v>-0.18605732128482461</v>
       </c>
       <c r="F74" s="80"/>
-      <c r="G74" s="80"/>
       <c r="H74" s="82"/>
       <c r="I74" s="84"/>
       <c r="J74" s="80"/>
-      <c r="K74" s="80"/>
       <c r="L74" s="86"/>
       <c r="M74" s="80"/>
       <c r="N74" s="80"/>
@@ -9670,7 +9868,7 @@
         <v>14</v>
       </c>
       <c r="C75" s="94">
-        <v>2.9110311040311032E-2</v>
+        <v>-0.20280761557303617</v>
       </c>
       <c r="F75" s="82"/>
       <c r="G75" s="84"/>
@@ -9690,14 +9888,12 @@
         <v>16</v>
       </c>
       <c r="C76" s="94">
-        <v>4.326892690321249E-2</v>
+        <v>-0.22178013208346986</v>
       </c>
       <c r="F76" s="80"/>
-      <c r="G76" s="80"/>
       <c r="H76" s="81"/>
       <c r="I76" s="81"/>
       <c r="J76" s="80"/>
-      <c r="K76" s="80"/>
       <c r="L76" s="81"/>
       <c r="M76" s="80"/>
       <c r="N76" s="80"/>
@@ -9716,7 +9912,6 @@
       <c r="H77" s="80"/>
       <c r="I77" s="80"/>
       <c r="J77" s="82"/>
-      <c r="K77" s="84"/>
       <c r="L77" s="80"/>
       <c r="M77" s="80"/>
     </row>
@@ -9727,11 +9922,9 @@
       <c r="D78" s="80"/>
       <c r="E78" s="80"/>
       <c r="F78" s="80"/>
-      <c r="G78" s="80"/>
       <c r="H78" s="80"/>
       <c r="I78" s="80"/>
       <c r="J78" s="80"/>
-      <c r="K78" s="80"/>
       <c r="L78" s="80"/>
       <c r="M78" s="80"/>
     </row>

</xml_diff>

<commit_message>
data analysis, more method
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="14680"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
   <si>
     <t>data</t>
   </si>
@@ -580,6 +580,9 @@
   <si>
     <t>Theoretical model</t>
   </si>
+  <si>
+    <t>Average Temp</t>
+  </si>
 </sst>
 </file>
 
@@ -839,7 +842,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1190,15 +1193,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color auto="1"/>
@@ -1208,7 +1202,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1257,8 +1251,22 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1425,10 +1433,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1521,15 +1526,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1650,8 +1646,29 @@
     <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="17" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="11" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="62">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1676,6 +1693,13 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1699,6 +1723,13 @@
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2050,49 +2081,49 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0789725165104337</c:v>
+                  <c:v>0.0404830578141262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.118458774765651</c:v>
+                  <c:v>0.0607245867211894</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.157945033020867</c:v>
+                  <c:v>0.0809661156282525</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.197431291276084</c:v>
+                  <c:v>0.101207644535316</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.236917549531301</c:v>
+                  <c:v>0.121449173442379</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.276403807786518</c:v>
+                  <c:v>0.141690702349442</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.315890066041735</c:v>
+                  <c:v>0.161932231256505</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.355376324296952</c:v>
+                  <c:v>0.182173760163568</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.394862582552169</c:v>
+                  <c:v>0.202415289070631</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.434348840807385</c:v>
+                  <c:v>0.222656817977694</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.473835099062602</c:v>
+                  <c:v>0.242898346884758</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.552807615573036</c:v>
+                  <c:v>0.283381404698884</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63178013208347</c:v>
+                  <c:v>0.32386446251301</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.0</c:v>
@@ -2125,6 +2156,78 @@
               </a:ln>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Data!$N$4:$N$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>0.00579482057061753</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00607593600085659</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00608259310158183</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.00664461266310471</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.00675761854468597</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.00702978921630487</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.0074914265710133</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0.00808564672519466</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Data!$N$4:$N$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>0.00579482057061753</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00607593600085659</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00608259310158183</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.00664461266310471</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.00675761854468597</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.00702978921630487</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.0074914265710133</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0.00808564672519466</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Data!$K$4:$K$16</c:f>
@@ -2216,6 +2319,78 @@
               </a:ln>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Data!$W$4:$W$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>0.000793378274030248</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.000932858901973321</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00139045826361958</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.00162579267809792</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.00181226112322235</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.00198261445704349</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.0021792555150104</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0.00275502725285795</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Data!$W$4:$W$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>0.000793378274030248</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.000932858901973321</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00139045826361958</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.00162579267809792</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.00181226112322235</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.00198261445704349</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.0021792555150104</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0.00275502725285795</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Data!$T$4:$T$16</c:f>
@@ -2350,49 +2525,49 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0302049478777284</c:v>
+                  <c:v>0.0201584041427971</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0604098957554567</c:v>
+                  <c:v>0.0403168082855942</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0906148436331851</c:v>
+                  <c:v>0.0604752124283912</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.120819791510913</c:v>
+                  <c:v>0.0806336165711883</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.151024739388642</c:v>
+                  <c:v>0.100792020713985</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18122968726637</c:v>
+                  <c:v>0.120950424856783</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.211434635144099</c:v>
+                  <c:v>0.14110882899958</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.241639583021827</c:v>
+                  <c:v>0.161267233142377</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.0</c:v>
@@ -2468,49 +2643,49 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0253163423467092</c:v>
+                  <c:v>0.0181364494301323</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0506326846934183</c:v>
+                  <c:v>0.0362728988602646</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0759490270401275</c:v>
+                  <c:v>0.054409348290397</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.101265369386837</c:v>
+                  <c:v>0.0725457977205293</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.126581711733546</c:v>
+                  <c:v>0.0906822471506616</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.151898054080255</c:v>
+                  <c:v>0.108818696580794</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.177214396426964</c:v>
+                  <c:v>0.126955146010926</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.202530738773673</c:v>
+                  <c:v>0.145091595441059</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.0</c:v>
@@ -2528,11 +2703,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1680730592"/>
-        <c:axId val="1678716304"/>
+        <c:axId val="806208000"/>
+        <c:axId val="771343632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1680730592"/>
+        <c:axId val="806208000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2561,12 +2736,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1678716304"/>
+        <c:crossAx val="771343632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1678716304"/>
+        <c:axId val="771343632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2595,7 +2770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1680730592"/>
+        <c:crossAx val="806208000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2774,48 +2949,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$C$64:$C$76</c:f>
+              <c:f>Data!$C$64:$C$75</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>-0.0367502942882115</c:v>
+                  <c:v>0.00173916440809597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.0406809969878728</c:v>
+                  <c:v>0.0170531910565884</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0723894774653119</c:v>
+                  <c:v>0.00458943992730304</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0952090690538621</c:v>
+                  <c:v>0.00101457768690658</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.122473105086857</c:v>
+                  <c:v>-0.00700472899793432</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.105292696675407</c:v>
+                  <c:v>0.0294204087616692</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.129223399375068</c:v>
+                  <c:v>0.0247344354101616</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.158709657630285</c:v>
+                  <c:v>0.0144929065030985</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.197084804774391</c:v>
+                  <c:v>-0.0046375112928535</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.19879328525183</c:v>
+                  <c:v>0.0128987375778612</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.186057321284825</c:v>
+                  <c:v>0.0448794308930202</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.202807615573036</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-0.22178013208347</c:v>
+                  <c:v>0.0666185953011162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2830,11 +3002,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1678731152"/>
-        <c:axId val="1678733200"/>
+        <c:axId val="771481776"/>
+        <c:axId val="771484256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1678731152"/>
+        <c:axId val="771481776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2890,12 +3062,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1678733200"/>
+        <c:crossAx val="771484256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1678733200"/>
+        <c:axId val="771484256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,7 +3123,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1678731152"/>
+        <c:crossAx val="771481776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3153,28 +3325,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.00909383676661726</c:v>
+                  <c:v>0.00095270696831402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.0154098957554567</c:v>
+                  <c:v>0.00468319171440581</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0450592880776296</c:v>
+                  <c:v>-0.0149196568728357</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0297086803998024</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>-0.0510247393886419</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>-0.0601185761552591</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>-0.0553235240329875</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>-0.041639583021827</c:v>
+                  <c:v>0.0104774945399227</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.000792020713985444</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.000160686254328593</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0150022821115315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0387327668576233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3189,11 +3361,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1679648080"/>
-        <c:axId val="1679650128"/>
+        <c:axId val="806153584"/>
+        <c:axId val="806149728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1679648080"/>
+        <c:axId val="806153584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3250,12 +3422,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1679650128"/>
+        <c:crossAx val="806149728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1679650128"/>
+        <c:axId val="806149728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3311,7 +3483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1679648080"/>
+        <c:crossAx val="806153584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3513,28 +3685,28 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.00642745345782028</c:v>
+                  <c:v>-0.000752439458756561</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0217437958045294</c:v>
+                  <c:v>0.00738400997137576</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0159490270401275</c:v>
+                  <c:v>-0.00559065170960301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0257098138312811</c:v>
+                  <c:v>-0.00300975783502624</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>0.038803933955768</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>0.0530091651913661</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.0655477297602975</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>0.0536418498847844</c:v>
+                <c:pt idx="5">
+                  <c:v>0.00290446937288387</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0099298076919051</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0152884793442596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3549,11 +3721,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1680764368"/>
-        <c:axId val="1680766848"/>
+        <c:axId val="806129312"/>
+        <c:axId val="806119264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1680764368"/>
+        <c:axId val="806129312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3573,6 +3745,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3609,12 +3782,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1680766848"/>
+        <c:crossAx val="806119264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1680766848"/>
+        <c:axId val="806119264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3670,7 +3843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1680764368"/>
+        <c:crossAx val="806129312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6073,8 +6246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6082,20 +6255,20 @@
     <col min="1" max="2" width="9.1640625" style="2"/>
     <col min="3" max="3" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" style="2"/>
     <col min="10" max="10" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="9.1640625" style="2" customWidth="1"/>
     <col min="14" max="14" width="9.33203125" style="2" customWidth="1"/>
     <col min="15" max="15" width="9.1640625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.1640625" style="2"/>
+    <col min="16" max="16" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.1640625" style="2"/>
     <col min="19" max="19" width="9.1640625" style="2" customWidth="1"/>
     <col min="20" max="23" width="9.1640625" style="2"/>
     <col min="24" max="24" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1640625" style="2"/>
+    <col min="25" max="25" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="9.1640625" style="2"/>
   </cols>
@@ -6132,151 +6305,151 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:36" s="72" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="73" t="s">
+    <row r="2" spans="1:36" s="71" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="68"/>
+      <c r="B2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="73" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="74"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="73" t="s">
+      <c r="L2" s="73"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="74"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
-      <c r="AC2" s="69"/>
-      <c r="AD2" s="73" t="s">
+      <c r="U2" s="73"/>
+      <c r="V2" s="68"/>
+      <c r="W2" s="68"/>
+      <c r="X2" s="68"/>
+      <c r="Y2" s="68"/>
+      <c r="Z2" s="68"/>
+      <c r="AA2" s="68"/>
+      <c r="AB2" s="68"/>
+      <c r="AC2" s="68"/>
+      <c r="AD2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="AE2" s="74"/>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="69"/>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="69"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="68"/>
+      <c r="AG2" s="68"/>
+      <c r="AH2" s="68"/>
+      <c r="AI2" s="68"/>
+      <c r="AJ2" s="68"/>
     </row>
-    <row r="3" spans="1:36" s="72" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62" t="s">
+    <row r="3" spans="1:36" s="71" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="69"/>
-      <c r="J3" s="62" t="s">
+      <c r="I3" s="68"/>
+      <c r="J3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="65" t="s">
+      <c r="M3" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="66" t="s">
+      <c r="N3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="67" t="s">
+      <c r="O3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="68" t="s">
+      <c r="P3" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="98" t="s">
+      <c r="Q3" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="69"/>
-      <c r="S3" s="62" t="s">
+      <c r="R3" s="68"/>
+      <c r="S3" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="63" t="s">
+      <c r="T3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="64" t="s">
+      <c r="U3" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="65" t="s">
+      <c r="V3" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="66" t="s">
+      <c r="W3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="67" t="s">
+      <c r="X3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="68" t="s">
+      <c r="Y3" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="98" t="s">
+      <c r="Z3" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="AA3" s="69"/>
-      <c r="AB3" s="69"/>
-      <c r="AC3" s="62" t="s">
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="AD3" s="70" t="s">
+      <c r="AD3" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="AE3" s="71" t="s">
+      <c r="AE3" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="AF3" s="65" t="s">
+      <c r="AF3" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="AG3" s="66" t="s">
+      <c r="AG3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="AH3" s="67" t="s">
+      <c r="AH3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="AI3" s="68" t="s">
+      <c r="AI3" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="AJ3" s="61" t="s">
+      <c r="AJ3" s="60" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6305,7 +6478,7 @@
         <f t="shared" ref="G4:G16" si="2">F4/1.001</f>
         <v>4.1958041958041967</v>
       </c>
-      <c r="H4" s="99"/>
+      <c r="H4" s="95"/>
       <c r="I4" s="1"/>
       <c r="J4" s="14" t="s">
         <v>16</v>
@@ -6415,29 +6588,29 @@
         <f t="shared" si="2"/>
         <v>6.7932067932067941</v>
       </c>
-      <c r="H5" s="100"/>
+      <c r="H5" s="96"/>
       <c r="I5" s="1"/>
       <c r="J5" s="53">
         <v>0.05</v>
       </c>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="100"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="96"/>
       <c r="R5" s="1"/>
       <c r="S5" s="53">
         <v>0.05</v>
       </c>
-      <c r="T5" s="107"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="104"/>
-      <c r="X5" s="105"/>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="100"/>
+      <c r="T5" s="103"/>
+      <c r="U5" s="104"/>
+      <c r="V5" s="99"/>
+      <c r="W5" s="100"/>
+      <c r="X5" s="101"/>
+      <c r="Y5" s="102"/>
+      <c r="Z5" s="96"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="53">
@@ -6476,7 +6649,7 @@
         <f t="shared" si="2"/>
         <v>7.4925074925074933</v>
       </c>
-      <c r="H6" s="100"/>
+      <c r="H6" s="96"/>
       <c r="I6" s="1"/>
       <c r="J6" s="15" t="s">
         <v>6</v>
@@ -6586,29 +6759,29 @@
         <f t="shared" si="2"/>
         <v>8.5914085914085927</v>
       </c>
-      <c r="H7" s="100"/>
+      <c r="H7" s="96"/>
       <c r="I7" s="1"/>
       <c r="J7" s="53">
         <v>0.5</v>
       </c>
-      <c r="K7" s="101"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="104"/>
-      <c r="O7" s="105"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="100"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="102"/>
+      <c r="Q7" s="96"/>
       <c r="R7" s="1"/>
       <c r="S7" s="53">
         <v>0.05</v>
       </c>
-      <c r="T7" s="107"/>
-      <c r="U7" s="108"/>
-      <c r="V7" s="103"/>
-      <c r="W7" s="104"/>
-      <c r="X7" s="105"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="100"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="99"/>
+      <c r="W7" s="100"/>
+      <c r="X7" s="101"/>
+      <c r="Y7" s="102"/>
+      <c r="Z7" s="96"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="53">
@@ -6645,7 +6818,7 @@
         <f t="shared" si="2"/>
         <v>10.589410589410591</v>
       </c>
-      <c r="H8" s="100"/>
+      <c r="H8" s="96"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="50">
@@ -6746,27 +6919,27 @@
         <f t="shared" si="2"/>
         <v>15.284715284715286</v>
       </c>
-      <c r="H9" s="122">
+      <c r="H9" s="118">
         <v>11.7</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="100"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="101"/>
+      <c r="P9" s="102"/>
+      <c r="Q9" s="96"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="107"/>
-      <c r="U9" s="108"/>
-      <c r="V9" s="103"/>
-      <c r="W9" s="104"/>
-      <c r="X9" s="105"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="100"/>
+      <c r="T9" s="103"/>
+      <c r="U9" s="104"/>
+      <c r="V9" s="99"/>
+      <c r="W9" s="100"/>
+      <c r="X9" s="101"/>
+      <c r="Y9" s="102"/>
+      <c r="Z9" s="96"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
@@ -6801,7 +6974,7 @@
         <f t="shared" si="2"/>
         <v>16.583416583416586</v>
       </c>
-      <c r="H10" s="122">
+      <c r="H10" s="118">
         <v>12.2</v>
       </c>
       <c r="I10" s="1"/>
@@ -6905,27 +7078,27 @@
         <f t="shared" si="2"/>
         <v>17.582417582417587</v>
       </c>
-      <c r="H11" s="122">
+      <c r="H11" s="118">
         <v>12.5</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="102"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="104"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="100"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="99"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="101"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="96"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="107"/>
-      <c r="U11" s="108"/>
-      <c r="V11" s="103"/>
-      <c r="W11" s="104"/>
-      <c r="X11" s="105"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="100"/>
+      <c r="T11" s="103"/>
+      <c r="U11" s="104"/>
+      <c r="V11" s="99"/>
+      <c r="W11" s="100"/>
+      <c r="X11" s="101"/>
+      <c r="Y11" s="102"/>
+      <c r="Z11" s="96"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
@@ -6960,7 +7133,7 @@
         <f t="shared" si="2"/>
         <v>17.582417582417587</v>
       </c>
-      <c r="H12" s="122">
+      <c r="H12" s="118">
         <v>12.7</v>
       </c>
       <c r="I12" s="1"/>
@@ -7064,27 +7237,27 @@
         <f t="shared" si="2"/>
         <v>21.178821178821181</v>
       </c>
-      <c r="H13" s="122">
+      <c r="H13" s="118">
         <v>13</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="103"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="105"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="100"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="96"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="107"/>
-      <c r="U13" s="108"/>
-      <c r="V13" s="103"/>
-      <c r="W13" s="104"/>
-      <c r="X13" s="105"/>
-      <c r="Y13" s="106"/>
-      <c r="Z13" s="100"/>
+      <c r="T13" s="103"/>
+      <c r="U13" s="104"/>
+      <c r="V13" s="99"/>
+      <c r="W13" s="100"/>
+      <c r="X13" s="101"/>
+      <c r="Y13" s="102"/>
+      <c r="Z13" s="96"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
@@ -7119,7 +7292,7 @@
         <f t="shared" si="2"/>
         <v>25.674325674325676</v>
       </c>
-      <c r="H14" s="122">
+      <c r="H14" s="118">
         <v>13.2</v>
       </c>
       <c r="I14" s="1"/>
@@ -7223,7 +7396,7 @@
         <f t="shared" si="2"/>
         <v>31.268731268731273</v>
       </c>
-      <c r="H15" s="122">
+      <c r="H15" s="118">
         <v>13.5</v>
       </c>
       <c r="I15" s="1"/>
@@ -7327,7 +7500,7 @@
         <f t="shared" si="2"/>
         <v>36.463536463536471</v>
       </c>
-      <c r="H16" s="122">
+      <c r="H16" s="118">
         <v>13.6</v>
       </c>
       <c r="I16" s="1"/>
@@ -7415,8 +7588,13 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="127">
+        <f>AVERAGE(H9:H16)</f>
+        <v>12.799999999999999</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -7424,8 +7602,13 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="P17" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17" s="127">
+        <f>AVERAGE(Q4:Q16)</f>
+        <v>12.662500000000001</v>
+      </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -7433,8 +7616,13 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+      <c r="Y17" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z17" s="127">
+        <f>AVERAGE(Z4:Z16)</f>
+        <v>12.375</v>
+      </c>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
@@ -7459,7 +7647,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="129" t="s">
+      <c r="J18" s="125" t="s">
         <v>43</v>
       </c>
       <c r="K18" s="1"/>
@@ -7468,7 +7656,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="129" t="s">
+      <c r="Q18" s="125" t="s">
         <v>43</v>
       </c>
       <c r="R18" s="1"/>
@@ -7490,77 +7678,77 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
     </row>
-    <row r="19" spans="1:35" s="72" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="69" t="s">
+    <row r="19" spans="1:35" s="71" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="77" t="s">
+      <c r="D19" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="78" t="s">
+      <c r="E19" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="79" t="s">
+      <c r="F19" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69" t="s">
+      <c r="G19" s="68"/>
+      <c r="H19" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="75" t="s">
+      <c r="I19" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="76" t="s">
+      <c r="J19" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="77" t="s">
+      <c r="K19" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="78" t="s">
+      <c r="L19" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="M19" s="79" t="s">
+      <c r="M19" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69" t="s">
+      <c r="N19" s="68"/>
+      <c r="O19" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="P19" s="75" t="s">
+      <c r="P19" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="Q19" s="76" t="s">
+      <c r="Q19" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="R19" s="77" t="s">
+      <c r="R19" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="S19" s="78" t="s">
+      <c r="S19" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="T19" s="79" t="s">
+      <c r="T19" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="U19" s="69"/>
-      <c r="V19" s="69"/>
-      <c r="X19" s="69"/>
-      <c r="Y19" s="69"/>
-      <c r="Z19" s="69"/>
-      <c r="AA19" s="69"/>
-      <c r="AB19" s="69"/>
-      <c r="AC19" s="69"/>
-      <c r="AD19" s="69"/>
-      <c r="AE19" s="69"/>
-      <c r="AF19" s="69"/>
-      <c r="AG19" s="69"/>
-      <c r="AH19" s="69"/>
-      <c r="AI19" s="69"/>
+      <c r="U19" s="68"/>
+      <c r="V19" s="68"/>
+      <c r="X19" s="68"/>
+      <c r="Y19" s="68"/>
+      <c r="Z19" s="68"/>
+      <c r="AA19" s="68"/>
+      <c r="AB19" s="68"/>
+      <c r="AC19" s="68"/>
+      <c r="AD19" s="68"/>
+      <c r="AE19" s="68"/>
+      <c r="AF19" s="68"/>
+      <c r="AG19" s="68"/>
+      <c r="AH19" s="68"/>
+      <c r="AI19" s="68"/>
     </row>
     <row r="20" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -7569,19 +7757,19 @@
       </c>
       <c r="C20" s="37">
         <f>(PI()*$X$21*$X$22*B20*$X$27^4)/(8*$X$30*$X$31*100)*10^6</f>
-        <v>7.897251651043373E-2</v>
+        <v>4.0483057814126255E-2</v>
       </c>
       <c r="D20" s="38">
         <f>D4-C20</f>
-        <v>-3.6750294288211506E-2</v>
+        <v>1.7391644080959681E-3</v>
       </c>
       <c r="E20" s="40">
         <f t="shared" ref="E20:E30" si="14">D20/E4</f>
-        <v>-6.0817383347002858</v>
+        <v>0.28781110616728967</v>
       </c>
       <c r="F20" s="42">
         <f>E20^2</f>
-        <v>36.987541171763006</v>
+        <v>8.2835232833238889E-2</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -7590,19 +7778,19 @@
       </c>
       <c r="J20" s="37">
         <f>(PI()*$X$21*$X$22*I20*$X$26^4)/(8*$X$29*$X$31*100)*10^6</f>
-        <v>3.0204947877728372E-2</v>
+        <v>2.0158404142797091E-2</v>
       </c>
       <c r="K20" s="45">
         <f>M4-J20</f>
-        <v>-9.0938367666172602E-3</v>
+        <v>9.5270696831402032E-4</v>
       </c>
       <c r="L20" s="40">
         <f>K20/N4</f>
-        <v>-1.5693042874748002</v>
+        <v>0.16440663808379041</v>
       </c>
       <c r="M20" s="42">
         <f>L20^2</f>
-        <v>2.4627159466867905</v>
+        <v>2.7029542646014443E-2</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -7611,19 +7799,19 @@
       </c>
       <c r="Q20" s="37">
         <f>(PI()*$X$21*$X$22*P20*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
-        <v>2.5316342346709167E-2</v>
+        <v>1.8136449430132328E-2</v>
       </c>
       <c r="R20" s="45">
         <f>Q20-V4</f>
-        <v>6.4274534578202779E-3</v>
+        <v>-7.524394587565611E-4</v>
       </c>
       <c r="S20" s="40">
         <f>R20/W4</f>
-        <v>8.1013731636105071</v>
+        <v>-0.94839937440469102</v>
       </c>
       <c r="T20" s="42">
         <f>S20^2</f>
-        <v>65.632247136068514</v>
+        <v>0.89946137337120935</v>
       </c>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -7654,40 +7842,40 @@
       </c>
       <c r="C21" s="37">
         <f t="shared" ref="C21:C34" si="15">(PI()*$X$21*$X$22*B21*$X$27^4)/(8*$X$30*$X$31*100)*10^6</f>
-        <v>0.11845877476565059</v>
+        <v>6.0724586721189383E-2</v>
       </c>
       <c r="D21" s="39">
         <f t="shared" ref="D21:D30" si="16">D5-C21</f>
-        <v>-4.0680996987872808E-2</v>
+        <v>1.7053191056588396E-2</v>
       </c>
       <c r="E21" s="41">
         <f t="shared" si="14"/>
-        <v>-6.2808163353479545</v>
+        <v>2.6328745332853916</v>
       </c>
       <c r="F21" s="43">
         <f t="shared" ref="F21:F34" si="17">E21^2</f>
-        <v>39.448653838373708</v>
+        <v>6.932028308022768</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="109"/>
+      <c r="I21" s="105"/>
       <c r="J21" s="37">
         <f t="shared" ref="J21:J35" si="18">(PI()*$X$21*$X$22*I21*$X$26^4)/(8*$X$29*$X$31*100)*10^6</f>
         <v>0</v>
       </c>
-      <c r="K21" s="117"/>
-      <c r="L21" s="111"/>
-      <c r="M21" s="112"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="108"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="109"/>
+      <c r="P21" s="105"/>
       <c r="Q21" s="37">
         <f t="shared" ref="Q21:Q35" si="19">(PI()*$X$21*$X$22*P21*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
         <v>0</v>
       </c>
-      <c r="R21" s="120"/>
-      <c r="S21" s="121"/>
-      <c r="T21" s="112"/>
+      <c r="R21" s="116"/>
+      <c r="S21" s="117"/>
+      <c r="T21" s="108"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="6" t="s">
@@ -7717,19 +7905,19 @@
       </c>
       <c r="C22" s="37">
         <f t="shared" si="15"/>
-        <v>0.15794503302086746</v>
+        <v>8.0966115628252511E-2</v>
       </c>
       <c r="D22" s="39">
         <f t="shared" si="16"/>
-        <v>-7.2389477465311908E-2</v>
+        <v>4.5894399273030406E-3</v>
       </c>
       <c r="E22" s="41">
         <f t="shared" si="14"/>
-        <v>-11.010650108672287</v>
+        <v>0.69806716395374968</v>
       </c>
       <c r="F22" s="43">
         <f t="shared" si="17"/>
-        <v>121.23441581560505</v>
+        <v>0.48729776539043124</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -7738,19 +7926,19 @@
       </c>
       <c r="J22" s="37">
         <f t="shared" si="18"/>
-        <v>6.0409895755456744E-2</v>
+        <v>4.0316808285594183E-2</v>
       </c>
       <c r="K22" s="47">
         <f>M6-J22</f>
-        <v>-1.5409895755456746E-2</v>
+        <v>4.6831917144058155E-3</v>
       </c>
       <c r="L22" s="41">
         <f>K22/N6</f>
-        <v>-2.5362175890733929</v>
+        <v>0.77077699859668891</v>
       </c>
       <c r="M22" s="43">
         <f t="shared" ref="M22:M34" si="20">L22^2</f>
-        <v>6.4323996591252532</v>
+        <v>0.59409718156572022</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -7759,19 +7947,19 @@
       </c>
       <c r="Q22" s="37">
         <f t="shared" si="19"/>
-        <v>5.0632684693418334E-2</v>
+        <v>3.6272898860264656E-2</v>
       </c>
       <c r="R22" s="48">
         <f>Q22-V6</f>
-        <v>2.1743795804529443E-2</v>
+        <v>7.384009971375765E-3</v>
       </c>
       <c r="S22" s="46">
         <f>R22/W6</f>
-        <v>23.308772375472582</v>
+        <v>7.9154628376874703</v>
       </c>
       <c r="T22" s="43">
         <f t="shared" ref="T22:T34" si="21">S22^2</f>
-        <v>543.2988696515938</v>
+        <v>62.65455193481138</v>
       </c>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
@@ -7802,40 +7990,40 @@
       </c>
       <c r="C23" s="37">
         <f t="shared" si="15"/>
-        <v>0.19743129127608433</v>
+        <v>0.10120764453531564</v>
       </c>
       <c r="D23" s="39">
         <f t="shared" si="16"/>
-        <v>-9.5209069053862116E-2</v>
+        <v>1.0145776869065759E-3</v>
       </c>
       <c r="E23" s="41">
         <f t="shared" si="14"/>
-        <v>-14.030172483866622</v>
+        <v>0.1495099163035484</v>
       </c>
       <c r="F23" s="43">
         <f t="shared" si="17"/>
-        <v>196.8457399270481</v>
+        <v>2.2353215073094047E-2</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="109"/>
+      <c r="I23" s="105"/>
       <c r="J23" s="37">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K23" s="117"/>
-      <c r="L23" s="111"/>
-      <c r="M23" s="112"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="108"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="109"/>
+      <c r="P23" s="105"/>
       <c r="Q23" s="37">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="R23" s="120"/>
-      <c r="S23" s="121"/>
-      <c r="T23" s="112"/>
+      <c r="R23" s="116"/>
+      <c r="S23" s="117"/>
+      <c r="T23" s="108"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="3" t="s">
@@ -7867,19 +8055,19 @@
       </c>
       <c r="C24" s="37">
         <f t="shared" si="15"/>
-        <v>0.23691754953130117</v>
+        <v>0.12144917344237877</v>
       </c>
       <c r="D24" s="39">
         <f t="shared" si="16"/>
-        <v>-0.12247310508685673</v>
+        <v>-7.0047289979343202E-3</v>
       </c>
       <c r="E24" s="41">
         <f t="shared" si="14"/>
-        <v>-17.639058409235997</v>
+        <v>-1.0088486271970269</v>
       </c>
       <c r="F24" s="43">
         <f t="shared" si="17"/>
-        <v>311.13638156443915</v>
+        <v>1.0177755525973258</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -7888,19 +8076,19 @@
       </c>
       <c r="J24" s="37">
         <f t="shared" si="18"/>
-        <v>9.061484363318513E-2</v>
+        <v>6.047521242839126E-2</v>
       </c>
       <c r="K24" s="47">
         <f>M8-J24</f>
-        <v>-4.5059288077629579E-2</v>
+        <v>-1.491965687283571E-2</v>
       </c>
       <c r="L24" s="41">
         <f>K24/N8</f>
-        <v>-7.4079076678516476</v>
+        <v>-2.4528448021544831</v>
       </c>
       <c r="M24" s="43">
         <f t="shared" si="20"/>
-        <v>54.877096015415233</v>
+        <v>6.0164476234562656</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -7909,19 +8097,19 @@
       </c>
       <c r="Q24" s="37">
         <f t="shared" si="19"/>
-        <v>7.5949027040127501E-2</v>
+        <v>5.4409348290396994E-2</v>
       </c>
       <c r="R24" s="48">
         <f>Q24-V8</f>
-        <v>1.5949027040127496E-2</v>
+        <v>-5.5906517096030103E-3</v>
       </c>
       <c r="S24" s="46">
         <f>R24/W8</f>
-        <v>11.470338562057684</v>
+        <v>-4.0207260123361417</v>
       </c>
       <c r="T24" s="43">
         <f t="shared" si="21"/>
-        <v>131.56866672822753</v>
+        <v>16.166237666276491</v>
       </c>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
@@ -7935,17 +8123,17 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Z24" s="1"/>
-      <c r="AA24" s="1" t="s">
+      <c r="AA24" s="131" t="s">
         <v>25</v>
       </c>
       <c r="AB24" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="AC24" s="53" t="s">
+      <c r="AC24" s="130" t="s">
         <v>30</v>
       </c>
       <c r="AD24" s="1"/>
-      <c r="AE24" s="1" t="s">
+      <c r="AE24" s="131" t="s">
         <v>27</v>
       </c>
       <c r="AF24" s="53" t="s">
@@ -7964,48 +8152,48 @@
       </c>
       <c r="C25" s="37">
         <f t="shared" si="15"/>
-        <v>0.27640380778651807</v>
+        <v>0.14169070234944187</v>
       </c>
       <c r="D25" s="39">
         <f t="shared" si="16"/>
-        <v>-0.10529269667540697</v>
+        <v>2.9420408761669237E-2</v>
       </c>
       <c r="E25" s="41">
         <f t="shared" si="14"/>
-        <v>-13.687242937518132</v>
+        <v>3.8244274746180764</v>
       </c>
       <c r="F25" s="43">
         <f t="shared" si="17"/>
-        <v>187.34061923063999</v>
+        <v>14.626245508613598</v>
       </c>
       <c r="G25" s="36"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="109"/>
+      <c r="I25" s="105"/>
       <c r="J25" s="37">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K25" s="117"/>
-      <c r="L25" s="111"/>
-      <c r="M25" s="112"/>
+      <c r="K25" s="113"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="108"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="109"/>
+      <c r="P25" s="105"/>
       <c r="Q25" s="37">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="R25" s="120"/>
-      <c r="S25" s="121"/>
-      <c r="T25" s="112"/>
+      <c r="R25" s="116"/>
+      <c r="S25" s="117"/>
+      <c r="T25" s="108"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="X25" s="11">
-        <f>50*0.00001</f>
-        <v>5.0000000000000001E-4</v>
+        <f>46*0.00001</f>
+        <v>4.6000000000000001E-4</v>
       </c>
       <c r="Y25" s="9">
         <f>3*0.001</f>
@@ -8013,7 +8201,7 @@
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
-      <c r="AB25" s="59">
+      <c r="AB25" s="58">
         <v>65</v>
       </c>
       <c r="AC25" s="56">
@@ -8021,10 +8209,10 @@
       </c>
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
-      <c r="AF25" s="88">
+      <c r="AF25" s="58">
         <v>52</v>
       </c>
-      <c r="AG25" s="56">
+      <c r="AG25" s="58">
         <v>47</v>
       </c>
       <c r="AH25" s="1"/>
@@ -8037,19 +8225,19 @@
       </c>
       <c r="C26" s="37">
         <f t="shared" si="15"/>
-        <v>0.31589006604173492</v>
+        <v>0.16193223125650502</v>
       </c>
       <c r="D26" s="39">
         <f t="shared" si="16"/>
-        <v>-0.12922339937506824</v>
+        <v>2.4734435410161654E-2</v>
       </c>
       <c r="E26" s="41">
         <f t="shared" si="14"/>
-        <v>-16.35010709043663</v>
+        <v>3.1295467363757963</v>
       </c>
       <c r="F26" s="43">
         <f t="shared" si="17"/>
-        <v>267.32600186874618</v>
+        <v>9.7940627751603984</v>
       </c>
       <c r="G26" s="36"/>
       <c r="H26" s="1"/>
@@ -8058,19 +8246,19 @@
       </c>
       <c r="J26" s="37">
         <f t="shared" si="18"/>
-        <v>0.12081979151091349</v>
+        <v>8.0633616571188366E-2</v>
       </c>
       <c r="K26" s="47">
         <f>M10-J26</f>
-        <v>-2.9708680399802387E-2</v>
+        <v>1.0477494539922735E-2</v>
       </c>
       <c r="L26" s="41">
         <f>K26/N10</f>
-        <v>-4.4710928847312132</v>
+        <v>1.5768405279815216</v>
       </c>
       <c r="M26" s="43">
         <f t="shared" si="20"/>
-        <v>19.99067158389408</v>
+        <v>2.486426050685044</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -8079,19 +8267,19 @@
       </c>
       <c r="Q26" s="37">
         <f t="shared" si="19"/>
-        <v>0.10126536938683667</v>
+        <v>7.2545797720529312E-2</v>
       </c>
       <c r="R26" s="48">
         <f>Q26-V10</f>
-        <v>2.5709813831281111E-2</v>
+        <v>-3.0097578350262444E-3</v>
       </c>
       <c r="S26" s="46">
         <f>R26/W10</f>
-        <v>15.813709938317631</v>
+        <v>-1.8512556216869429</v>
       </c>
       <c r="T26" s="43">
         <f t="shared" si="21"/>
-        <v>250.07342201324582</v>
+        <v>3.4271473768275094</v>
       </c>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
@@ -8099,15 +8287,15 @@
         <v>12</v>
       </c>
       <c r="X26" s="11">
-        <f>52*0.00001</f>
-        <v>5.2000000000000006E-4</v>
+        <f>47*0.00001</f>
+        <v>4.7000000000000004E-4</v>
       </c>
       <c r="Y26" s="9">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
-      <c r="AB26" s="59">
+      <c r="AB26" s="58">
         <v>66</v>
       </c>
       <c r="AC26" s="56">
@@ -8115,10 +8303,10 @@
       </c>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
-      <c r="AF26" s="88">
+      <c r="AF26" s="58">
         <v>50</v>
       </c>
-      <c r="AG26" s="56">
+      <c r="AG26" s="58">
         <v>50</v>
       </c>
       <c r="AH26" s="1"/>
@@ -8131,55 +8319,55 @@
       </c>
       <c r="C27" s="37">
         <f t="shared" si="15"/>
-        <v>0.35537632429695182</v>
-      </c>
-      <c r="D27" s="39">
+        <v>0.18217376016356815</v>
+      </c>
+      <c r="D27" s="128">
         <f t="shared" si="16"/>
-        <v>-0.15870965763028516</v>
+        <v>1.4492906503098507E-2</v>
       </c>
       <c r="E27" s="41">
         <f t="shared" si="14"/>
-        <v>-19.740024810674072</v>
+        <v>1.8026019224135235</v>
       </c>
       <c r="F27" s="43">
         <f t="shared" si="17"/>
-        <v>389.66857952602794</v>
+        <v>3.2493736906889303</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="109"/>
+      <c r="I27" s="105"/>
       <c r="J27" s="37">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K27" s="117"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="112"/>
+      <c r="K27" s="113"/>
+      <c r="L27" s="107"/>
+      <c r="M27" s="108"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="109"/>
+      <c r="P27" s="105"/>
       <c r="Q27" s="37">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="R27" s="120"/>
-      <c r="S27" s="121"/>
-      <c r="T27" s="112"/>
+      <c r="R27" s="116"/>
+      <c r="S27" s="117"/>
+      <c r="T27" s="108"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="10" t="s">
         <v>14</v>
       </c>
       <c r="X27" s="11">
-        <f>65*0.00001</f>
-        <v>6.5000000000000008E-4</v>
+        <f>55*0.00001</f>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="Y27" s="9">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
-      <c r="AB27" s="59">
+      <c r="AB27" s="58">
         <v>68</v>
       </c>
       <c r="AC27" s="56">
@@ -8187,10 +8375,10 @@
       </c>
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
-      <c r="AF27" s="88">
+      <c r="AF27" s="58">
         <v>53</v>
       </c>
-      <c r="AG27" s="56">
+      <c r="AG27" s="58">
         <v>51</v>
       </c>
       <c r="AH27" s="1"/>
@@ -8203,19 +8391,19 @@
       </c>
       <c r="C28" s="37">
         <f t="shared" si="15"/>
-        <v>0.39486258255216866</v>
+        <v>0.20241528907063128</v>
       </c>
       <c r="D28" s="39">
         <f t="shared" si="16"/>
-        <v>-0.19708480477439089</v>
+        <v>-4.6375112928535023E-3</v>
       </c>
       <c r="E28" s="41">
         <f t="shared" si="14"/>
-        <v>-24.466774044514008</v>
+        <v>-0.57571633216987739</v>
       </c>
       <c r="F28" s="43">
         <f t="shared" si="17"/>
-        <v>598.62303214530436</v>
+        <v>0.33144929512713661</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -8224,19 +8412,19 @@
       </c>
       <c r="J28" s="37">
         <f t="shared" si="18"/>
-        <v>0.15102473938864189</v>
+        <v>0.10079202071398545</v>
       </c>
       <c r="K28" s="47">
         <f>M12-J28</f>
-        <v>-5.1024739388641882E-2</v>
+        <v>-7.920207139854446E-4</v>
       </c>
       <c r="L28" s="41">
         <f>K28/N12</f>
-        <v>-7.5506983786124611</v>
+        <v>-0.1172041169160503</v>
       </c>
       <c r="M28" s="43">
         <f t="shared" si="20"/>
-        <v>57.013046004780847</v>
+        <v>1.3736805022071188E-2</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -8245,19 +8433,19 @@
       </c>
       <c r="Q28" s="37">
         <f>(PI()*$X$21*$X$22*P28*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
-        <v>0.12658171173354582</v>
+        <v>9.0682247150661657E-2</v>
       </c>
       <c r="R28" s="48">
         <f>Q28-V12</f>
-        <v>3.8803933955768033E-2</v>
+        <v>2.9044693728838694E-3</v>
       </c>
       <c r="S28" s="46">
         <f>R28/W12</f>
-        <v>21.411888970377245</v>
+        <v>1.6026770842600699</v>
       </c>
       <c r="T28" s="43">
         <f>S28^2</f>
-        <v>458.4689892797627</v>
+        <v>2.5685738364123591</v>
       </c>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
@@ -8272,7 +8460,7 @@
       </c>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
-      <c r="AB28" s="59">
+      <c r="AB28" s="58">
         <v>66</v>
       </c>
       <c r="AC28" s="56">
@@ -8280,10 +8468,10 @@
       </c>
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
-      <c r="AF28" s="88">
+      <c r="AF28" s="58">
         <v>53</v>
       </c>
-      <c r="AG28" s="56">
+      <c r="AG28" s="58">
         <v>47</v>
       </c>
       <c r="AH28" s="1"/>
@@ -8296,40 +8484,40 @@
       </c>
       <c r="C29" s="37">
         <f t="shared" si="15"/>
-        <v>0.43434884080738551</v>
+        <v>0.22265681797769438</v>
       </c>
       <c r="D29" s="39">
         <f t="shared" si="16"/>
-        <v>-0.19879328525182996</v>
+        <v>1.2898737577861169E-2</v>
       </c>
       <c r="E29" s="41">
         <f t="shared" si="14"/>
-        <v>-23.176686189624011</v>
+        <v>1.5038233947675417</v>
       </c>
       <c r="F29" s="43">
         <f t="shared" si="17"/>
-        <v>537.1587827323084</v>
+        <v>2.2614848026501737</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="109"/>
+      <c r="I29" s="105"/>
       <c r="J29" s="37">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K29" s="117"/>
-      <c r="L29" s="111"/>
-      <c r="M29" s="112"/>
+      <c r="K29" s="113"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="108"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="109"/>
+      <c r="P29" s="105"/>
       <c r="Q29" s="37">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="R29" s="120"/>
-      <c r="S29" s="121"/>
-      <c r="T29" s="112"/>
+      <c r="R29" s="116"/>
+      <c r="S29" s="117"/>
+      <c r="T29" s="108"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="27" t="s">
@@ -8351,10 +8539,10 @@
       </c>
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
-      <c r="AF29" s="89">
+      <c r="AF29" s="58">
         <v>52</v>
       </c>
-      <c r="AG29" s="90">
+      <c r="AG29" s="58">
         <v>47</v>
       </c>
       <c r="AH29" s="1"/>
@@ -8367,19 +8555,19 @@
       </c>
       <c r="C30" s="37">
         <f t="shared" si="15"/>
-        <v>0.47383509906260235</v>
+        <v>0.24289834688475753</v>
       </c>
       <c r="D30" s="39">
         <f t="shared" si="16"/>
-        <v>-0.18605732128482461</v>
+        <v>4.4879430893020211E-2</v>
       </c>
       <c r="E30" s="41">
         <f t="shared" si="14"/>
-        <v>-19.978686894096679</v>
+        <v>4.8191175257451828</v>
       </c>
       <c r="F30" s="43">
         <f t="shared" si="17"/>
-        <v>399.1479300123504</v>
+        <v>23.223893726944372</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -8388,19 +8576,19 @@
       </c>
       <c r="J30" s="37">
         <f t="shared" si="18"/>
-        <v>0.18122968726637026</v>
+        <v>0.12095042485678252</v>
       </c>
       <c r="K30" s="47">
         <f>M14-J30</f>
-        <v>-6.0118576155259146E-2</v>
+        <v>1.6068625432859307E-4</v>
       </c>
       <c r="L30" s="41">
         <f>K30/N14</f>
-        <v>-8.5519742207661515</v>
+        <v>2.2857905035886125E-2</v>
       </c>
       <c r="M30" s="43">
         <f t="shared" si="20"/>
-        <v>73.136263072648831</v>
+        <v>5.2248382262958827E-4</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -8409,19 +8597,19 @@
       </c>
       <c r="Q30" s="37">
         <f t="shared" si="19"/>
-        <v>0.151898054080255</v>
+        <v>0.10881869658079399</v>
       </c>
       <c r="R30" s="48">
         <f>Q30-V14</f>
-        <v>5.3009165191366114E-2</v>
+        <v>9.9298076919051015E-3</v>
       </c>
       <c r="S30" s="46">
         <f>R30/W14</f>
-        <v>26.737001237454084</v>
+        <v>5.008441079720872</v>
       </c>
       <c r="T30" s="43">
         <f t="shared" si="21"/>
-        <v>714.86723517162125</v>
+        <v>25.084482049035575</v>
       </c>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
@@ -8436,57 +8624,48 @@
       </c>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
-      <c r="AB30" s="53">
-        <f>SUM(AB25:AB29)/5</f>
-        <v>65.2</v>
-      </c>
-      <c r="AC30" s="53">
-        <f t="shared" ref="AC30" si="22">SUM(AC25:AC29)/5</f>
+      <c r="AB30" s="132">
         <v>65</v>
       </c>
-      <c r="AD30" s="1"/>
+      <c r="AC30" s="129"/>
       <c r="AE30" s="1"/>
-      <c r="AF30" s="53">
-        <f>SUM(AF25:AF29)/5</f>
-        <v>52</v>
-      </c>
-      <c r="AG30" s="53">
-        <f>SUM(AG25:AG29)/5</f>
-        <v>48.4</v>
-      </c>
+      <c r="AF30" s="132">
+        <v>50</v>
+      </c>
+      <c r="AG30" s="132"/>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
     </row>
     <row r="31" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="109"/>
+      <c r="B31" s="105"/>
       <c r="C31" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="D31" s="110"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="112"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="107"/>
+      <c r="F31" s="108"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="109"/>
+      <c r="I31" s="105"/>
       <c r="J31" s="37">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K31" s="117"/>
-      <c r="L31" s="111"/>
-      <c r="M31" s="112"/>
+      <c r="K31" s="113"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="108"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="109"/>
+      <c r="P31" s="105"/>
       <c r="Q31" s="37">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="R31" s="120"/>
-      <c r="S31" s="121"/>
-      <c r="T31" s="112"/>
+      <c r="R31" s="116"/>
+      <c r="S31" s="117"/>
+      <c r="T31" s="108"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="30" t="s">
@@ -8500,12 +8679,24 @@
       </c>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
+      <c r="AB31" s="53">
+        <f>SUM(AB25:AB30)/6</f>
+        <v>65.166666666666671</v>
+      </c>
+      <c r="AC31" s="53">
+        <f>SUM(AC25:AC29)/5</f>
+        <v>65</v>
+      </c>
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
-      <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
+      <c r="AF31" s="53">
+        <f>SUM(AF25:AF30)/6</f>
+        <v>51.666666666666664</v>
+      </c>
+      <c r="AG31" s="53">
+        <f>SUM(AG25:AG29)/5</f>
+        <v>48.4</v>
+      </c>
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
     </row>
@@ -8516,19 +8707,19 @@
       </c>
       <c r="C32" s="37">
         <f t="shared" si="15"/>
-        <v>0.55280761557303615</v>
+        <v>0.28338140469888373</v>
       </c>
       <c r="D32" s="39">
         <f>D15-C32</f>
-        <v>-0.20280761557303617</v>
+        <v>6.6618595301116246E-2</v>
       </c>
       <c r="E32" s="41">
         <f>D32/E15</f>
-        <v>-19.872182866448959</v>
+        <v>6.5276488971538882</v>
       </c>
       <c r="F32" s="43">
         <f t="shared" si="17"/>
-        <v>394.90365187758755</v>
+        <v>42.610200124514371</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -8537,19 +8728,19 @@
       </c>
       <c r="J32" s="37">
         <f t="shared" si="18"/>
-        <v>0.21143463514409863</v>
+        <v>0.14110882899957961</v>
       </c>
       <c r="K32" s="47">
         <f>M15-J32</f>
-        <v>-5.5323524032987514E-2</v>
+        <v>1.5002282111531512E-2</v>
       </c>
       <c r="L32" s="41">
         <f>K32/N15</f>
-        <v>-7.3849117399150295</v>
+        <v>2.0025934939521517</v>
       </c>
       <c r="M32" s="43">
         <f t="shared" si="20"/>
-        <v>54.536921406334827</v>
+        <v>4.0103807020194866</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -8558,19 +8749,19 @@
       </c>
       <c r="Q32" s="37">
         <f>(PI()*$X$21*$X$22*P32*$X$25^4)/(8*$X$28*$X$31*100)*10^6</f>
-        <v>0.17721439642696415</v>
+        <v>0.12695514601092628</v>
       </c>
       <c r="R32" s="48">
         <f>Q32-V15</f>
-        <v>6.5547729760297477E-2</v>
+        <v>1.5288479344259601E-2</v>
       </c>
       <c r="S32" s="46">
         <f>R32/W15</f>
-        <v>30.078037801815391</v>
+        <v>7.0154597471268261</v>
       </c>
       <c r="T32" s="43">
         <f t="shared" si="21"/>
-        <v>904.68835800743568</v>
+        <v>49.21667546355679</v>
       </c>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
@@ -8585,12 +8776,11 @@
       </c>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
-      <c r="AB32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC32" s="27" t="s">
-        <v>30</v>
-      </c>
+      <c r="AB32" s="1">
+        <f>AVERAGE(AB25:AB30)</f>
+        <v>65.166666666666671</v>
+      </c>
+      <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
@@ -8600,44 +8790,45 @@
     </row>
     <row r="33" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="109"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="37">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="D33" s="110"/>
-      <c r="E33" s="111"/>
-      <c r="F33" s="112"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="107"/>
+      <c r="F33" s="108"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="109"/>
+      <c r="I33" s="105"/>
       <c r="J33" s="37">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K33" s="117"/>
-      <c r="L33" s="111"/>
-      <c r="M33" s="112"/>
+      <c r="K33" s="113"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="108"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="109"/>
+      <c r="P33" s="105"/>
       <c r="Q33" s="37">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="R33" s="120"/>
-      <c r="S33" s="121"/>
-      <c r="T33" s="112"/>
+      <c r="R33" s="116"/>
+      <c r="S33" s="117"/>
+      <c r="T33" s="108"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="57">
-        <v>53</v>
+      <c r="AA33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB33" s="53" t="s">
+        <v>30</v>
       </c>
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
@@ -8653,19 +8844,19 @@
       </c>
       <c r="C34" s="37">
         <f t="shared" si="15"/>
-        <v>0.63178013208346984</v>
+        <v>0.32386446251301004</v>
       </c>
       <c r="D34" s="39">
         <f>D16-C34</f>
-        <v>-0.22178013208346986</v>
+        <v>8.6135537486989933E-2</v>
       </c>
       <c r="E34" s="41">
         <f>D34/E16</f>
-        <v>-20.016862985777802</v>
+        <v>7.7742006729191306</v>
       </c>
       <c r="F34" s="43">
         <f t="shared" si="17"/>
-        <v>400.67480379140142</v>
+        <v>60.438196102816264</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -8674,19 +8865,19 @@
       </c>
       <c r="J34" s="37">
         <f t="shared" si="18"/>
-        <v>0.24163958302182698</v>
+        <v>0.16126723314237673</v>
       </c>
       <c r="K34" s="44">
         <f>M16-J34</f>
-        <v>-4.1639583021826965E-2</v>
+        <v>3.873276685762328E-2</v>
       </c>
       <c r="L34" s="46">
         <f>K34/N16</f>
-        <v>-5.1498147813061266</v>
+        <v>4.7903115451399803</v>
       </c>
       <c r="M34" s="43">
         <f t="shared" si="20"/>
-        <v>26.520592281759068</v>
+        <v>22.947084699501385</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -8695,19 +8886,19 @@
       </c>
       <c r="Q34" s="37">
         <f t="shared" si="19"/>
-        <v>0.20253073877367334</v>
+        <v>0.14509159544105862</v>
       </c>
       <c r="R34" s="48">
         <f>Q34-V16</f>
-        <v>5.3641849884784432E-2</v>
+        <v>-3.79729344783028E-3</v>
       </c>
       <c r="S34" s="46">
         <f>R34/W16</f>
-        <v>19.470533305664606</v>
+        <v>-1.3783142957628181</v>
       </c>
       <c r="T34" s="43">
         <f t="shared" si="21"/>
-        <v>379.1016672069947</v>
+        <v>1.8997502979041532</v>
       </c>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
@@ -8716,10 +8907,10 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="57">
-        <v>50</v>
-      </c>
+      <c r="AB34" s="58">
+        <v>53</v>
+      </c>
+      <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
       <c r="AE34" s="1"/>
       <c r="AF34" s="1"/>
@@ -8729,37 +8920,37 @@
     </row>
     <row r="35" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="113"/>
+      <c r="B35" s="109"/>
       <c r="C35" s="37">
         <f>(PI()*$X$21*$X$22*B35*$X$27^4)/(8*$X$30*$X$31*100)*10^6</f>
         <v>0</v>
       </c>
-      <c r="D35" s="114"/>
-      <c r="E35" s="115"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="124">
+      <c r="D35" s="110"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="120">
         <f>SUM(F20:F35)</f>
-        <v>3880.4961335015951</v>
+        <v>165.0771961004321</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="113"/>
+      <c r="I35" s="109"/>
       <c r="J35" s="37">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K35" s="118"/>
-      <c r="L35" s="119"/>
-      <c r="M35" s="116"/>
+      <c r="K35" s="114"/>
+      <c r="L35" s="115"/>
+      <c r="M35" s="112"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="113"/>
+      <c r="P35" s="109"/>
       <c r="Q35" s="37">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="R35" s="118"/>
-      <c r="S35" s="119"/>
-      <c r="T35" s="116"/>
+      <c r="R35" s="114"/>
+      <c r="S35" s="115"/>
+      <c r="T35" s="112"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
@@ -8767,10 +8958,10 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="57">
-        <v>47</v>
-      </c>
+      <c r="AB35" s="58">
+        <v>50</v>
+      </c>
+      <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
       <c r="AF35" s="1"/>
@@ -8788,7 +8979,7 @@
       </c>
       <c r="F36" s="54">
         <f>SUM(F20:F35)/11</f>
-        <v>352.77237577287229</v>
+        <v>15.00701782731201</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -8800,7 +8991,7 @@
       </c>
       <c r="M36" s="54">
         <f>SUM(M20:M35)/6</f>
-        <v>49.161617661774159</v>
+        <v>6.015954181453103</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -8811,7 +9002,7 @@
       </c>
       <c r="T36" s="54">
         <f>SUM(T20:T35)/6</f>
-        <v>574.61657586582498</v>
+        <v>26.986146666365908</v>
       </c>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
@@ -8820,10 +9011,10 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="57">
-        <v>56</v>
-      </c>
+      <c r="AB36" s="58">
+        <v>47</v>
+      </c>
+      <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
       <c r="AF36" s="1"/>
@@ -8832,60 +9023,60 @@
       <c r="AI36" s="1"/>
     </row>
     <row r="37" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="130" t="s">
+      <c r="A37" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="125">
+      <c r="B37" s="121">
         <f>AVERAGE(B20:B35)</f>
         <v>8.2307692307692299</v>
       </c>
-      <c r="C37" s="126">
+      <c r="C37" s="122">
         <f>AVERAGE(C20:C35)</f>
-        <v>0.26406435208176277</v>
+        <v>0.13536522456598465</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="127">
+      <c r="F37" s="123">
         <f>2.15384512*10^-3</f>
         <v>2.1538451200000001E-3</v>
       </c>
-      <c r="G37" s="127">
+      <c r="G37" s="123">
         <f>1.47803503*10^-3</f>
         <v>1.47803503E-3</v>
       </c>
-      <c r="H37" s="130" t="s">
+      <c r="H37" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="I37" s="125">
+      <c r="I37" s="121">
         <f>AVERAGE(I20:I35)</f>
         <v>9</v>
       </c>
-      <c r="J37" s="126">
+      <c r="J37" s="122">
         <f>AVERAGE(J20:J35)</f>
-        <v>6.7961132724888851E-2</v>
+        <v>4.535640932129345E-2</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="N37" s="127">
+      <c r="N37" s="123">
         <f>2.46907554*10^-3</f>
         <v>2.4690755399999998E-3</v>
       </c>
-      <c r="O37" s="130" t="s">
+      <c r="O37" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="P37" s="125">
+      <c r="P37" s="121">
         <f>AVERAGE(P20:P35)</f>
         <v>9</v>
       </c>
-      <c r="Q37" s="126">
+      <c r="Q37" s="122">
         <f>AVERAGE(Q20:Q35)</f>
-        <v>5.6961770280095622E-2</v>
+        <v>4.0807011217797742E-2</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="127">
+      <c r="U37" s="123">
         <f>2.46883066*10^-3</f>
         <v>2.4688306599999999E-3</v>
       </c>
@@ -8895,10 +9086,10 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="57">
+      <c r="AB37" s="58">
         <v>56</v>
       </c>
+      <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
       <c r="AE37" s="1"/>
       <c r="AF37" s="1"/>
@@ -8911,10 +9102,10 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="123" t="s">
+      <c r="E38" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="60">
+      <c r="F38" s="59">
         <v>2.1292993709564399E-3</v>
       </c>
       <c r="G38" s="1"/>
@@ -8922,10 +9113,10 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="123" t="s">
+      <c r="L38" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="M38" s="60">
+      <c r="M38" s="59">
         <v>1.7083014917976815E-3</v>
       </c>
       <c r="N38" s="1"/>
@@ -8933,10 +9124,10 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="123" t="s">
+      <c r="S38" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="T38" s="60">
+      <c r="T38" s="59">
         <v>1.8023969417446609E-3</v>
       </c>
       <c r="U38" s="1"/>
@@ -8946,11 +9137,10 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="53">
-        <f>SUM(AC33:AC37)/5</f>
-        <v>52.4</v>
-      </c>
+      <c r="AB38" s="58">
+        <v>56</v>
+      </c>
+      <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
       <c r="AE38" s="1"/>
       <c r="AF38" s="1"/>
@@ -8958,7 +9148,7 @@
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -8986,6 +9176,9 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
+      <c r="AB39" s="57">
+        <v>52</v>
+      </c>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
@@ -8994,7 +9187,7 @@
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -9022,8 +9215,10 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
-      <c r="AB40" s="1"/>
-      <c r="AC40" s="1"/>
+      <c r="AB40" s="53">
+        <f>SUM(AB34:AB39)/6</f>
+        <v>52.333333333333336</v>
+      </c>
       <c r="AD40" s="1"/>
       <c r="AE40" s="1"/>
       <c r="AF40" s="1"/>
@@ -9477,522 +9672,552 @@
       <c r="S57" s="1"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F58" s="80"/>
-      <c r="G58" s="80"/>
-      <c r="H58" s="80"/>
-      <c r="I58" s="80"/>
-      <c r="J58" s="80"/>
-      <c r="K58" s="80"/>
-      <c r="L58" s="80"/>
-      <c r="M58" s="80"/>
-      <c r="N58" s="80"/>
-      <c r="O58" s="80"/>
-      <c r="P58" s="80"/>
-      <c r="Q58" s="80"/>
+      <c r="F58" s="79"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="79"/>
+      <c r="J58" s="79"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="79"/>
+      <c r="M58" s="79"/>
+      <c r="N58" s="79"/>
+      <c r="O58" s="79"/>
+      <c r="P58" s="79"/>
+      <c r="Q58" s="79"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F59" s="80"/>
-      <c r="G59" s="81"/>
-      <c r="H59" s="82"/>
-      <c r="I59" s="81"/>
-      <c r="J59" s="83"/>
-      <c r="K59" s="83"/>
-      <c r="L59" s="83"/>
-      <c r="M59" s="80"/>
-      <c r="N59" s="80"/>
-      <c r="O59" s="80"/>
-      <c r="P59" s="80"/>
-      <c r="Q59" s="80"/>
+      <c r="F59" s="79"/>
+      <c r="G59" s="80"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="80"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="82"/>
+      <c r="L59" s="82"/>
+      <c r="M59" s="79"/>
+      <c r="N59" s="79"/>
+      <c r="O59" s="79"/>
+      <c r="P59" s="79"/>
+      <c r="Q59" s="79"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F60" s="80"/>
-      <c r="G60" s="81"/>
-      <c r="H60" s="82"/>
-      <c r="I60" s="84"/>
-      <c r="J60" s="84"/>
-      <c r="K60" s="85"/>
-      <c r="L60" s="86"/>
-      <c r="M60" s="80"/>
-      <c r="N60" s="80"/>
-      <c r="O60" s="80"/>
-      <c r="P60" s="80"/>
-      <c r="Q60" s="80"/>
+      <c r="F60" s="79"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="81"/>
+      <c r="I60" s="83"/>
+      <c r="J60" s="83"/>
+      <c r="K60" s="84"/>
+      <c r="L60" s="85"/>
+      <c r="M60" s="79"/>
+      <c r="N60" s="79"/>
+      <c r="O60" s="79"/>
+      <c r="P60" s="79"/>
+      <c r="Q60" s="79"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="F61" s="80"/>
-      <c r="G61" s="81"/>
-      <c r="H61" s="82"/>
-      <c r="I61" s="84"/>
-      <c r="J61" s="84"/>
-      <c r="K61" s="85"/>
-      <c r="L61" s="86"/>
-      <c r="M61" s="80"/>
-      <c r="N61" s="80"/>
-      <c r="O61" s="80"/>
-      <c r="P61" s="80"/>
-      <c r="Q61" s="80"/>
+      <c r="F61" s="79"/>
+      <c r="G61" s="80"/>
+      <c r="H61" s="81"/>
+      <c r="I61" s="83"/>
+      <c r="J61" s="83"/>
+      <c r="K61" s="84"/>
+      <c r="L61" s="85"/>
+      <c r="M61" s="79"/>
+      <c r="N61" s="79"/>
+      <c r="O61" s="79"/>
+      <c r="P61" s="79"/>
+      <c r="Q61" s="79"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B62" s="72" t="s">
+      <c r="B62" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="F62" s="80"/>
-      <c r="G62" s="81"/>
-      <c r="H62" s="82"/>
-      <c r="I62" s="84"/>
-      <c r="J62" s="84"/>
-      <c r="K62" s="85"/>
-      <c r="L62" s="86"/>
-      <c r="M62" s="80"/>
-      <c r="N62" s="80"/>
-      <c r="O62" s="80"/>
-      <c r="P62" s="80"/>
-      <c r="Q62" s="80"/>
+      <c r="F62" s="79"/>
+      <c r="G62" s="80"/>
+      <c r="H62" s="81"/>
+      <c r="I62" s="83"/>
+      <c r="J62" s="83"/>
+      <c r="K62" s="84"/>
+      <c r="L62" s="85"/>
+      <c r="M62" s="79"/>
+      <c r="N62" s="79"/>
+      <c r="O62" s="79"/>
+      <c r="P62" s="79"/>
+      <c r="Q62" s="79"/>
     </row>
-    <row r="63" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="72" t="s">
+    <row r="63" spans="1:19" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="91" t="s">
+      <c r="B63" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="C63" s="92" t="s">
+      <c r="C63" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="72" t="s">
+      <c r="E63" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="91" t="s">
+      <c r="F63" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="G63" s="92" t="s">
+      <c r="G63" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="H63" s="95"/>
-      <c r="I63" s="96" t="s">
+      <c r="H63" s="91"/>
+      <c r="I63" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="J63" s="91" t="s">
+      <c r="J63" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="K63" s="92" t="s">
+      <c r="K63" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="L63" s="97"/>
-      <c r="M63" s="87"/>
-      <c r="N63" s="87"/>
-      <c r="O63" s="87"/>
-      <c r="P63" s="87"/>
-      <c r="Q63" s="87"/>
+      <c r="L63" s="93"/>
+      <c r="M63" s="86"/>
+      <c r="N63" s="86"/>
+      <c r="O63" s="86"/>
+      <c r="P63" s="86"/>
+      <c r="Q63" s="86"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B64" s="93">
+      <c r="B64" s="89">
         <v>2</v>
       </c>
-      <c r="C64" s="94">
-        <v>-3.6750294288211506E-2</v>
-      </c>
-      <c r="F64" s="93">
+      <c r="C64" s="90">
+        <f>D20</f>
+        <v>1.7391644080959681E-3</v>
+      </c>
+      <c r="F64" s="89">
         <v>2</v>
       </c>
-      <c r="G64" s="94">
-        <v>-9.0938367666172602E-3</v>
-      </c>
-      <c r="H64" s="82"/>
-      <c r="I64" s="84"/>
-      <c r="J64" s="93">
+      <c r="G64" s="90">
+        <f>K20</f>
+        <v>9.5270696831402032E-4</v>
+      </c>
+      <c r="H64" s="81"/>
+      <c r="I64" s="83"/>
+      <c r="J64" s="89">
         <v>2</v>
       </c>
-      <c r="K64" s="94">
-        <v>6.4274534578202779E-3</v>
-      </c>
-      <c r="L64" s="86"/>
-      <c r="M64" s="80"/>
-      <c r="N64" s="80"/>
-      <c r="O64" s="80"/>
-      <c r="P64" s="80"/>
-      <c r="Q64" s="80"/>
+      <c r="K64" s="90">
+        <f>R20</f>
+        <v>-7.524394587565611E-4</v>
+      </c>
+      <c r="L64" s="85"/>
+      <c r="M64" s="79"/>
+      <c r="N64" s="79"/>
+      <c r="O64" s="79"/>
+      <c r="P64" s="79"/>
+      <c r="Q64" s="79"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B65" s="93">
+      <c r="B65" s="89">
         <v>3</v>
       </c>
-      <c r="C65" s="94">
-        <v>-4.0680996987872808E-2</v>
-      </c>
-      <c r="F65" s="93">
+      <c r="C65" s="90">
+        <f t="shared" ref="C65:C76" si="22">D21</f>
+        <v>1.7053191056588396E-2</v>
+      </c>
+      <c r="F65" s="89">
         <v>4</v>
       </c>
-      <c r="G65" s="94">
-        <v>-1.5409895755456746E-2</v>
-      </c>
-      <c r="H65" s="82"/>
-      <c r="I65" s="84"/>
-      <c r="J65" s="93">
+      <c r="G65" s="90">
+        <f>K22</f>
+        <v>4.6831917144058155E-3</v>
+      </c>
+      <c r="H65" s="81"/>
+      <c r="I65" s="83"/>
+      <c r="J65" s="89">
         <v>4</v>
       </c>
-      <c r="K65" s="94">
-        <v>2.1743795804529443E-2</v>
-      </c>
-      <c r="L65" s="86"/>
-      <c r="M65" s="80"/>
-      <c r="N65" s="80"/>
-      <c r="O65" s="80"/>
-      <c r="P65" s="80"/>
-      <c r="Q65" s="80"/>
+      <c r="K65" s="90">
+        <f>R22</f>
+        <v>7.384009971375765E-3</v>
+      </c>
+      <c r="L65" s="85"/>
+      <c r="M65" s="79"/>
+      <c r="N65" s="79"/>
+      <c r="O65" s="79"/>
+      <c r="P65" s="79"/>
+      <c r="Q65" s="79"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B66" s="93">
+      <c r="B66" s="89">
         <v>4</v>
       </c>
-      <c r="C66" s="94">
-        <v>-7.2389477465311908E-2</v>
-      </c>
-      <c r="F66" s="93">
+      <c r="C66" s="90">
+        <f t="shared" si="22"/>
+        <v>4.5894399273030406E-3</v>
+      </c>
+      <c r="F66" s="89">
         <v>6</v>
       </c>
-      <c r="G66" s="94">
-        <v>-4.5059288077629579E-2</v>
-      </c>
-      <c r="H66" s="82"/>
-      <c r="I66" s="84"/>
-      <c r="J66" s="93">
+      <c r="G66" s="133">
+        <f>K24</f>
+        <v>-1.491965687283571E-2</v>
+      </c>
+      <c r="H66" s="81"/>
+      <c r="I66" s="83"/>
+      <c r="J66" s="89">
         <v>6</v>
       </c>
-      <c r="K66" s="94">
-        <v>1.5949027040127496E-2</v>
-      </c>
-      <c r="L66" s="86"/>
-      <c r="M66" s="80"/>
-      <c r="N66" s="80"/>
-      <c r="O66" s="80"/>
-      <c r="P66" s="80"/>
-      <c r="Q66" s="80"/>
+      <c r="K66" s="90">
+        <f>R24</f>
+        <v>-5.5906517096030103E-3</v>
+      </c>
+      <c r="L66" s="85"/>
+      <c r="M66" s="79"/>
+      <c r="N66" s="79"/>
+      <c r="O66" s="79"/>
+      <c r="P66" s="79"/>
+      <c r="Q66" s="79"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B67" s="93">
+      <c r="B67" s="89">
         <v>5</v>
       </c>
-      <c r="C67" s="94">
-        <v>-9.5209069053862116E-2</v>
-      </c>
-      <c r="F67" s="93">
+      <c r="C67" s="90">
+        <f t="shared" si="22"/>
+        <v>1.0145776869065759E-3</v>
+      </c>
+      <c r="F67" s="89">
         <v>8</v>
       </c>
-      <c r="G67" s="94">
-        <v>-2.9708680399802387E-2</v>
-      </c>
-      <c r="H67" s="82"/>
-      <c r="I67" s="84"/>
-      <c r="J67" s="93">
+      <c r="G67" s="133">
+        <f>K26</f>
+        <v>1.0477494539922735E-2</v>
+      </c>
+      <c r="H67" s="81"/>
+      <c r="I67" s="83"/>
+      <c r="J67" s="89">
         <v>8</v>
       </c>
-      <c r="K67" s="94">
-        <v>2.5709813831281111E-2</v>
-      </c>
-      <c r="L67" s="86"/>
-      <c r="M67" s="80"/>
-      <c r="N67" s="80"/>
-      <c r="O67" s="80"/>
-      <c r="P67" s="80"/>
-      <c r="Q67" s="80"/>
+      <c r="K67" s="90">
+        <f>R26</f>
+        <v>-3.0097578350262444E-3</v>
+      </c>
+      <c r="L67" s="85"/>
+      <c r="M67" s="79"/>
+      <c r="N67" s="79"/>
+      <c r="O67" s="79"/>
+      <c r="P67" s="79"/>
+      <c r="Q67" s="79"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B68" s="93">
+      <c r="B68" s="89">
         <v>6</v>
       </c>
-      <c r="C68" s="94">
-        <v>-0.12247310508685673</v>
-      </c>
-      <c r="F68" s="93">
+      <c r="C68" s="90">
+        <f t="shared" si="22"/>
+        <v>-7.0047289979343202E-3</v>
+      </c>
+      <c r="F68" s="89">
         <v>10</v>
       </c>
-      <c r="G68" s="128">
-        <v>-5.1024739388641882E-2</v>
-      </c>
-      <c r="H68" s="82"/>
-      <c r="I68" s="84"/>
-      <c r="J68" s="93">
+      <c r="G68" s="133">
+        <f>K28</f>
+        <v>-7.920207139854446E-4</v>
+      </c>
+      <c r="H68" s="81"/>
+      <c r="I68" s="83"/>
+      <c r="J68" s="89">
         <v>10</v>
       </c>
-      <c r="K68" s="128">
-        <v>3.8803933955768033E-2</v>
-      </c>
-      <c r="L68" s="86"/>
-      <c r="M68" s="80"/>
-      <c r="N68" s="80"/>
-      <c r="O68" s="80"/>
-      <c r="P68" s="80"/>
-      <c r="Q68" s="80"/>
+      <c r="K68" s="124">
+        <v>3.8803933955767998E-2</v>
+      </c>
+      <c r="L68" s="85"/>
+      <c r="M68" s="79"/>
+      <c r="N68" s="79"/>
+      <c r="O68" s="79"/>
+      <c r="P68" s="79"/>
+      <c r="Q68" s="79"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B69" s="93">
+      <c r="B69" s="89">
         <v>7</v>
       </c>
-      <c r="C69" s="94">
-        <v>-0.10529269667540697</v>
-      </c>
-      <c r="F69" s="93">
+      <c r="C69" s="90">
+        <f t="shared" si="22"/>
+        <v>2.9420408761669237E-2</v>
+      </c>
+      <c r="F69" s="89">
         <v>12</v>
       </c>
-      <c r="G69" s="128">
-        <v>-6.0118576155259146E-2</v>
-      </c>
-      <c r="H69" s="82"/>
-      <c r="I69" s="84"/>
-      <c r="J69" s="93">
+      <c r="G69" s="133">
+        <f>K30</f>
+        <v>1.6068625432859307E-4</v>
+      </c>
+      <c r="H69" s="81"/>
+      <c r="I69" s="83"/>
+      <c r="J69" s="89">
         <v>12</v>
       </c>
-      <c r="K69" s="128">
-        <v>5.3009165191366114E-2</v>
-      </c>
-      <c r="L69" s="86"/>
-      <c r="M69" s="80"/>
-      <c r="N69" s="80"/>
-      <c r="O69" s="80"/>
-      <c r="P69" s="80"/>
-      <c r="Q69" s="80"/>
+      <c r="K69" s="133">
+        <f>R28</f>
+        <v>2.9044693728838694E-3</v>
+      </c>
+      <c r="L69" s="85"/>
+      <c r="M69" s="79"/>
+      <c r="N69" s="79"/>
+      <c r="O69" s="79"/>
+      <c r="P69" s="79"/>
+      <c r="Q69" s="79"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B70" s="93">
+      <c r="B70" s="89">
         <v>8</v>
       </c>
-      <c r="C70" s="94">
-        <v>-0.12922339937506824</v>
-      </c>
-      <c r="F70" s="93">
+      <c r="C70" s="90">
+        <f t="shared" si="22"/>
+        <v>2.4734435410161654E-2</v>
+      </c>
+      <c r="F70" s="89">
         <v>14</v>
       </c>
-      <c r="G70" s="128">
-        <v>-5.5323524032987514E-2</v>
-      </c>
-      <c r="H70" s="82"/>
-      <c r="I70" s="84"/>
-      <c r="J70" s="93">
+      <c r="G70" s="133">
+        <f>K32</f>
+        <v>1.5002282111531512E-2</v>
+      </c>
+      <c r="H70" s="81"/>
+      <c r="I70" s="83"/>
+      <c r="J70" s="89">
         <v>14</v>
       </c>
-      <c r="K70" s="128">
-        <v>6.5547729760297477E-2</v>
-      </c>
-      <c r="L70" s="86"/>
-      <c r="M70" s="80"/>
-      <c r="N70" s="80"/>
-      <c r="O70" s="80"/>
-      <c r="P70" s="80"/>
-      <c r="Q70" s="80"/>
+      <c r="K70" s="133">
+        <f>R30</f>
+        <v>9.9298076919051015E-3</v>
+      </c>
+      <c r="L70" s="85"/>
+      <c r="M70" s="79"/>
+      <c r="N70" s="79"/>
+      <c r="O70" s="79"/>
+      <c r="P70" s="79"/>
+      <c r="Q70" s="79"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B71" s="93">
+      <c r="B71" s="89">
         <v>9</v>
       </c>
-      <c r="C71" s="94">
-        <v>-0.15870965763028516</v>
-      </c>
-      <c r="F71" s="93">
+      <c r="C71" s="90">
+        <f t="shared" si="22"/>
+        <v>1.4492906503098507E-2</v>
+      </c>
+      <c r="F71" s="89">
         <v>16</v>
       </c>
-      <c r="G71" s="128">
-        <v>-4.1639583021826965E-2</v>
-      </c>
-      <c r="H71" s="82"/>
-      <c r="I71" s="84"/>
-      <c r="J71" s="93">
+      <c r="G71" s="133">
+        <f>K34</f>
+        <v>3.873276685762328E-2</v>
+      </c>
+      <c r="H71" s="81"/>
+      <c r="I71" s="83"/>
+      <c r="J71" s="89">
         <v>16</v>
       </c>
-      <c r="K71" s="128">
-        <v>5.3641849884784432E-2</v>
-      </c>
-      <c r="L71" s="86"/>
-      <c r="M71" s="80"/>
-      <c r="N71" s="80"/>
-      <c r="O71" s="80"/>
-      <c r="P71" s="80"/>
-      <c r="Q71" s="80"/>
+      <c r="K71" s="133">
+        <f>R32</f>
+        <v>1.5288479344259601E-2</v>
+      </c>
+      <c r="L71" s="85"/>
+      <c r="M71" s="79"/>
+      <c r="N71" s="79"/>
+      <c r="O71" s="79"/>
+      <c r="P71" s="79"/>
+      <c r="Q71" s="79"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B72" s="93">
+      <c r="B72" s="89">
         <v>10</v>
       </c>
-      <c r="C72" s="94">
-        <v>-0.19708480477439089</v>
-      </c>
-      <c r="H72" s="82"/>
-      <c r="I72" s="84"/>
-      <c r="L72" s="86"/>
-      <c r="M72" s="80"/>
-      <c r="N72" s="80"/>
-      <c r="O72" s="80"/>
-      <c r="P72" s="80"/>
-      <c r="Q72" s="80"/>
+      <c r="C72" s="90">
+        <f t="shared" si="22"/>
+        <v>-4.6375112928535023E-3</v>
+      </c>
+      <c r="H72" s="81"/>
+      <c r="I72" s="83"/>
+      <c r="L72" s="85"/>
+      <c r="M72" s="79"/>
+      <c r="N72" s="79"/>
+      <c r="O72" s="79"/>
+      <c r="P72" s="79"/>
+      <c r="Q72" s="79"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B73" s="93">
+      <c r="B73" s="89">
         <v>11</v>
       </c>
-      <c r="C73" s="94">
-        <v>-0.19879328525182996</v>
-      </c>
-      <c r="F73" s="82"/>
-      <c r="G73" s="84"/>
-      <c r="H73" s="82"/>
-      <c r="I73" s="84"/>
-      <c r="J73" s="82"/>
-      <c r="K73" s="84"/>
-      <c r="L73" s="86"/>
-      <c r="M73" s="80"/>
-      <c r="N73" s="80"/>
-      <c r="O73" s="80"/>
-      <c r="P73" s="80"/>
-      <c r="Q73" s="80"/>
+      <c r="C73" s="90">
+        <f t="shared" si="22"/>
+        <v>1.2898737577861169E-2</v>
+      </c>
+      <c r="F73" s="81"/>
+      <c r="G73" s="83"/>
+      <c r="H73" s="81"/>
+      <c r="I73" s="83"/>
+      <c r="J73" s="81"/>
+      <c r="K73" s="83"/>
+      <c r="L73" s="85"/>
+      <c r="M73" s="79"/>
+      <c r="N73" s="79"/>
+      <c r="O73" s="79"/>
+      <c r="P73" s="79"/>
+      <c r="Q73" s="79"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B74" s="93">
+      <c r="B74" s="89">
         <v>12</v>
       </c>
-      <c r="C74" s="94">
-        <v>-0.18605732128482461</v>
-      </c>
-      <c r="F74" s="80"/>
-      <c r="H74" s="82"/>
-      <c r="I74" s="84"/>
-      <c r="J74" s="80"/>
-      <c r="L74" s="86"/>
-      <c r="M74" s="80"/>
-      <c r="N74" s="80"/>
-      <c r="O74" s="80"/>
-      <c r="P74" s="80"/>
-      <c r="Q74" s="80"/>
+      <c r="C74" s="90">
+        <f t="shared" si="22"/>
+        <v>4.4879430893020211E-2</v>
+      </c>
+      <c r="F74" s="79"/>
+      <c r="H74" s="81"/>
+      <c r="I74" s="83"/>
+      <c r="J74" s="79"/>
+      <c r="L74" s="85"/>
+      <c r="M74" s="79"/>
+      <c r="N74" s="79"/>
+      <c r="O74" s="79"/>
+      <c r="P74" s="79"/>
+      <c r="Q74" s="79"/>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B75" s="93">
+      <c r="B75" s="89">
         <v>14</v>
       </c>
-      <c r="C75" s="94">
-        <v>-0.20280761557303617</v>
-      </c>
-      <c r="F75" s="82"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="82"/>
-      <c r="I75" s="84"/>
-      <c r="J75" s="82"/>
-      <c r="K75" s="84"/>
-      <c r="L75" s="86"/>
-      <c r="M75" s="80"/>
-      <c r="N75" s="80"/>
-      <c r="O75" s="80"/>
-      <c r="P75" s="80"/>
-      <c r="Q75" s="80"/>
+      <c r="C75" s="90">
+        <f>D32</f>
+        <v>6.6618595301116246E-2</v>
+      </c>
+      <c r="F75" s="81"/>
+      <c r="G75" s="83"/>
+      <c r="H75" s="81"/>
+      <c r="I75" s="83"/>
+      <c r="J75" s="81"/>
+      <c r="K75" s="83"/>
+      <c r="L75" s="85"/>
+      <c r="M75" s="79"/>
+      <c r="N75" s="79"/>
+      <c r="O75" s="79"/>
+      <c r="P75" s="79"/>
+      <c r="Q75" s="79"/>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B76" s="93">
+      <c r="B76" s="89">
         <v>16</v>
       </c>
-      <c r="C76" s="94">
-        <v>-0.22178013208346986</v>
-      </c>
-      <c r="F76" s="80"/>
-      <c r="H76" s="81"/>
-      <c r="I76" s="81"/>
-      <c r="J76" s="80"/>
-      <c r="L76" s="81"/>
-      <c r="M76" s="80"/>
-      <c r="N76" s="80"/>
-      <c r="O76" s="80"/>
-      <c r="P76" s="80"/>
-      <c r="Q76" s="80"/>
+      <c r="C76" s="90">
+        <f>D34</f>
+        <v>8.6135537486989933E-2</v>
+      </c>
+      <c r="F76" s="79"/>
+      <c r="H76" s="80"/>
+      <c r="I76" s="80"/>
+      <c r="J76" s="79"/>
+      <c r="L76" s="80"/>
+      <c r="M76" s="79"/>
+      <c r="N76" s="79"/>
+      <c r="O76" s="79"/>
+      <c r="P76" s="79"/>
+      <c r="Q76" s="79"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A77" s="80"/>
-      <c r="B77" s="82"/>
-      <c r="C77" s="84"/>
-      <c r="D77" s="80"/>
-      <c r="E77" s="80"/>
-      <c r="F77" s="82"/>
-      <c r="G77" s="84"/>
-      <c r="H77" s="80"/>
-      <c r="I77" s="80"/>
-      <c r="J77" s="82"/>
-      <c r="L77" s="80"/>
-      <c r="M77" s="80"/>
+      <c r="A77" s="79"/>
+      <c r="B77" s="81"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="79"/>
+      <c r="E77" s="79"/>
+      <c r="F77" s="81"/>
+      <c r="G77" s="83"/>
+      <c r="H77" s="79"/>
+      <c r="I77" s="79"/>
+      <c r="J77" s="81"/>
+      <c r="L77" s="79"/>
+      <c r="M77" s="79"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78" s="80"/>
-      <c r="B78" s="80"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="80"/>
-      <c r="E78" s="80"/>
-      <c r="F78" s="80"/>
-      <c r="H78" s="80"/>
-      <c r="I78" s="80"/>
-      <c r="J78" s="80"/>
-      <c r="L78" s="80"/>
-      <c r="M78" s="80"/>
+      <c r="A78" s="79"/>
+      <c r="B78" s="79"/>
+      <c r="D78" s="79"/>
+      <c r="E78" s="79"/>
+      <c r="F78" s="79"/>
+      <c r="H78" s="79"/>
+      <c r="I78" s="79"/>
+      <c r="J78" s="79"/>
+      <c r="L78" s="79"/>
+      <c r="M78" s="79"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A79" s="80"/>
-      <c r="B79" s="82"/>
-      <c r="C79" s="84"/>
-      <c r="D79" s="80"/>
-      <c r="E79" s="80"/>
-      <c r="F79" s="82"/>
-      <c r="G79" s="84"/>
-      <c r="H79" s="80"/>
-      <c r="I79" s="80"/>
-      <c r="J79" s="82"/>
-      <c r="K79" s="84"/>
-      <c r="L79" s="80"/>
-      <c r="M79" s="80"/>
+      <c r="A79" s="79"/>
+      <c r="B79" s="81"/>
+      <c r="C79" s="83"/>
+      <c r="D79" s="79"/>
+      <c r="E79" s="79"/>
+      <c r="F79" s="81"/>
+      <c r="G79" s="83"/>
+      <c r="H79" s="79"/>
+      <c r="I79" s="79"/>
+      <c r="J79" s="81"/>
+      <c r="K79" s="83"/>
+      <c r="L79" s="79"/>
+      <c r="M79" s="79"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A80" s="80"/>
-      <c r="B80" s="80"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="80"/>
-      <c r="E80" s="80"/>
-      <c r="F80" s="80"/>
-      <c r="G80" s="80"/>
-      <c r="H80" s="80"/>
-      <c r="I80" s="80"/>
-      <c r="J80" s="80"/>
-      <c r="K80" s="80"/>
-      <c r="L80" s="80"/>
-      <c r="M80" s="80"/>
+      <c r="A80" s="79"/>
+      <c r="B80" s="79"/>
+      <c r="C80" s="79"/>
+      <c r="D80" s="79"/>
+      <c r="E80" s="79"/>
+      <c r="F80" s="79"/>
+      <c r="G80" s="79"/>
+      <c r="H80" s="79"/>
+      <c r="I80" s="79"/>
+      <c r="J80" s="79"/>
+      <c r="K80" s="79"/>
+      <c r="L80" s="79"/>
+      <c r="M80" s="79"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A81" s="80"/>
-      <c r="B81" s="80"/>
-      <c r="C81" s="80"/>
-      <c r="D81" s="80"/>
-      <c r="E81" s="80"/>
-      <c r="F81" s="80"/>
-      <c r="J81" s="80"/>
-      <c r="K81" s="80"/>
-      <c r="L81" s="80"/>
-      <c r="M81" s="80"/>
+      <c r="A81" s="79"/>
+      <c r="B81" s="79"/>
+      <c r="C81" s="79"/>
+      <c r="D81" s="79"/>
+      <c r="E81" s="79"/>
+      <c r="F81" s="79"/>
+      <c r="J81" s="79"/>
+      <c r="K81" s="79"/>
+      <c r="L81" s="79"/>
+      <c r="M81" s="79"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A82" s="80"/>
-      <c r="B82" s="80"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="80"/>
-      <c r="E82" s="80"/>
-      <c r="F82" s="80"/>
-      <c r="J82" s="80"/>
-      <c r="K82" s="80"/>
-      <c r="L82" s="80"/>
-      <c r="M82" s="80"/>
+      <c r="A82" s="79"/>
+      <c r="B82" s="79"/>
+      <c r="C82" s="79"/>
+      <c r="D82" s="79"/>
+      <c r="E82" s="79"/>
+      <c r="F82" s="79"/>
+      <c r="J82" s="79"/>
+      <c r="K82" s="79"/>
+      <c r="L82" s="79"/>
+      <c r="M82" s="79"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A83" s="80"/>
-      <c r="B83" s="80"/>
-      <c r="C83" s="80"/>
-      <c r="D83" s="80"/>
-      <c r="E83" s="80"/>
-      <c r="F83" s="80"/>
+      <c r="A83" s="79"/>
+      <c r="B83" s="79"/>
+      <c r="C83" s="79"/>
+      <c r="D83" s="79"/>
+      <c r="E83" s="79"/>
+      <c r="F83" s="79"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C75" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
cp and lab report done
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14680"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
   <si>
     <t>data</t>
   </si>
@@ -621,6 +621,39 @@
   <si>
     <t>Changing the model to have +c (the error on dV/dt) shifts the model to match data more!</t>
   </si>
+  <si>
+    <t>Look over to the right for uncertainty calculations</t>
+  </si>
+  <si>
+    <t>Error on numerator</t>
+  </si>
+  <si>
+    <t>Error on rho*g</t>
+  </si>
+  <si>
+    <t>Error on h*a^4</t>
+  </si>
+  <si>
+    <t>a^4</t>
+  </si>
+  <si>
+    <t>Uncertainty on viscosity_blue</t>
+  </si>
+  <si>
+    <t>Error on denominator</t>
+  </si>
+  <si>
+    <t>Error on LV'</t>
+  </si>
+  <si>
+    <t>Total Error</t>
+  </si>
+  <si>
+    <t>Uncertainty on viscosity_red</t>
+  </si>
+  <si>
+    <t>Uncertainty on viscosity_black</t>
+  </si>
 </sst>
 </file>
 
@@ -632,7 +665,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -769,6 +802,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1248,7 +1289,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1327,8 +1368,36 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1738,8 +1807,14 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="106">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1779,6 +1854,20 @@
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1817,6 +1906,20 @@
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2790,11 +2893,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1870133648"/>
-        <c:axId val="-1870132784"/>
+        <c:axId val="1957962080"/>
+        <c:axId val="1957965264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1870133648"/>
+        <c:axId val="1957962080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2823,12 +2926,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1870132784"/>
+        <c:crossAx val="1957965264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1870132784"/>
+        <c:axId val="1957965264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2857,7 +2960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1870133648"/>
+        <c:crossAx val="1957962080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2914,7 +3017,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3089,11 +3191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1906187472"/>
-        <c:axId val="-1906140944"/>
+        <c:axId val="1923376592"/>
+        <c:axId val="1886961024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1906187472"/>
+        <c:axId val="1923376592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3113,6 +3215,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3149,12 +3252,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1906140944"/>
+        <c:crossAx val="1886961024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1906140944"/>
+        <c:axId val="1886961024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3210,7 +3313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1906187472"/>
+        <c:crossAx val="1923376592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3300,7 +3403,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3448,11 +3550,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1870169392"/>
-        <c:axId val="-1870173328"/>
+        <c:axId val="1885558144"/>
+        <c:axId val="1921166016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1870169392"/>
+        <c:axId val="1885558144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3509,12 +3611,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1870173328"/>
+        <c:crossAx val="1921166016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1870173328"/>
+        <c:axId val="1921166016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3571,7 +3673,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1870169392"/>
+        <c:crossAx val="1885558144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3661,7 +3763,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3809,11 +3910,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1906238768"/>
-        <c:axId val="-1906170784"/>
+        <c:axId val="1957991248"/>
+        <c:axId val="1957993728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1906238768"/>
+        <c:axId val="1957991248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3870,12 +3971,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1906170784"/>
+        <c:crossAx val="1957993728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1906170784"/>
+        <c:axId val="1957993728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3895,6 +3996,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3931,7 +4033,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1906238768"/>
+        <c:crossAx val="1957991248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6353,6 +6455,253 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>981850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>21344</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="687816" cy="337913"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15122606" y="7908151"/>
+              <a:ext cx="687816" cy="337913"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" charset="0"/>
+                        <a:ea typeface="Cambria Math" charset="0"/>
+                        <a:cs typeface="Cambria Math" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝜂</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" charset="0"/>
+                        <a:ea typeface="Cambria Math" charset="0"/>
+                        <a:cs typeface="Cambria Math" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="mr-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:ea typeface="Cambria Math" charset="0"/>
+                            <a:cs typeface="Cambria Math" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="mr-IN" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:ea typeface="Cambria Math" charset="0"/>
+                            <a:cs typeface="Cambria Math" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜌</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:ea typeface="Cambria Math" charset="0"/>
+                            <a:cs typeface="Cambria Math" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑔h</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" charset="0"/>
+                                <a:ea typeface="Cambria Math" charset="0"/>
+                                <a:cs typeface="Cambria Math" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" charset="0"/>
+                                <a:ea typeface="Cambria Math" charset="0"/>
+                                <a:cs typeface="Cambria Math" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" charset="0"/>
+                                <a:ea typeface="Cambria Math" charset="0"/>
+                                <a:cs typeface="Cambria Math" charset="0"/>
+                              </a:rPr>
+                              <m:t>4</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:ea typeface="Cambria Math" charset="0"/>
+                            <a:cs typeface="Cambria Math" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐿𝑉</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" charset="0"/>
+                            <a:ea typeface="Cambria Math" charset="0"/>
+                            <a:cs typeface="Cambria Math" charset="0"/>
+                          </a:rPr>
+                          <m:t>′</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15122606" y="7908151"/>
+              <a:ext cx="687816" cy="337913"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:ea typeface="Cambria Math" charset="0"/>
+                  <a:cs typeface="Cambria Math" charset="0"/>
+                </a:rPr>
+                <a:t>𝜂</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:ea typeface="Cambria Math" charset="0"/>
+                  <a:cs typeface="Cambria Math" charset="0"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="mr-IN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:ea typeface="Cambria Math" charset="0"/>
+                  <a:cs typeface="Cambria Math" charset="0"/>
+                </a:rPr>
+                <a:t>(𝜌</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:ea typeface="Cambria Math" charset="0"/>
+                  <a:cs typeface="Cambria Math" charset="0"/>
+                </a:rPr>
+                <a:t>𝑔ℎ𝑎^4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="mr-IN" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:ea typeface="Cambria Math" charset="0"/>
+                  <a:cs typeface="Cambria Math" charset="0"/>
+                </a:rPr>
+                <a:t>)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" charset="0"/>
+                  <a:ea typeface="Cambria Math" charset="0"/>
+                  <a:cs typeface="Cambria Math" charset="0"/>
+                </a:rPr>
+                <a:t>𝐿𝑉′</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6645,8 +6994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q24" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="N23" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AD46" sqref="AD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6663,14 +7012,23 @@
     <col min="14" max="14" width="9.33203125" style="2" customWidth="1"/>
     <col min="15" max="15" width="9.1640625" style="2" customWidth="1"/>
     <col min="16" max="16" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" style="2"/>
+    <col min="17" max="17" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.1640625" style="2" customWidth="1"/>
-    <col min="20" max="23" width="9.1640625" style="2"/>
-    <col min="24" max="24" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" style="2"/>
+    <col min="22" max="22" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1640625" style="2"/>
+    <col min="27" max="27" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.1640625" style="2"/>
+    <col min="32" max="32" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6704,6 +7062,11 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
     </row>
     <row r="2" spans="1:36" s="71" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
@@ -7981,7 +8344,7 @@
       </c>
       <c r="AJ16" s="26"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -8032,8 +8395,9 @@
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
     </row>
-    <row r="18" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>7</v>
@@ -8077,8 +8441,9 @@
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
     </row>
-    <row r="19" spans="1:35" s="71" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" s="71" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="68" t="s">
         <v>23</v>
       </c>
@@ -8149,8 +8514,9 @@
       <c r="AG19" s="68"/>
       <c r="AH19" s="68"/>
       <c r="AI19" s="68"/>
+      <c r="AJ19" s="68"/>
     </row>
-    <row r="20" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="34">
         <v>2</v>
@@ -8234,8 +8600,9 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
     </row>
-    <row r="21" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="35">
         <v>3</v>
@@ -8297,8 +8664,9 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
     </row>
-    <row r="22" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="35">
         <v>4</v>
@@ -8382,8 +8750,9 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
     </row>
-    <row r="23" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="35">
         <v>5</v>
@@ -8447,8 +8816,9 @@
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
     </row>
-    <row r="24" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="35">
         <v>6</v>
@@ -8543,9 +8913,14 @@
         <v>28</v>
       </c>
       <c r="AH24" s="1"/>
-      <c r="AI24" s="1"/>
+      <c r="AI24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ24" s="53" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="25" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="35">
         <v>7</v>
@@ -8599,7 +8974,9 @@
         <f>3*0.001</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Z25" s="1"/>
+      <c r="Z25" s="1">
+        <v>3.0000000000000001E-5</v>
+      </c>
       <c r="AA25" s="1"/>
       <c r="AB25" s="58">
         <v>65</v>
@@ -8617,8 +8994,11 @@
       </c>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
+      <c r="AJ25" s="58">
+        <v>53</v>
+      </c>
     </row>
-    <row r="26" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="35">
         <v>8</v>
@@ -8693,7 +9073,9 @@
       <c r="Y26" s="9">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Z26" s="1"/>
+      <c r="Z26" s="1">
+        <v>3.0000000000000001E-5</v>
+      </c>
       <c r="AA26" s="1"/>
       <c r="AB26" s="58">
         <v>66</v>
@@ -8711,8 +9093,11 @@
       </c>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
+      <c r="AJ26" s="58">
+        <v>50</v>
+      </c>
     </row>
-    <row r="27" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="35">
         <v>9</v>
@@ -8765,7 +9150,9 @@
       <c r="Y27" s="9">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Z27" s="1"/>
+      <c r="Z27" s="1">
+        <v>3.0000000000000001E-5</v>
+      </c>
       <c r="AA27" s="1"/>
       <c r="AB27" s="58">
         <v>68</v>
@@ -8783,8 +9170,11 @@
       </c>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
+      <c r="AJ27" s="58">
+        <v>47</v>
+      </c>
     </row>
-    <row r="28" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="35">
         <v>10</v>
@@ -8876,8 +9266,11 @@
       </c>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
+      <c r="AJ28" s="58">
+        <v>56</v>
+      </c>
     </row>
-    <row r="29" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="35">
         <v>11</v>
@@ -8947,8 +9340,11 @@
       </c>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
+      <c r="AJ29" s="58">
+        <v>56</v>
+      </c>
     </row>
-    <row r="30" spans="1:35" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="35">
         <v>12</v>
@@ -9035,8 +9431,11 @@
       <c r="AG30" s="132"/>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
+      <c r="AJ30" s="57">
+        <v>52</v>
+      </c>
     </row>
-    <row r="31" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="105"/>
       <c r="C31" s="37">
@@ -9099,8 +9498,12 @@
       </c>
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
+      <c r="AJ31" s="53">
+        <f>SUM(AJ25:AJ30)/6</f>
+        <v>52.333333333333336</v>
+      </c>
     </row>
-    <row r="32" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="35">
         <v>14</v>
@@ -9187,8 +9590,9 @@
       <c r="AG32" s="1"/>
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
     </row>
-    <row r="33" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="105"/>
       <c r="C33" s="37">
@@ -9224,20 +9628,18 @@
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB33" s="53" t="s">
-        <v>28</v>
-      </c>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
+      <c r="AJ33" s="1"/>
     </row>
-    <row r="34" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="35">
         <v>16</v>
@@ -9307,9 +9709,7 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
-      <c r="AB34" s="58">
-        <v>53</v>
-      </c>
+      <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
       <c r="AE34" s="1"/>
@@ -9317,8 +9717,9 @@
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
     </row>
-    <row r="35" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="109"/>
       <c r="C35" s="37">
@@ -9358,9 +9759,7 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
-      <c r="AB35" s="58">
-        <v>50</v>
-      </c>
+      <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
@@ -9368,8 +9767,9 @@
       <c r="AG35" s="1"/>
       <c r="AH35" s="1"/>
       <c r="AI35" s="1"/>
+      <c r="AJ35" s="1"/>
     </row>
-    <row r="36" spans="1:35" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" ht="19" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -9411,9 +9811,7 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
-      <c r="AB36" s="58">
-        <v>47</v>
-      </c>
+      <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
@@ -9421,8 +9819,9 @@
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
       <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
     </row>
-    <row r="37" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="126" t="s">
         <v>40</v>
       </c>
@@ -9434,7 +9833,10 @@
         <f>AVERAGE(C20:C35)</f>
         <v>0.13799022456598464</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1">
+        <f>SUM(E4:E16)/13</f>
+        <v>7.9761839996009623E-3</v>
+      </c>
       <c r="E37" s="1"/>
       <c r="F37" s="123">
         <f>2.15384512*10^-3</f>
@@ -9455,7 +9857,10 @@
         <f>AVERAGE(J20:J35)</f>
         <v>4.535640932129345E-2</v>
       </c>
-      <c r="K37" s="1"/>
+      <c r="K37" s="1">
+        <f>SUM(N4:N16)/8</f>
+        <v>6.7453054241699353E-3</v>
+      </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="123">
@@ -9473,7 +9878,10 @@
         <f>AVERAGE(Q20:Q35)</f>
         <v>4.0807011217797742E-2</v>
       </c>
-      <c r="R37" s="1"/>
+      <c r="R37" s="1">
+        <f>SUM(W4:W16)/8</f>
+        <v>1.6839558082319081E-3</v>
+      </c>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="123">
@@ -9486,9 +9894,7 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
-      <c r="AB37" s="58">
-        <v>56</v>
-      </c>
+      <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
       <c r="AE37" s="1"/>
@@ -9496,8 +9902,9 @@
       <c r="AG37" s="1"/>
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
     </row>
-    <row r="38" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -9537,9 +9944,7 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
-      <c r="AB38" s="58">
-        <v>56</v>
-      </c>
+      <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
       <c r="AE38" s="1"/>
@@ -9547,8 +9952,9 @@
       <c r="AG38" s="1"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
     </row>
-    <row r="39" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A39" s="68" t="s">
         <v>44</v>
       </c>
@@ -9584,9 +9990,7 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
-      <c r="AB39" s="57">
-        <v>52</v>
-      </c>
+      <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
@@ -9594,8 +9998,9 @@
       <c r="AG39" s="1"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
     </row>
-    <row r="40" spans="1:35" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -9634,18 +10039,17 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
-      <c r="AB40" s="53">
-        <f>SUM(AB34:AB39)/6</f>
-        <v>52.333333333333336</v>
-      </c>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
       <c r="AE40" s="1"/>
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A41" s="126"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -9662,17 +10066,23 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="Q41" s="68" t="s">
+        <v>56</v>
+      </c>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
+      <c r="V41" s="68" t="s">
+        <v>60</v>
+      </c>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
-      <c r="AA41" s="1"/>
+      <c r="AA41" s="68" t="s">
+        <v>61</v>
+      </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
@@ -9681,8 +10091,9 @@
       <c r="AG41" s="1"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
+      <c r="AJ41" s="1"/>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
@@ -9710,27 +10121,46 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
+      <c r="Q42" s="137" t="s">
+        <v>52</v>
+      </c>
+      <c r="R42" s="126" t="s">
+        <v>53</v>
+      </c>
+      <c r="T42" s="68">
+        <f>X21*X22*SQRT((Y21/X21)^2+(Y22/X22)^2)</f>
+        <v>9.8579536416033129</v>
+      </c>
       <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-      <c r="Y42" s="1"/>
+      <c r="V42" s="137" t="s">
+        <v>52</v>
+      </c>
+      <c r="W42" s="126" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y42" s="68">
+        <f>X21*X22*SQRT((Y21/X21)^2+(Y22/X22)^2)</f>
+        <v>9.8579536416033129</v>
+      </c>
       <c r="Z42" s="1"/>
-      <c r="AA42" s="1"/>
-      <c r="AB42" s="1"/>
-      <c r="AC42" s="1"/>
-      <c r="AD42" s="1"/>
+      <c r="AA42" s="137" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB42" s="126" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD42" s="68">
+        <f>X21*X22*SQRT((Y21/X21)^2+(Y22/X22)^2)</f>
+        <v>9.8579536416033129</v>
+      </c>
       <c r="AE42" s="1"/>
       <c r="AF42" s="1"/>
       <c r="AG42" s="1"/>
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
+      <c r="AJ42" s="1"/>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -9748,26 +10178,48 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
+      <c r="R43" s="126" t="s">
+        <v>54</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T43" s="68">
+        <f>B37*10^-2*(X27^4)*SQRT((0.5/B37)^2+(S44/X27^4)^2)</f>
+        <v>1.705778781104631E-15</v>
+      </c>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
+      <c r="W43" s="126" t="s">
+        <v>54</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y43" s="71">
+        <f>I37*10^-2*X26^4*SQRT((0.5/I37)^2+(X44/X26^4)^2)</f>
+        <v>1.1475259877793456E-15</v>
+      </c>
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
+      <c r="AB43" s="126" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD43" s="71">
+        <f>P37*10^-2*X25^4*SQRT((0.5/P37)^2+(AC44/X25^4)^2)</f>
+        <v>1.0748027821555357E-15</v>
+      </c>
       <c r="AE43" s="1"/>
       <c r="AF43" s="1"/>
       <c r="AG43" s="1"/>
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
+      <c r="AJ43" s="1"/>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -9797,25 +10249,35 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
+      <c r="S44" s="1">
+        <f>X27^4*ABS(4*Z27/X27)</f>
+        <v>1.9965000000000003E-14</v>
+      </c>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
+      <c r="X44" s="138">
+        <f>X26^4*ABS(4*Z26/X26)</f>
+        <v>1.2458760000000002E-14</v>
+      </c>
+      <c r="Y44" s="138"/>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
-      <c r="AD44" s="1"/>
+      <c r="AC44" s="138">
+        <f>X25^4*ABS(4*Z25/X25)</f>
+        <v>1.1680320000000001E-14</v>
+      </c>
+      <c r="AD44" s="138"/>
       <c r="AE44" s="1"/>
       <c r="AF44" s="1"/>
       <c r="AG44" s="1"/>
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
+      <c r="AJ44" s="1"/>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -9832,18 +10294,33 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
+      <c r="Q45" s="137" t="s">
+        <v>57</v>
+      </c>
+      <c r="R45" s="126" t="s">
+        <v>58</v>
+      </c>
       <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
+      <c r="T45" s="68">
+        <f>X30*C37*10^-6*SQRT((Y30/X30)^2+(D37/C37)^2)</f>
+        <v>1.3194135265229834E-9</v>
+      </c>
       <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
-      <c r="W45" s="1"/>
+      <c r="V45" s="137" t="s">
+        <v>57</v>
+      </c>
+      <c r="W45" s="126" t="s">
+        <v>58</v>
+      </c>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
-      <c r="AA45" s="1"/>
-      <c r="AB45" s="1"/>
+      <c r="AA45" s="137" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB45" s="126" t="s">
+        <v>58</v>
+      </c>
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
       <c r="AE45" s="1"/>
@@ -9851,8 +10328,9 @@
       <c r="AG45" s="1"/>
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
+      <c r="AJ45" s="1"/>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -9869,27 +10347,49 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
+      <c r="Q46" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
+      <c r="T46" s="123">
+        <f>B44*SQRT((T42/(X21*X22))^2+(T43/(B37*10^-2*X27^4))^2+(Y30/X30)^2+(D37/C37)^2)</f>
+        <v>3.5280392096732465E-4</v>
+      </c>
       <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
+      <c r="V46" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
-      <c r="Y46" s="1"/>
+      <c r="Y46" s="123">
+        <f>C44*SQRT((Y42/(X21*X22))^2+(Y43/(I37*10^-2*X26^4))^2+(Y29/X29)^2+(K37/J37)^2)</f>
+        <v>7.4770838307456158E-4</v>
+      </c>
       <c r="Z46" s="1"/>
-      <c r="AA46" s="1"/>
+      <c r="AA46" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
-      <c r="AD46" s="1"/>
-      <c r="AE46" s="1"/>
-      <c r="AF46" s="1"/>
+      <c r="AD46" s="123">
+        <f>D44*SQRT((AD42/(X21*X22))^2 + (AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(R37/Q37)^2)</f>
+        <v>6.719904064974593E-4</v>
+      </c>
+      <c r="AE46" s="123">
+        <f>T38*SQRT((AD42/(X21*X22))^2+(AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(R37/Q37)^2)</f>
+        <v>4.8996498930128332E-4</v>
+      </c>
+      <c r="AF46" s="1">
+        <f>T38*SQRT((AD42/(X21*X22))^2+(AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(R37/Q37)^2)</f>
+        <v>4.8996498930128332E-4</v>
+      </c>
       <c r="AG46" s="1"/>
       <c r="AH46" s="1"/>
       <c r="AI46" s="1"/>
+      <c r="AJ46" s="1"/>
     </row>
-    <row r="47" spans="1:35" ht="60" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:36" ht="60" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="135" t="s">
         <v>50</v>
@@ -9916,7 +10416,9 @@
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
+      <c r="Y47" s="1">
+        <v>2.6028167053712123E-4</v>
+      </c>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
@@ -9927,8 +10429,9 @@
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
+      <c r="AJ47" s="1"/>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -9964,10 +10467,13 @@
       <c r="AG48" s="1"/>
       <c r="AH48" s="1"/>
       <c r="AI48" s="1"/>
+      <c r="AJ48" s="1"/>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -10001,8 +10507,9 @@
       <c r="AG49" s="1"/>
       <c r="AH49" s="1"/>
       <c r="AI49" s="1"/>
+      <c r="AJ49" s="1"/>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -10038,8 +10545,9 @@
       <c r="AG50" s="1"/>
       <c r="AH50" s="1"/>
       <c r="AI50" s="1"/>
+      <c r="AJ50" s="1"/>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -10075,8 +10583,9 @@
       <c r="AG51" s="1"/>
       <c r="AH51" s="1"/>
       <c r="AI51" s="1"/>
+      <c r="AJ51" s="1"/>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -10112,8 +10621,9 @@
       <c r="AG52" s="1"/>
       <c r="AH52" s="1"/>
       <c r="AI52" s="1"/>
+      <c r="AJ52" s="1"/>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -10149,8 +10659,9 @@
       <c r="AG53" s="1"/>
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
+      <c r="AJ53" s="1"/>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -10186,8 +10697,9 @@
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
       <c r="AI54" s="1"/>
+      <c r="AJ54" s="1"/>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -10223,8 +10735,9 @@
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
       <c r="AI55" s="1"/>
+      <c r="AJ55" s="1"/>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -10260,8 +10773,9 @@
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -10297,8 +10811,9 @@
       <c r="AG57" s="1"/>
       <c r="AH57" s="1"/>
       <c r="AI57" s="1"/>
+      <c r="AJ57" s="1"/>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="F58" s="79"/>
       <c r="G58" s="79"/>
       <c r="H58" s="79"/>
@@ -10312,7 +10827,7 @@
       <c r="P58" s="79"/>
       <c r="Q58" s="79"/>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
       <c r="F59" s="79"/>
       <c r="G59" s="80"/>
       <c r="H59" s="81"/>
@@ -10326,7 +10841,7 @@
       <c r="P59" s="79"/>
       <c r="Q59" s="79"/>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
       <c r="F60" s="79"/>
       <c r="G60" s="80"/>
       <c r="H60" s="81"/>
@@ -10340,7 +10855,7 @@
       <c r="P60" s="79"/>
       <c r="Q60" s="79"/>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
       <c r="F61" s="79"/>
       <c r="G61" s="80"/>
       <c r="H61" s="81"/>
@@ -10354,7 +10869,7 @@
       <c r="P61" s="79"/>
       <c r="Q61" s="79"/>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B62" s="71" t="s">
         <v>38</v>
       </c>
@@ -10371,7 +10886,7 @@
       <c r="P62" s="79"/>
       <c r="Q62" s="79"/>
     </row>
-    <row r="63" spans="1:35" s="71" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:36" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="71" t="s">
         <v>23</v>
       </c>
@@ -10407,7 +10922,7 @@
       <c r="P63" s="86"/>
       <c r="Q63" s="86"/>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B64" s="89">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
finished cp7, needs tidying and answer
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -2423,7 +2423,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2877,7 +2876,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2975,7 +2973,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3055,11 +3052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-385266240"/>
-        <c:axId val="-385270384"/>
+        <c:axId val="302552864"/>
+        <c:axId val="268391296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-385266240"/>
+        <c:axId val="302552864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3081,19 +3078,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-385270384"/>
+        <c:crossAx val="268391296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-385270384"/>
+        <c:axId val="268391296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3115,14 +3111,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-385266240"/>
+        <c:crossAx val="302552864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3179,7 +3174,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3354,11 +3348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-385416144"/>
-        <c:axId val="-385414512"/>
+        <c:axId val="304990720"/>
+        <c:axId val="304992352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-385416144"/>
+        <c:axId val="304990720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3415,12 +3409,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-385414512"/>
+        <c:crossAx val="304992352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-385414512"/>
+        <c:axId val="304992352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3477,7 +3471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-385416144"/>
+        <c:crossAx val="304990720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3567,7 +3561,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3715,11 +3708,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-385743328"/>
-        <c:axId val="-385747200"/>
+        <c:axId val="302499632"/>
+        <c:axId val="302501680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-385743328"/>
+        <c:axId val="302499632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3776,12 +3769,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-385747200"/>
+        <c:crossAx val="302501680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-385747200"/>
+        <c:axId val="302501680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3838,7 +3831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-385743328"/>
+        <c:crossAx val="302499632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3928,7 +3921,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4076,11 +4068,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-385795040"/>
-        <c:axId val="-385809200"/>
+        <c:axId val="266954128"/>
+        <c:axId val="266956176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-385795040"/>
+        <c:axId val="266954128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4137,12 +4129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-385809200"/>
+        <c:crossAx val="266956176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-385809200"/>
+        <c:axId val="266956176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4199,7 +4191,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-385795040"/>
+        <c:crossAx val="266954128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7161,7 +7153,7 @@
   <dimension ref="A1:AJ117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7540,7 +7532,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N5" s="32">
-        <f t="shared" ref="N4:N11" si="8">((M5/($X$32+$Y$32))^2+((M5+$J$7)/$X$32)^2)^0.5</f>
+        <f t="shared" ref="N5:N11" si="8">((M5/($X$32+$Y$32))^2+((M5+$J$7)/$X$32)^2)^0.5</f>
         <v>6.0759360008565948E-3</v>
       </c>
       <c r="O5" s="21">

</xml_diff>

<commit_message>
data analysed, python, more work
lab report:
- raw data analysed and now more or less completed with it
- python graph with residuals created
- added graph into tex, along with new data

python:
- forgot to git add the new images
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Data!$G$102:$H$102</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Data!$A$102:$B$102</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -32,7 +32,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Data!$R$36</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Data!$D$36</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -42,7 +42,7 @@
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
   <si>
     <t>data</t>
   </si>
@@ -665,6 +665,21 @@
   </si>
   <si>
     <t>Normalised Residuals</t>
+  </si>
+  <si>
+    <t>old V' error</t>
+  </si>
+  <si>
+    <t>old v' error</t>
+  </si>
+  <si>
+    <t>^ standard error</t>
+  </si>
+  <si>
+    <t>^ average h (cm)</t>
+  </si>
+  <si>
+    <t>^ average V' (cm^3s^-1)</t>
   </si>
 </sst>
 </file>
@@ -1327,9 +1342,63 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="180">
+  <cellStyleXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1904,9 +1973,6 @@
     <xf numFmtId="166" fontId="0" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1946,8 +2012,11 @@
     <xf numFmtId="11" fontId="0" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="180">
+  <cellStyles count="234">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2038,6 +2107,33 @@
     <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2127,6 +2223,33 @@
     <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2204,43 +2327,43 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="13"/>
                   <c:pt idx="0">
-                    <c:v>0.00555560507522512</c:v>
+                    <c:v>0.00556045082089978</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.00647702381598444</c:v>
+                    <c:v>0.00557214944939765</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.00657449621510504</c:v>
+                    <c:v>0.00557562789263145</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00678602270665906</c:v>
+                    <c:v>0.00558418799119772</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00694329040957926</c:v>
+                    <c:v>0.00559142091571405</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.00769276158508073</c:v>
+                    <c:v>0.00563541595587823</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.00790352006016233</c:v>
+                    <c:v>0.00565046836951423</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00803999281421701</c:v>
+                    <c:v>0.00566081282504454</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.00805520190016966</c:v>
+                    <c:v>0.00566199432055071</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.00857729546085099</c:v>
+                    <c:v>0.00570595044564296</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.00931279028852496</c:v>
+                    <c:v>0.00577858830532677</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.0102056033268215</c:v>
+                    <c:v>0.00588246543814092</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.0110796647926824</c:v>
+                    <c:v>0.00599960819846658</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2252,43 +2375,43 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="13"/>
                   <c:pt idx="0">
-                    <c:v>0.00555560507522512</c:v>
+                    <c:v>0.00556045082089978</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.00647702381598444</c:v>
+                    <c:v>0.00557214944939765</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.00657449621510504</c:v>
+                    <c:v>0.00557562789263145</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00678602270665906</c:v>
+                    <c:v>0.00558418799119772</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00694329040957926</c:v>
+                    <c:v>0.00559142091571405</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.00769276158508073</c:v>
+                    <c:v>0.00563541595587823</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.00790352006016233</c:v>
+                    <c:v>0.00565046836951423</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00803999281421701</c:v>
+                    <c:v>0.00566081282504454</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.00805520190016966</c:v>
+                    <c:v>0.00566199432055071</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.00857729546085099</c:v>
+                    <c:v>0.00570595044564296</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0.00931279028852496</c:v>
+                    <c:v>0.00577858830532677</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0.0102056033268215</c:v>
+                    <c:v>0.00588246543814092</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0.0110796647926824</c:v>
+                    <c:v>0.00599960819846658</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2423,6 +2546,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2481,43 +2605,43 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.0365573675446015</c:v>
+                  <c:v>0.0321786816547358</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0608036676729043</c:v>
+                  <c:v>0.0573178452365171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.085049967801207</c:v>
+                  <c:v>0.0824570088182983</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10929626792951</c:v>
+                  <c:v>0.10759617240008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.133542568057813</c:v>
+                  <c:v>0.132735335981861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.157788868186115</c:v>
+                  <c:v>0.157874499563642</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.182035168314418</c:v>
+                  <c:v>0.183013663145423</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.206281468442721</c:v>
+                  <c:v>0.208152826727204</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.230527768571024</c:v>
+                  <c:v>0.233291990308986</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.254774068699326</c:v>
+                  <c:v>0.258431153890767</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.279020368827629</c:v>
+                  <c:v>0.283570317472548</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.327512969084235</c:v>
+                  <c:v>0.333848644636111</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.37600556934084</c:v>
+                  <c:v>0.384126971799673</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2559,28 +2683,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.00579482057061753</c:v>
+                    <c:v>0.00555677977618867</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.00607593600085659</c:v>
+                    <c:v>0.00556111579009874</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.00608259310158183</c:v>
+                    <c:v>0.00556125385653654</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00664461266310471</c:v>
+                    <c:v>0.00557831383437482</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00675761854468597</c:v>
+                    <c:v>0.00558295965582987</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.00702978921630487</c:v>
+                    <c:v>0.00559570567462091</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0074914265710133</c:v>
+                    <c:v>0.00562210730458561</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00808564672519466</c:v>
+                    <c:v>0.00566437653073164</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2592,28 +2716,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.00579482057061753</c:v>
+                    <c:v>0.00555677977618867</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.00607593600085659</c:v>
+                    <c:v>0.00556111579009874</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.00608259310158183</c:v>
+                    <c:v>0.00556125385653654</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00664461266310471</c:v>
+                    <c:v>0.00557831383437482</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00675761854468597</c:v>
+                    <c:v>0.00558295965582987</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.00702978921630487</c:v>
+                    <c:v>0.00559570567462091</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0074914265710133</c:v>
+                    <c:v>0.00562210730458561</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00808564672519466</c:v>
+                    <c:v>0.00566437653073164</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2722,28 +2846,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.000793378274030248</c:v>
+                    <c:v>0.00555653563183346</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.000932858901973321</c:v>
+                    <c:v>0.00555784778164324</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.00139045826361958</c:v>
+                    <c:v>0.00556543657644733</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00162579267809792</c:v>
+                    <c:v>0.00557121608649271</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00181226112322235</c:v>
+                    <c:v>0.00557668215229535</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.00198261445704349</c:v>
+                    <c:v>0.00558235551265192</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0021792555150104</c:v>
+                    <c:v>0.00558970626104521</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00275502725285795</c:v>
+                    <c:v>0.00561612435206025</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2755,28 +2879,28 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.000793378274030248</c:v>
+                    <c:v>0.00555653563183346</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.000932858901973321</c:v>
+                    <c:v>0.00555784778164324</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.00139045826361958</c:v>
+                    <c:v>0.00556543657644733</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.00162579267809792</c:v>
+                    <c:v>0.00557121608649271</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.00181226112322235</c:v>
+                    <c:v>0.00557668215229535</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.00198261445704349</c:v>
+                    <c:v>0.00558235551265192</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.0021792555150104</c:v>
+                    <c:v>0.00558970626104521</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.00275502725285795</c:v>
+                    <c:v>0.00561612435206025</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2876,6 +3000,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2973,6 +3098,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3052,11 +3178,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302552864"/>
-        <c:axId val="268391296"/>
+        <c:axId val="-1996630416"/>
+        <c:axId val="-1996627568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302552864"/>
+        <c:axId val="-1996630416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3078,18 +3204,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="268391296"/>
+        <c:crossAx val="-1996627568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="268391296"/>
+        <c:axId val="-1996627568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3111,13 +3238,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="302552864"/>
+        <c:crossAx val="-1996630416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3174,6 +3302,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3300,40 +3429,40 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0056648546776207</c:v>
+                  <c:v>0.0100435405674864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0169741101048735</c:v>
+                  <c:v>0.0204599325412607</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000505587754348516</c:v>
+                  <c:v>0.00309854673725726</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.00707404570728757</c:v>
+                  <c:v>-0.0053739501778573</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0190981236133681</c:v>
+                  <c:v>-0.0182908915374163</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0133222429249958</c:v>
+                  <c:v>0.0132366115474691</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00463149835224863</c:v>
+                  <c:v>0.00365300352124348</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.00961480177605414</c:v>
+                  <c:v>-0.0114861600605378</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0327499907932458</c:v>
+                  <c:v>-0.0355142125312079</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0192185131437708</c:v>
+                  <c:v>-0.0228755983352113</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.00875740895014865</c:v>
+                  <c:v>0.00420746030522961</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0224870309157654</c:v>
+                  <c:v>0.0161513553638894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3348,11 +3477,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="304990720"/>
-        <c:axId val="304992352"/>
+        <c:axId val="-1996609488"/>
+        <c:axId val="-1996607440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="304990720"/>
+        <c:axId val="-1996609488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3409,12 +3538,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304992352"/>
+        <c:crossAx val="-1996607440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="304992352"/>
+        <c:axId val="-1996607440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3471,7 +3600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304990720"/>
+        <c:crossAx val="-1996609488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3561,6 +3690,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3708,11 +3838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="302499632"/>
-        <c:axId val="302501680"/>
+        <c:axId val="-1977901296"/>
+        <c:axId val="-1977899248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="302499632"/>
+        <c:axId val="-1977901296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3769,12 +3899,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302501680"/>
+        <c:crossAx val="-1977899248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="302501680"/>
+        <c:axId val="-1977899248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3831,7 +3961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302499632"/>
+        <c:crossAx val="-1977901296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3921,6 +4051,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4068,11 +4199,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266954128"/>
-        <c:axId val="266956176"/>
+        <c:axId val="-1977908320"/>
+        <c:axId val="-1977906272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266954128"/>
+        <c:axId val="-1977908320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4129,12 +4260,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="266956176"/>
+        <c:crossAx val="-1977906272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266956176"/>
+        <c:axId val="-1977906272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4191,7 +4322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="266954128"/>
+        <c:crossAx val="-1977908320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7150,29 +7281,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ117"/>
+  <dimension ref="A1:AJ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="2"/>
-    <col min="10" max="10" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.1640625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.1640625" style="2" customWidth="1"/>
     <col min="20" max="20" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.1640625" style="2"/>
@@ -7298,8 +7431,8 @@
       <c r="H3" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="63">
-        <v>5.5556050752251177E-3</v>
+      <c r="I3" s="63" t="s">
+        <v>66</v>
       </c>
       <c r="J3" s="56" t="s">
         <v>22</v>
@@ -7325,7 +7458,9 @@
       <c r="Q3" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="63"/>
+      <c r="R3" s="63" t="s">
+        <v>66</v>
+      </c>
       <c r="S3" s="56" t="s">
         <v>25</v>
       </c>
@@ -7350,8 +7485,12 @@
       <c r="Z3" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
+      <c r="AA3" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB3" s="63">
+        <v>5.6527221077931351E-4</v>
+      </c>
       <c r="AC3" s="56" t="s">
         <v>29</v>
       </c>
@@ -7392,8 +7531,8 @@
         <v>4.2222222222222223E-2</v>
       </c>
       <c r="E4" s="32">
-        <f>D4*SQRT(($A$7/C4)^2+($A$5/$X$32)^2)</f>
-        <v>5.5556050752251177E-3</v>
+        <f>SQRT( ((C4+$A$7)/$X$32 - C4/$X$32)^2 + (C4/($X$32+$Y$32) - C4/$X$32)^2)</f>
+        <v>5.5604508208997785E-3</v>
       </c>
       <c r="F4" s="18">
         <v>4.2</v>
@@ -7420,8 +7559,8 @@
         <v>2.1111111111111112E-2</v>
       </c>
       <c r="N4" s="32">
-        <f>((M4/($X$32+$Y$32))^2+((M4+$J$7)/$X$32)^2)^0.5</f>
-        <v>5.7948205706175315E-3</v>
+        <f>SQRT( ((L4+$J$7)/$X$32 - L4/$X$32)^2 + (L4/($X$32+$Y$32) - L4/$X$32)^2)</f>
+        <v>5.5567797761886693E-3</v>
       </c>
       <c r="O4" s="18">
         <v>1.4</v>
@@ -7433,7 +7572,9 @@
       <c r="Q4" s="25">
         <v>12.4</v>
       </c>
-      <c r="R4" s="1"/>
+      <c r="R4" s="1">
+        <v>5.7948205706175315E-3</v>
+      </c>
       <c r="S4" s="14" t="s">
         <v>16</v>
       </c>
@@ -7448,21 +7589,25 @@
         <v>1.8888888888888889E-2</v>
       </c>
       <c r="W4" s="32">
-        <f t="shared" ref="W4:W11" si="3">((V4/($X$32+$Y$32))^2+((V4+$S$7)/$X$32)^2)^0.5</f>
-        <v>7.9337827403024844E-4</v>
+        <f>SQRT( ((U4+$S$7)/$X$32 - U4/$X$32)^2 + (U4/($X$32+$Y$32) - U4/$X$32)^2)</f>
+        <v>5.5565356318334628E-3</v>
       </c>
       <c r="X4" s="18">
         <v>1.3</v>
       </c>
       <c r="Y4" s="22">
-        <f t="shared" ref="Y4" si="4">X4/1.001</f>
+        <f t="shared" ref="Y4" si="3">X4/1.001</f>
         <v>1.2987012987012989</v>
       </c>
       <c r="Z4" s="25">
         <v>12.6</v>
       </c>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+      <c r="AA4" s="1">
+        <v>7.9337827403024844E-4</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>5.7802803423466227E-4</v>
+      </c>
       <c r="AC4" s="14" t="s">
         <v>16</v>
       </c>
@@ -7484,7 +7629,7 @@
         <v>1.9</v>
       </c>
       <c r="AI4" s="22">
-        <f t="shared" ref="AI4" si="5">AH4/1.001</f>
+        <f t="shared" ref="AI4" si="4">AH4/1.001</f>
         <v>1.8981018981018982</v>
       </c>
       <c r="AJ4" s="25"/>
@@ -7504,8 +7649,8 @@
         <v>7.7777777777777779E-2</v>
       </c>
       <c r="E5" s="32">
-        <f t="shared" ref="E5:E16" si="6">((D5/($X$32+$Y$32))^2+((D5+$A$7)/$X$32)^2)^0.5</f>
-        <v>6.477023815984439E-3</v>
+        <f t="shared" ref="E5:E16" si="5">SQRT( ((C5+$A$7)/$X$32 - C5/$X$32)^2 + (C5/($X$32+$Y$32) - C5/$X$32)^2)</f>
+        <v>5.5721494493976521E-3</v>
       </c>
       <c r="F5" s="21">
         <v>6.8</v>
@@ -7528,24 +7673,26 @@
         <v>4.05</v>
       </c>
       <c r="M5" s="31">
-        <f t="shared" ref="M5" si="7">L5/90</f>
+        <f t="shared" ref="M5" si="6">L5/90</f>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N5" s="32">
-        <f t="shared" ref="N5:N11" si="8">((M5/($X$32+$Y$32))^2+((M5+$J$7)/$X$32)^2)^0.5</f>
-        <v>6.0759360008565948E-3</v>
+        <f t="shared" ref="N5:N11" si="7">SQRT( ((L5+$J$7)/$X$32 - L5/$X$32)^2 + (L5/($X$32+$Y$32) - L5/$X$32)^2)</f>
+        <v>5.5611157900987435E-3</v>
       </c>
       <c r="O5" s="21">
         <v>3.5</v>
       </c>
       <c r="P5" s="23">
-        <f t="shared" ref="P5:P11" si="9">O5/1.001</f>
+        <f t="shared" ref="P5:P11" si="8">O5/1.001</f>
         <v>3.4965034965034967</v>
       </c>
       <c r="Q5" s="26">
         <v>12.3</v>
       </c>
-      <c r="R5" s="1"/>
+      <c r="R5" s="1">
+        <v>6.0759360008565948E-3</v>
+      </c>
       <c r="S5" s="50">
         <v>0.05</v>
       </c>
@@ -7556,12 +7703,12 @@
         <v>2.6</v>
       </c>
       <c r="V5" s="31">
-        <f t="shared" ref="V5" si="10">U5/90</f>
+        <f t="shared" ref="V5" si="9">U5/90</f>
         <v>2.8888888888888891E-2</v>
       </c>
       <c r="W5" s="32">
-        <f t="shared" si="3"/>
-        <v>9.328589019733215E-4</v>
+        <f t="shared" ref="W5:W11" si="10">SQRT( ((U5+$S$7)/$X$32 - U5/$X$32)^2 + (U5/($X$32+$Y$32) - U5/$X$32)^2)</f>
+        <v>5.5578477816432435E-3</v>
       </c>
       <c r="X5" s="21">
         <v>2.5</v>
@@ -7573,8 +7720,12 @@
       <c r="Z5" s="26">
         <v>12.1</v>
       </c>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
+      <c r="AA5" s="1">
+        <v>9.328589019733215E-4</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>6.4693796526574211E-4</v>
+      </c>
       <c r="AC5" s="50">
         <v>0.05</v>
       </c>
@@ -7601,8 +7752,8 @@
         <v>8.5555555555555551E-2</v>
       </c>
       <c r="E6" s="32">
-        <f t="shared" si="6"/>
-        <v>6.5744962151050457E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.5756278926314485E-3</v>
       </c>
       <c r="F6" s="21">
         <v>7.5</v>
@@ -7629,20 +7780,22 @@
         <v>4.5555555555555551E-2</v>
       </c>
       <c r="N6" s="32">
-        <f t="shared" si="8"/>
-        <v>6.0825931015818305E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.5612538565365383E-3</v>
       </c>
       <c r="O6" s="21">
         <v>4</v>
       </c>
       <c r="P6" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>3.9960039960039966</v>
       </c>
       <c r="Q6" s="26">
         <v>12.5</v>
       </c>
-      <c r="R6" s="1"/>
+      <c r="R6" s="1">
+        <v>6.0825931015818305E-3</v>
+      </c>
       <c r="S6" s="51" t="s">
         <v>6</v>
       </c>
@@ -7657,8 +7810,8 @@
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="W6" s="32">
-        <f t="shared" si="3"/>
-        <v>1.3904582636195852E-3</v>
+        <f t="shared" si="10"/>
+        <v>5.5654365764473274E-3</v>
       </c>
       <c r="X6" s="21">
         <v>5.3</v>
@@ -7670,8 +7823,12 @@
       <c r="Z6" s="26">
         <v>12.1</v>
       </c>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
+      <c r="AA6" s="1">
+        <v>1.3904582636195852E-3</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>6.9490512074647922E-4</v>
+      </c>
       <c r="AC6" s="15" t="s">
         <v>6</v>
       </c>
@@ -7713,8 +7870,8 @@
         <v>0.10222222222222221</v>
       </c>
       <c r="E7" s="32">
-        <f t="shared" si="6"/>
-        <v>6.7860227066590655E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.5841879911977246E-3</v>
       </c>
       <c r="F7" s="21">
         <v>8.6</v>
@@ -7741,22 +7898,24 @@
         <v>9.1111111111111101E-2</v>
       </c>
       <c r="N7" s="32">
-        <f t="shared" si="8"/>
-        <v>6.6446126631047103E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.5783138343748206E-3</v>
       </c>
       <c r="O7" s="21">
         <v>7.9</v>
       </c>
       <c r="P7" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>7.8921078921078935</v>
       </c>
       <c r="Q7" s="26">
         <v>12.6</v>
       </c>
-      <c r="R7" s="1"/>
+      <c r="R7" s="1">
+        <v>6.6446126631047103E-3</v>
+      </c>
       <c r="S7" s="50">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="T7" s="19">
         <v>8</v>
@@ -7769,8 +7928,8 @@
         <v>7.5555555555555556E-2</v>
       </c>
       <c r="W7" s="32">
-        <f t="shared" si="3"/>
-        <v>1.6257926780979199E-3</v>
+        <f t="shared" si="10"/>
+        <v>5.5712160864927127E-3</v>
       </c>
       <c r="X7" s="21">
         <v>6.8</v>
@@ -7782,8 +7941,12 @@
       <c r="Z7" s="26">
         <v>12.4</v>
       </c>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
+      <c r="AA7" s="1">
+        <v>1.6257926780979199E-3</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>7.3744713178231403E-4</v>
+      </c>
       <c r="AC7" s="50">
         <v>0.5</v>
       </c>
@@ -7808,8 +7971,8 @@
         <v>0.11444444444444445</v>
       </c>
       <c r="E8" s="32">
-        <f t="shared" si="6"/>
-        <v>6.9432904095792615E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.5914209157140486E-3</v>
       </c>
       <c r="F8" s="21">
         <v>10.6</v>
@@ -7834,20 +7997,22 @@
         <v>0.1</v>
       </c>
       <c r="N8" s="32">
-        <f t="shared" si="8"/>
-        <v>6.7576185446859742E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.5829596558298698E-3</v>
       </c>
       <c r="O8" s="21">
         <v>9</v>
       </c>
       <c r="P8" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>8.9910089910089912</v>
       </c>
       <c r="Q8" s="26">
         <v>12.9</v>
       </c>
-      <c r="R8" s="1"/>
+      <c r="R8" s="1">
+        <v>6.7576185446859742E-3</v>
+      </c>
       <c r="T8" s="19">
         <v>10</v>
       </c>
@@ -7859,8 +8024,8 @@
         <v>8.7777777777777788E-2</v>
       </c>
       <c r="W8" s="32">
-        <f t="shared" si="3"/>
-        <v>1.8122611232223463E-3</v>
+        <f t="shared" si="10"/>
+        <v>5.5766821522953468E-3</v>
       </c>
       <c r="X8" s="21">
         <v>7.8</v>
@@ -7872,8 +8037,12 @@
       <c r="Z8" s="26">
         <v>12.4</v>
       </c>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
+      <c r="AA8" s="1">
+        <v>1.8122611232223463E-3</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>7.7919029388187622E-4</v>
+      </c>
       <c r="AC8" s="1"/>
       <c r="AD8" s="47">
         <v>6</v>
@@ -7911,8 +8080,8 @@
         <v>0.1711111111111111</v>
       </c>
       <c r="E9" s="32">
-        <f t="shared" si="6"/>
-        <v>7.6927615850807271E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.6354159558782346E-3</v>
       </c>
       <c r="F9" s="21">
         <v>15.3</v>
@@ -7939,20 +8108,22 @@
         <v>0.12111111111111111</v>
       </c>
       <c r="N9" s="32">
-        <f t="shared" si="8"/>
-        <v>7.0297892163048705E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.5957056746209063E-3</v>
       </c>
       <c r="O9" s="21">
         <v>10.9</v>
       </c>
       <c r="P9" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>10.88911088911089</v>
       </c>
       <c r="Q9" s="26">
         <v>12.9</v>
       </c>
-      <c r="R9" s="1"/>
+      <c r="R9" s="1">
+        <v>7.0297892163048705E-3</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="19">
         <v>12</v>
@@ -7965,8 +8136,8 @@
         <v>9.8888888888888887E-2</v>
       </c>
       <c r="W9" s="32">
-        <f t="shared" si="3"/>
-        <v>1.9826144570434887E-3</v>
+        <f t="shared" si="10"/>
+        <v>5.5823555126519259E-3</v>
       </c>
       <c r="X9" s="21">
         <v>8.6999999999999993</v>
@@ -7978,8 +8149,12 @@
       <c r="Z9" s="26">
         <v>12.5</v>
       </c>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
+      <c r="AA9" s="1">
+        <v>1.9826144570434887E-3</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>8.3021715786444467E-4</v>
+      </c>
       <c r="AC9" s="1"/>
       <c r="AD9" s="47"/>
       <c r="AE9" s="20"/>
@@ -8002,8 +8177,8 @@
         <v>0.18666666666666668</v>
       </c>
       <c r="E10" s="32">
-        <f t="shared" si="6"/>
-        <v>7.9035200601623289E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.6504683695142287E-3</v>
       </c>
       <c r="F10" s="21">
         <v>16.600000000000001</v>
@@ -8030,20 +8205,22 @@
         <v>0.15611111111111112</v>
       </c>
       <c r="N10" s="32">
-        <f t="shared" si="8"/>
-        <v>7.4914265710133007E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.6221073045856149E-3</v>
       </c>
       <c r="O10" s="21">
         <v>13.9</v>
       </c>
       <c r="P10" s="23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>13.886113886113888</v>
       </c>
       <c r="Q10" s="26">
         <v>12.9</v>
       </c>
-      <c r="R10" s="1"/>
+      <c r="R10" s="1">
+        <v>7.4914265710133007E-3</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="19">
         <v>14</v>
@@ -8056,8 +8233,8 @@
         <v>0.11166666666666668</v>
       </c>
       <c r="W10" s="32">
-        <f t="shared" si="3"/>
-        <v>2.1792555150103999E-3</v>
+        <f t="shared" si="10"/>
+        <v>5.5897062610452079E-3</v>
       </c>
       <c r="X10" s="21">
         <v>10</v>
@@ -8069,8 +8246,12 @@
       <c r="Z10" s="26">
         <v>12.4</v>
       </c>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
+      <c r="AA10" s="1">
+        <v>2.1792555150103999E-3</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>9.9262136902690382E-4</v>
+      </c>
       <c r="AC10" s="1"/>
       <c r="AD10" s="47">
         <v>8</v>
@@ -8108,8 +8289,8 @@
         <v>0.19666666666666666</v>
       </c>
       <c r="E11" s="32">
-        <f t="shared" si="6"/>
-        <v>8.039992814217016E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.6608128250445382E-3</v>
       </c>
       <c r="F11" s="21">
         <v>17.600000000000001</v>
@@ -8135,47 +8316,51 @@
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="N11" s="132">
+      <c r="N11" s="32">
+        <f t="shared" si="7"/>
+        <v>5.6643765307316371E-3</v>
+      </c>
+      <c r="O11" s="132">
+        <v>17.3</v>
+      </c>
+      <c r="P11" s="133">
         <f t="shared" si="8"/>
+        <v>17.282717282717286</v>
+      </c>
+      <c r="Q11" s="134">
+        <v>12.8</v>
+      </c>
+      <c r="R11" s="1">
         <v>8.0856467251946649E-3</v>
       </c>
-      <c r="O11" s="133">
-        <v>17.3</v>
-      </c>
-      <c r="P11" s="134">
-        <f t="shared" si="9"/>
-        <v>17.282717282717286</v>
-      </c>
-      <c r="Q11" s="135">
-        <v>12.8</v>
-      </c>
-      <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="136">
+      <c r="T11" s="135">
         <v>16</v>
       </c>
-      <c r="U11" s="137">
+      <c r="U11" s="136">
         <v>13.4</v>
       </c>
       <c r="V11" s="131">
         <f t="shared" si="13"/>
         <v>0.1488888888888889</v>
       </c>
-      <c r="W11" s="132">
-        <f t="shared" si="3"/>
-        <v>2.7550272528579526E-3</v>
-      </c>
-      <c r="X11" s="133">
+      <c r="W11" s="32">
+        <f t="shared" si="10"/>
+        <v>5.6161243520602517E-3</v>
+      </c>
+      <c r="X11" s="132">
         <v>13.5</v>
       </c>
-      <c r="Y11" s="134">
+      <c r="Y11" s="133">
         <f t="shared" si="11"/>
         <v>13.486513486513488</v>
       </c>
-      <c r="Z11" s="135">
+      <c r="Z11" s="134">
         <v>12.5</v>
       </c>
-      <c r="AA11" s="1"/>
+      <c r="AA11" s="1">
+        <v>2.7550272528579526E-3</v>
+      </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="47"/>
@@ -8199,8 +8384,8 @@
         <v>0.19777777777777777</v>
       </c>
       <c r="E12" s="32">
-        <f t="shared" si="6"/>
-        <v>8.0552019001696572E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.6619943205507136E-3</v>
       </c>
       <c r="F12" s="21">
         <v>17.600000000000001</v>
@@ -8221,10 +8406,10 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="141" t="s">
+      <c r="P12" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="140">
+      <c r="Q12" s="139">
         <f>AVERAGE(Q4:Q11)</f>
         <v>12.662500000000001</v>
       </c>
@@ -8235,10 +8420,10 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="139" t="s">
+      <c r="Y12" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="Z12" s="140">
+      <c r="Z12" s="139">
         <f>AVERAGE(Z4:Z11)</f>
         <v>12.375</v>
       </c>
@@ -8281,8 +8466,8 @@
         <v>0.23555555555555555</v>
       </c>
       <c r="E13" s="32">
-        <f t="shared" si="6"/>
-        <v>8.5772954608509949E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.7059504456429657E-3</v>
       </c>
       <c r="F13" s="21">
         <v>21.2</v>
@@ -8338,8 +8523,8 @@
         <v>0.28777777777777774</v>
       </c>
       <c r="E14" s="32">
-        <f t="shared" si="6"/>
-        <v>9.3127902885249674E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.7785883053267737E-3</v>
       </c>
       <c r="F14" s="21">
         <v>25.7</v>
@@ -8410,8 +8595,8 @@
         <v>0.35</v>
       </c>
       <c r="E15" s="32">
-        <f t="shared" si="6"/>
-        <v>1.0205603326821473E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.8824654381409254E-3</v>
       </c>
       <c r="F15" s="21">
         <v>31.3</v>
@@ -8471,28 +8656,28 @@
     </row>
     <row r="16" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="136">
+      <c r="B16" s="135">
         <v>16</v>
       </c>
-      <c r="C16" s="137">
+      <c r="C16" s="136">
         <v>36.9</v>
       </c>
       <c r="D16" s="131">
         <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
-      <c r="E16" s="132">
-        <f t="shared" si="6"/>
-        <v>1.1079664792682402E-2</v>
-      </c>
-      <c r="F16" s="133">
+      <c r="E16" s="32">
+        <f t="shared" si="5"/>
+        <v>5.9996081984665783E-3</v>
+      </c>
+      <c r="F16" s="132">
         <v>36.5</v>
       </c>
-      <c r="G16" s="134">
+      <c r="G16" s="133">
         <f t="shared" si="1"/>
         <v>36.463536463536471</v>
       </c>
-      <c r="H16" s="138">
+      <c r="H16" s="137">
         <v>13.6</v>
       </c>
       <c r="I16" s="1">
@@ -8548,10 +8733,10 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="139" t="s">
+      <c r="G17" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="140">
+      <c r="H17" s="139">
         <f>AVERAGE(H9:H16)</f>
         <v>12.799999999999999</v>
       </c>
@@ -8713,19 +8898,19 @@
       </c>
       <c r="C20" s="35">
         <f>$A$102*B20+$B$102</f>
-        <v>3.6557367544601524E-2</v>
+        <v>3.2178681654735836E-2</v>
       </c>
       <c r="D20" s="36">
         <f>D4-C20</f>
-        <v>5.6648546776206996E-3</v>
+        <v>1.0043540567486388E-2</v>
       </c>
       <c r="E20" s="38">
         <f t="shared" ref="E20:E30" si="20">D20/E4</f>
-        <v>1.0196647531486307</v>
+        <v>1.8062457327625761</v>
       </c>
       <c r="F20" s="40">
         <f>E20^2</f>
-        <v>1.039716208813658</v>
+        <v>3.2625236471230155</v>
       </c>
       <c r="G20" s="1">
         <v>4.0483057814126255E-2</v>
@@ -8744,11 +8929,11 @@
       </c>
       <c r="L20" s="38">
         <f t="shared" ref="L20:L27" si="22">K20/N4</f>
-        <v>1.209133081473291</v>
+        <v>1.2609298074327162</v>
       </c>
       <c r="M20" s="40">
         <f>L20^2</f>
-        <v>1.4620028087130963</v>
+        <v>1.5899439792723067</v>
       </c>
       <c r="N20" s="1">
         <v>2.0158404142797091E-2</v>
@@ -8767,11 +8952,11 @@
       </c>
       <c r="S20" s="38">
         <f t="shared" ref="S20:S27" si="24">R20/W4</f>
-        <v>-1.7207798426970529</v>
+        <v>-0.24569793699578096</v>
       </c>
       <c r="T20" s="40">
         <f>S20^2</f>
-        <v>2.9610832670324938</v>
+        <v>6.0367476243982754E-2</v>
       </c>
       <c r="U20" s="1">
         <v>1.8136449430132328E-2</v>
@@ -8805,19 +8990,19 @@
       </c>
       <c r="C21" s="35">
         <f t="shared" ref="C21:C30" si="25">$A$102*B21+$B$102</f>
-        <v>6.080366767290428E-2</v>
+        <v>5.7317845236517062E-2</v>
       </c>
       <c r="D21" s="37">
         <f t="shared" ref="D21:D30" si="26">D5-C21</f>
-        <v>1.6974110104873499E-2</v>
+        <v>2.0459932541260717E-2</v>
       </c>
       <c r="E21" s="39">
         <f t="shared" si="20"/>
-        <v>2.6206650750586462</v>
+        <v>3.6718204935211189</v>
       </c>
       <c r="F21" s="41">
         <f t="shared" ref="F21:F30" si="27">E21^2</f>
-        <v>6.8678854356321395</v>
+        <v>13.482265736641674</v>
       </c>
       <c r="G21" s="1">
         <v>6.0724586721189383E-2</v>
@@ -8836,11 +9021,11 @@
       </c>
       <c r="L21" s="39">
         <f t="shared" si="22"/>
-        <v>1.1899072683584724</v>
+        <v>1.3000629158580779</v>
       </c>
       <c r="M21" s="41">
         <f t="shared" ref="M21" si="29">L21^2</f>
-        <v>1.4158793072923217</v>
+        <v>1.6901635851894077</v>
       </c>
       <c r="N21" s="1">
         <v>4.0316808285594183E-2</v>
@@ -8859,11 +9044,11 @@
       </c>
       <c r="S21" s="43">
         <f t="shared" si="24"/>
-        <v>6.372185901875171</v>
+        <v>1.0695417681690509</v>
       </c>
       <c r="T21" s="41">
         <f t="shared" ref="T21" si="31">S21^2</f>
-        <v>40.604753168056689</v>
+        <v>1.1439195938581799</v>
       </c>
       <c r="U21" s="1">
         <v>3.6272898860264656E-2</v>
@@ -8897,19 +9082,19 @@
       </c>
       <c r="C22" s="35">
         <f t="shared" si="25"/>
-        <v>8.5049967801207035E-2</v>
+        <v>8.2457008818298289E-2</v>
       </c>
       <c r="D22" s="37">
         <f t="shared" si="26"/>
-        <v>5.0558775434851599E-4</v>
+        <v>3.0985467372572628E-3</v>
       </c>
       <c r="E22" s="39">
         <f t="shared" si="20"/>
-        <v>7.6901368227563549E-2</v>
+        <v>0.55573054675190792</v>
       </c>
       <c r="F22" s="41">
         <f t="shared" si="27"/>
-        <v>5.9138204352713209E-3</v>
+        <v>0.3088364405931745</v>
       </c>
       <c r="G22" s="1">
         <v>8.0966115628252511E-2</v>
@@ -8928,11 +9113,11 @@
       </c>
       <c r="L22" s="39">
         <f t="shared" si="22"/>
-        <v>-2.6108012655554322</v>
+        <v>-2.8555505965265673</v>
       </c>
       <c r="M22" s="41">
         <f t="shared" ref="M22:M27" si="32">L22^2</f>
-        <v>6.8162832482258464</v>
+        <v>8.1541692093232339</v>
       </c>
       <c r="N22" s="1">
         <v>6.047521242839126E-2</v>
@@ -8951,11 +9136,11 @@
       </c>
       <c r="S22" s="43">
         <f t="shared" si="24"/>
-        <v>-5.6507852755582038</v>
+        <v>-1.4117816229531766</v>
       </c>
       <c r="T22" s="41">
         <f t="shared" ref="T22:T27" si="33">S22^2</f>
-        <v>31.931374230465405</v>
+        <v>1.9931273509083052</v>
       </c>
       <c r="U22" s="1">
         <v>5.4409348290396994E-2</v>
@@ -8989,19 +9174,19 @@
       </c>
       <c r="C23" s="35">
         <f t="shared" si="25"/>
-        <v>0.10929626792950979</v>
+        <v>0.10759617240007951</v>
       </c>
       <c r="D23" s="37">
         <f t="shared" si="26"/>
-        <v>-7.0740457072875768E-3</v>
+        <v>-5.3739501778573007E-3</v>
       </c>
       <c r="E23" s="39">
         <f t="shared" si="20"/>
-        <v>-1.0424435657054134</v>
+        <v>-0.9623512292795624</v>
       </c>
       <c r="F23" s="41">
         <f t="shared" si="27"/>
-        <v>1.0866885876806165</v>
+        <v>0.92611988849588489</v>
       </c>
       <c r="G23" s="1">
         <v>0.10120764453531564</v>
@@ -9020,11 +9205,11 @@
       </c>
       <c r="L23" s="39">
         <f t="shared" si="22"/>
-        <v>0.90438921879229384</v>
+        <v>1.0772638890504689</v>
       </c>
       <c r="M23" s="41">
         <f t="shared" si="32"/>
-        <v>0.81791985906773557</v>
+        <v>1.1604974866521409</v>
       </c>
       <c r="N23" s="1">
         <v>8.0633616571188366E-2</v>
@@ -9043,11 +9228,11 @@
       </c>
       <c r="S23" s="43">
         <f t="shared" si="24"/>
-        <v>-3.7539577062540768</v>
+        <v>-1.0954802071874588</v>
       </c>
       <c r="T23" s="41">
         <f t="shared" si="33"/>
-        <v>14.092198460344369</v>
+        <v>1.2000768843394776</v>
       </c>
       <c r="U23" s="1">
         <v>7.2545797720529312E-2</v>
@@ -9083,19 +9268,19 @@
       </c>
       <c r="C24" s="35">
         <f t="shared" si="25"/>
-        <v>0.13354256805781253</v>
+        <v>0.13273533598186074</v>
       </c>
       <c r="D24" s="37">
         <f t="shared" si="26"/>
-        <v>-1.9098123613368087E-2</v>
+        <v>-1.8290891537416296E-2</v>
       </c>
       <c r="E24" s="39">
         <f t="shared" si="20"/>
-        <v>-2.7505868956625372</v>
+        <v>-3.2712421069949928</v>
       </c>
       <c r="F24" s="41">
         <f t="shared" si="27"/>
-        <v>7.5657282705904736</v>
+        <v>10.701024922577041</v>
       </c>
       <c r="G24" s="1">
         <v>0.12144917344237877</v>
@@ -9114,11 +9299,11 @@
       </c>
       <c r="L24" s="39">
         <f t="shared" si="22"/>
-        <v>-1.297438251374424</v>
+        <v>-1.5704202302299293</v>
       </c>
       <c r="M24" s="41">
         <f t="shared" si="32"/>
-        <v>1.6833460161295231</v>
+        <v>2.466219699515424</v>
       </c>
       <c r="N24" s="1">
         <v>0.10079202071398545</v>
@@ -9137,11 +9322,11 @@
       </c>
       <c r="S24" s="43">
         <f t="shared" si="24"/>
-        <v>-0.56051497035648723</v>
+        <v>-0.18215122576836973</v>
       </c>
       <c r="T24" s="41">
         <f t="shared" si="33"/>
-        <v>0.31417703199373376</v>
+        <v>3.3179069048919603E-2</v>
       </c>
       <c r="U24" s="1">
         <v>9.0682247150661657E-2</v>
@@ -9191,19 +9376,19 @@
       </c>
       <c r="C25" s="35">
         <f t="shared" si="25"/>
-        <v>0.15778886818611529</v>
+        <v>0.15787449956364197</v>
       </c>
       <c r="D25" s="37">
         <f t="shared" si="26"/>
-        <v>1.3322242924995814E-2</v>
+        <v>1.3236611547469135E-2</v>
       </c>
       <c r="E25" s="39">
         <f t="shared" si="20"/>
-        <v>1.7317893941796991</v>
+        <v>2.3488260052325303</v>
       </c>
       <c r="F25" s="41">
         <f t="shared" si="27"/>
-        <v>2.9990945057932894</v>
+        <v>5.5169836028566062</v>
       </c>
       <c r="G25" s="1">
         <v>0.14169070234944187</v>
@@ -9222,11 +9407,11 @@
       </c>
       <c r="L25" s="39">
         <f t="shared" si="22"/>
-        <v>-1.6106143528777617</v>
+        <v>-2.0233872308255365</v>
       </c>
       <c r="M25" s="41">
         <f t="shared" si="32"/>
-        <v>2.5940785936958508</v>
+        <v>4.0940958858678327</v>
       </c>
       <c r="N25" s="1">
         <v>0.12095042485678252</v>
@@ -9245,11 +9430,11 @@
       </c>
       <c r="S25" s="43">
         <f t="shared" si="24"/>
-        <v>2.6140579505479793</v>
+        <v>0.92840183190766434</v>
       </c>
       <c r="T25" s="41">
         <f t="shared" si="33"/>
-        <v>6.8332989688231018</v>
+        <v>0.86192996148950707</v>
       </c>
       <c r="U25" s="1">
         <v>0.10881869658079399</v>
@@ -9297,19 +9482,19 @@
       </c>
       <c r="C26" s="35">
         <f t="shared" si="25"/>
-        <v>0.18203516831441804</v>
+        <v>0.18301366314542319</v>
       </c>
       <c r="D26" s="37">
         <f t="shared" si="26"/>
-        <v>4.6314983522486308E-3</v>
+        <v>3.6530035212434808E-3</v>
       </c>
       <c r="E26" s="39">
         <f t="shared" si="20"/>
-        <v>0.58600450394169123</v>
+        <v>0.64649570307346571</v>
       </c>
       <c r="F26" s="41">
         <f t="shared" si="27"/>
-        <v>0.34340127863994763</v>
+        <v>0.41795669409245473</v>
       </c>
       <c r="G26" s="1">
         <v>0.16193223125650502</v>
@@ -9328,11 +9513,11 @@
       </c>
       <c r="L26" s="39">
         <f t="shared" si="22"/>
-        <v>1.5915337188104367E-3</v>
+        <v>2.1207097879535949E-3</v>
       </c>
       <c r="M26" s="41">
         <f t="shared" si="32"/>
-        <v>2.5329795781105784E-6</v>
+        <v>4.4974100047221809E-6</v>
       </c>
       <c r="N26" s="1">
         <v>0.14110882899957961</v>
@@ -9351,11 +9536,11 @@
       </c>
       <c r="S26" s="43">
         <f t="shared" si="24"/>
-        <v>4.4577016897717607</v>
+        <v>1.7379215540191553</v>
       </c>
       <c r="T26" s="41">
         <f t="shared" si="33"/>
-        <v>19.87110435499401</v>
+        <v>3.0203713279243556</v>
       </c>
       <c r="U26" s="1">
         <v>0.12695514601092628</v>
@@ -9402,19 +9587,19 @@
       </c>
       <c r="C27" s="35">
         <f t="shared" si="25"/>
-        <v>0.2062814684427208</v>
+        <v>0.20815282672720442</v>
       </c>
       <c r="D27" s="100">
         <f t="shared" si="26"/>
-        <v>-9.6148017760541438E-3</v>
+        <v>-1.1486160060537765E-2</v>
       </c>
       <c r="E27" s="39">
         <f t="shared" si="20"/>
-        <v>-1.195871936483875</v>
+        <v>-2.0290655097657981</v>
       </c>
       <c r="F27" s="41">
         <f t="shared" si="27"/>
-        <v>1.4301096884696931</v>
+        <v>4.1171068429211379</v>
       </c>
       <c r="G27" s="1">
         <v>0.18217376016356815</v>
@@ -9433,11 +9618,11 @@
       </c>
       <c r="L27" s="123">
         <f t="shared" si="22"/>
-        <v>2.5025844811278448</v>
+        <v>3.5723285527667241</v>
       </c>
       <c r="M27" s="116">
         <f t="shared" si="32"/>
-        <v>6.2629290851819244</v>
+        <v>12.761531288912398</v>
       </c>
       <c r="N27" s="1">
         <v>0.16126723314237673</v>
@@ -9456,11 +9641,11 @@
       </c>
       <c r="S27" s="123">
         <f t="shared" si="24"/>
-        <v>-3.701659043393704</v>
+        <v>-1.8158735287968821</v>
       </c>
       <c r="T27" s="116">
         <f t="shared" si="33"/>
-        <v>13.702279673538392</v>
+        <v>3.2973966725852413</v>
       </c>
       <c r="U27" s="1">
         <v>0.14509159544105862</v>
@@ -9507,19 +9692,19 @@
       </c>
       <c r="C28" s="35">
         <f t="shared" si="25"/>
-        <v>0.23052776857102356</v>
+        <v>0.23329199030898565</v>
       </c>
       <c r="D28" s="37">
         <f t="shared" si="26"/>
-        <v>-3.2749990793245781E-2</v>
+        <v>-3.5514212531207873E-2</v>
       </c>
       <c r="E28" s="39">
         <f t="shared" si="20"/>
-        <v>-4.0656945907905806</v>
+        <v>-6.2723857567828825</v>
       </c>
       <c r="F28" s="41">
         <f t="shared" si="27"/>
-        <v>16.529872505583786</v>
+        <v>39.342823081892774</v>
       </c>
       <c r="G28" s="1">
         <v>0.20241528907063128</v>
@@ -9577,19 +9762,19 @@
       </c>
       <c r="C29" s="35">
         <f t="shared" si="25"/>
-        <v>0.25477406869932634</v>
+        <v>0.25843115389076687</v>
       </c>
       <c r="D29" s="37">
         <f t="shared" si="26"/>
-        <v>-1.9218513143770793E-2</v>
+        <v>-2.2875598335211328E-2</v>
       </c>
       <c r="E29" s="39">
         <f t="shared" si="20"/>
-        <v>-2.2406262243721322</v>
+        <v>-4.0090776380084083</v>
       </c>
       <c r="F29" s="41">
         <f t="shared" si="27"/>
-        <v>5.0204058773441167</v>
+        <v>16.072703507579078</v>
       </c>
       <c r="G29" s="1">
         <v>0.22265681797769438</v>
@@ -9647,19 +9832,19 @@
       </c>
       <c r="C30" s="35">
         <f t="shared" si="25"/>
-        <v>0.27902036882762909</v>
+        <v>0.28357031747254813</v>
       </c>
       <c r="D30" s="37">
         <f t="shared" si="26"/>
-        <v>8.7574089501486485E-3</v>
+        <v>4.2074603052296156E-3</v>
       </c>
       <c r="E30" s="39">
         <f t="shared" si="20"/>
-        <v>0.94036359445775897</v>
+        <v>0.72811214139465985</v>
       </c>
       <c r="F30" s="41">
         <f t="shared" si="27"/>
-        <v>0.88428368978151661</v>
+        <v>0.53014729044631714</v>
       </c>
       <c r="G30" s="1">
         <v>0.24289834688475753</v>
@@ -9712,19 +9897,19 @@
       </c>
       <c r="C31" s="35">
         <f>$A$102*B31+$B$102</f>
-        <v>0.32751296908423461</v>
+        <v>0.33384864463611058</v>
       </c>
       <c r="D31" s="37">
         <f>D15-C31</f>
-        <v>2.2487030915765371E-2</v>
+        <v>1.6151355363889397E-2</v>
       </c>
       <c r="E31" s="39">
         <f>D31/E15</f>
-        <v>2.203400445387381</v>
+        <v>2.7456779021882052</v>
       </c>
       <c r="F31" s="41">
         <f>E31^2</f>
-        <v>4.8549735227333093</v>
+        <v>7.5387471425646231</v>
       </c>
       <c r="G31" s="1">
         <v>0.28338140469888373</v>
@@ -9787,19 +9972,19 @@
       </c>
       <c r="C32" s="113">
         <f>$A$102*B32+$B$102</f>
-        <v>0.37600556934084012</v>
+        <v>0.38412697179967303</v>
       </c>
       <c r="D32" s="114">
         <f>D16-C32</f>
-        <v>3.3994430659159858E-2</v>
+        <v>2.5873028200326942E-2</v>
       </c>
       <c r="E32" s="115">
         <f>D32/E16</f>
-        <v>3.0681822325176826</v>
+        <v>4.3124529710022985</v>
       </c>
       <c r="F32" s="116">
         <f>E32^2</f>
-        <v>9.4137422119371905</v>
+        <v>18.597250627106551</v>
       </c>
       <c r="G32" s="1">
         <v>0.32386446251301004</v>
@@ -9928,7 +10113,7 @@
       <c r="F35" s="121"/>
       <c r="G35" s="94">
         <f>SUM(F20:F33)</f>
-        <v>58.041815603435012</v>
+        <v>120.81448942489034</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -9968,18 +10153,18 @@
       </c>
       <c r="D36" s="126">
         <f>SUM(F20:F33)</f>
-        <v>58.041815603435012</v>
+        <v>120.81448942489034</v>
       </c>
       <c r="E36" s="125" t="s">
         <v>20</v>
       </c>
       <c r="F36" s="29">
         <f>SUM(F20:F33)/11</f>
-        <v>5.2765286912213645</v>
+        <v>10.983135402262759</v>
       </c>
       <c r="G36" s="124">
         <f>D36/11</f>
-        <v>5.2765286912213645</v>
+        <v>10.983135402262759</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -9988,18 +10173,18 @@
       </c>
       <c r="K36" s="126">
         <f>SUM(M20:M27)</f>
-        <v>21.052441451285876</v>
+        <v>31.916625632142747</v>
       </c>
       <c r="L36" s="125" t="s">
         <v>20</v>
       </c>
       <c r="M36" s="29">
         <f>SUM(M20:M34)/6</f>
-        <v>3.5087402418809792</v>
+        <v>5.3194376053571242</v>
       </c>
       <c r="N36" s="128">
         <f>K36/6</f>
-        <v>3.5087402418809792</v>
+        <v>5.3194376053571242</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -10008,18 +10193,18 @@
       </c>
       <c r="R36" s="126">
         <f>SUM(T20:T27)</f>
-        <v>130.31026915524819</v>
+        <v>11.610368336397968</v>
       </c>
       <c r="S36" s="125" t="s">
         <v>20</v>
       </c>
       <c r="T36" s="29">
         <f>SUM(T20:T35)/6</f>
-        <v>21.718378192541365</v>
+        <v>1.9350613893996613</v>
       </c>
       <c r="U36" s="128">
         <f>R36/6</f>
-        <v>21.718378192541365</v>
+        <v>1.9350613893996613</v>
       </c>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
@@ -10038,11 +10223,11 @@
       <c r="AJ36" s="1"/>
     </row>
     <row r="37" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="145" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="95">
-        <f>SUM(B20:B33)/13</f>
+        <f>SUM(B20:B32)/13</f>
         <v>8.2307692307692299</v>
       </c>
       <c r="C37" s="96">
@@ -10062,7 +10247,7 @@
         <f>1.47803503*10^-3</f>
         <v>1.47803503E-3</v>
       </c>
-      <c r="H37" s="99" t="s">
+      <c r="H37" s="145" t="s">
         <v>40</v>
       </c>
       <c r="I37" s="95">
@@ -10083,7 +10268,7 @@
         <f>2.46907554*10^-3</f>
         <v>2.4690755399999998E-3</v>
       </c>
-      <c r="O37" s="99" t="s">
+      <c r="O37" s="145" t="s">
         <v>40</v>
       </c>
       <c r="P37" s="95">
@@ -10122,35 +10307,53 @@
     </row>
     <row r="38" spans="1:36" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="B38" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>68</v>
+      </c>
       <c r="E38" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="142">
+      <c r="F38" s="141">
         <v>2.1292993709564399E-3</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="I38" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="J38" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" s="63" t="s">
+        <v>68</v>
+      </c>
       <c r="L38" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="M38" s="142">
+      <c r="M38" s="141">
         <v>1.7083014917976815E-3</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
+      <c r="P38" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q38" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="R38" s="63" t="s">
+        <v>68</v>
+      </c>
       <c r="S38" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="T38" s="142">
+      <c r="T38" s="141">
         <v>1.8023969417446609E-3</v>
       </c>
       <c r="U38" s="1"/>
@@ -10439,15 +10642,15 @@
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="143">
+      <c r="B44" s="142">
         <f>B40/B42</f>
         <v>1.0891882517699914E-3</v>
       </c>
-      <c r="C44" s="144">
+      <c r="C44" s="143">
         <f>C40/C42</f>
         <v>1.1499594240229479E-3</v>
       </c>
-      <c r="D44" s="145">
+      <c r="D44" s="144">
         <f>D40/D42</f>
         <v>1.2798229223944515E-3</v>
       </c>
@@ -11146,7 +11349,7 @@
       </c>
       <c r="C64" s="85">
         <f>D20</f>
-        <v>5.6648546776206996E-3</v>
+        <v>1.0043540567486388E-2</v>
       </c>
       <c r="F64" s="84">
         <v>2</v>
@@ -11177,7 +11380,7 @@
       </c>
       <c r="C65" s="85">
         <f t="shared" ref="C65:C74" si="35">D21</f>
-        <v>1.6974110104873499E-2</v>
+        <v>2.0459932541260717E-2</v>
       </c>
       <c r="F65" s="84">
         <v>4</v>
@@ -11208,7 +11411,7 @@
       </c>
       <c r="C66" s="85">
         <f t="shared" si="35"/>
-        <v>5.0558775434851599E-4</v>
+        <v>3.0985467372572628E-3</v>
       </c>
       <c r="F66" s="84">
         <v>6</v>
@@ -11239,7 +11442,7 @@
       </c>
       <c r="C67" s="85">
         <f t="shared" si="35"/>
-        <v>-7.0740457072875768E-3</v>
+        <v>-5.3739501778573007E-3</v>
       </c>
       <c r="F67" s="84">
         <v>8</v>
@@ -11270,7 +11473,7 @@
       </c>
       <c r="C68" s="85">
         <f t="shared" si="35"/>
-        <v>-1.9098123613368087E-2</v>
+        <v>-1.8290891537416296E-2</v>
       </c>
       <c r="F68" s="84">
         <v>10</v>
@@ -11301,7 +11504,7 @@
       </c>
       <c r="C69" s="85">
         <f t="shared" si="35"/>
-        <v>1.3322242924995814E-2</v>
+        <v>1.3236611547469135E-2</v>
       </c>
       <c r="F69" s="84">
         <v>12</v>
@@ -11332,7 +11535,7 @@
       </c>
       <c r="C70" s="85">
         <f t="shared" si="35"/>
-        <v>4.6314983522486308E-3</v>
+        <v>3.6530035212434808E-3</v>
       </c>
       <c r="F70" s="84">
         <v>14</v>
@@ -11363,7 +11566,7 @@
       </c>
       <c r="C71" s="85">
         <f t="shared" si="35"/>
-        <v>-9.6148017760541438E-3</v>
+        <v>-1.1486160060537765E-2</v>
       </c>
       <c r="F71" s="84">
         <v>16</v>
@@ -11394,7 +11597,7 @@
       </c>
       <c r="C72" s="85">
         <f t="shared" si="35"/>
-        <v>-3.2749990793245781E-2</v>
+        <v>-3.5514212531207873E-2</v>
       </c>
       <c r="H72" s="76"/>
       <c r="I72" s="78"/>
@@ -11411,7 +11614,7 @@
       </c>
       <c r="C73" s="85">
         <f t="shared" si="35"/>
-        <v>-1.9218513143770793E-2</v>
+        <v>-2.2875598335211328E-2</v>
       </c>
       <c r="F73" s="76"/>
       <c r="G73" s="78"/>
@@ -11432,7 +11635,7 @@
       </c>
       <c r="C74" s="85">
         <f t="shared" si="35"/>
-        <v>8.7574089501486485E-3</v>
+        <v>4.2074603052296156E-3</v>
       </c>
       <c r="F74" s="74"/>
       <c r="H74" s="76"/>
@@ -11451,7 +11654,7 @@
       </c>
       <c r="C75" s="85">
         <f>D31</f>
-        <v>2.2487030915765371E-2</v>
+        <v>1.6151355363889397E-2</v>
       </c>
       <c r="F75" s="76"/>
       <c r="G75" s="78"/>
@@ -11472,7 +11675,7 @@
       </c>
       <c r="C76" s="85">
         <f>D32</f>
-        <v>3.3994430659159858E-2</v>
+        <v>2.5873028200326942E-2</v>
       </c>
       <c r="F76" s="74"/>
       <c r="H76" s="75"/>
@@ -11573,12 +11776,12 @@
       <c r="E83" s="74"/>
       <c r="F83" s="74"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="66" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="111" t="s">
         <v>23</v>
       </c>
@@ -11589,7 +11792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <f t="array" ref="A99:B100">LINEST(D4:D16,B4:B16,1,1)</f>
         <v>2.5290580384854128E-2</v>
@@ -11612,7 +11815,7 @@
         <v>-1.1964285714285719E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>1.2750312093211308E-3</v>
       </c>
@@ -11632,12 +11835,12 @@
         <v>9.9752793988224769E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>2.4246300128302756E-2</v>
+        <v>2.5139163581781226E-2</v>
       </c>
       <c r="B102" s="2">
-        <v>-1.1935232712003991E-2</v>
+        <v>-1.8099645508826614E-2</v>
       </c>
       <c r="D102" s="2">
         <v>1.1832898866262154E-2</v>
@@ -11651,8 +11854,11 @@
       <c r="H102" s="2">
         <v>2.1407986212567626E-4</v>
       </c>
+      <c r="K102" s="2">
+        <v>1.8062457327625761</v>
+      </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>1.2750312093211308E-3</v>
       </c>
@@ -11671,70 +11877,63 @@
       <c r="H103" s="2">
         <v>9.9752793988224769E-3</v>
       </c>
+      <c r="K103" s="2">
+        <v>3.6718204935211189</v>
+      </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J105" s="2">
-        <v>1.0196647531486307</v>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K104" s="2">
+        <v>0.55573054675190792</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J106" s="2">
-        <v>2.6206650750586462</v>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K105" s="2">
+        <v>-0.9623512292795624</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J107" s="2">
-        <v>7.6901368227563549E-2</v>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K106" s="2">
+        <v>-3.2712421069949928</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J108" s="2">
-        <v>-1.0424435657054134</v>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K107" s="2">
+        <v>2.3488260052325303</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J109" s="2">
-        <v>-2.7505868956625372</v>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K108" s="2">
+        <v>0.64649570307346571</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J110" s="2">
-        <v>1.7317893941796991</v>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K109" s="2">
+        <v>-2.0290655097657981</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J111" s="2">
-        <v>0.58600450394169123</v>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K110" s="2">
+        <v>-6.2723857567828825</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J112" s="2">
-        <v>-1.195871936483875</v>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K111" s="2">
+        <v>-4.0090776380084083</v>
       </c>
     </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J113" s="2">
-        <v>-4.0656945907905806</v>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K112" s="2">
+        <v>0.72811214139465985</v>
       </c>
     </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J114" s="2">
-        <v>-2.2406262243721322</v>
+    <row r="113" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K113" s="2">
+        <v>2.7456779021882052</v>
       </c>
     </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J115" s="2">
-        <v>0.94036359445775897</v>
-      </c>
-    </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J116" s="2">
-        <v>2.203400445387381</v>
-      </c>
-    </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J117" s="2">
-        <v>3.0681822325176826</v>
+    <row r="114" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K114" s="2">
+        <v>4.3124529710022985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more lab report work - added durbin-watson stuff - started on discussion - more work on the main report
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -42,7 +42,7 @@
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
   <si>
     <t>data</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>^ average V' (cm^3s^-1)</t>
+  </si>
+  <si>
+    <t>Viscosity_LINEST (Pa)</t>
   </si>
 </sst>
 </file>
@@ -1342,9 +1345,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="234">
+  <cellStyleXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2016,7 +2027,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="234">
+  <cellStyles count="242">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2134,6 +2145,10 @@
     <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2250,6 +2265,10 @@
     <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3178,11 +3197,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1996630416"/>
-        <c:axId val="-1996627568"/>
+        <c:axId val="-2046002048"/>
+        <c:axId val="-2002349728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1996630416"/>
+        <c:axId val="-2046002048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3211,12 +3230,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1996627568"/>
+        <c:crossAx val="-2002349728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1996627568"/>
+        <c:axId val="-2002349728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3245,7 +3264,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1996630416"/>
+        <c:crossAx val="-2046002048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3477,11 +3496,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1996609488"/>
-        <c:axId val="-1996607440"/>
+        <c:axId val="-1925179792"/>
+        <c:axId val="-1925178432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1996609488"/>
+        <c:axId val="-1925179792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3538,12 +3557,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1996607440"/>
+        <c:crossAx val="-1925178432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1996607440"/>
+        <c:axId val="-1925178432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3600,7 +3619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1996609488"/>
+        <c:crossAx val="-1925179792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3838,11 +3857,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1977901296"/>
-        <c:axId val="-1977899248"/>
+        <c:axId val="-1922301616"/>
+        <c:axId val="-1923379600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1977901296"/>
+        <c:axId val="-1922301616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3899,12 +3918,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1977899248"/>
+        <c:crossAx val="-1923379600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1977899248"/>
+        <c:axId val="-1923379600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3961,7 +3980,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1977901296"/>
+        <c:crossAx val="-1922301616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4199,11 +4218,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1977908320"/>
-        <c:axId val="-1977906272"/>
+        <c:axId val="-2045834496"/>
+        <c:axId val="-2045832864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1977908320"/>
+        <c:axId val="-2045834496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4260,12 +4279,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1977906272"/>
+        <c:crossAx val="-2045832864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1977906272"/>
+        <c:axId val="-2045832864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4322,7 +4341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1977908320"/>
+        <c:crossAx val="-2045834496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7283,8 +7302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10697,10 +10716,21 @@
       <c r="AJ44" s="1"/>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="97">
+        <f>(PI()*$X$21*$X$22*($X$27)^4)*10^-2/(8*$X$30*$A$102)*10^6</f>
+        <v>9.9520135774371489E-4</v>
+      </c>
+      <c r="C45" s="97">
+        <f>(PI()*$X$21*$X$22*($X$26)^4)*10^-2/(8*$X$29*$D$102)*10^6</f>
+        <v>1.0528184091700831E-3</v>
+      </c>
+      <c r="D45" s="97">
+        <f>(PI()*$X$21*$X$22*($X$25)^4)*10^-2/(8*$X$29*$D$102)*10^6</f>
+        <v>9.6603612060891736E-4</v>
+      </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>

</xml_diff>

<commit_message>
lab report is so difficult
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="84">
   <si>
     <t>data</t>
   </si>
@@ -684,16 +684,53 @@
   <si>
     <t>Viscosity_LINEST (Pa)</t>
   </si>
+  <si>
+    <t>Averaging all viscosities</t>
+  </si>
+  <si>
+    <t>Viscosity_average (Pa)</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Standard Dev</t>
+  </si>
+  <si>
+    <t>1 sigma</t>
+  </si>
+  <si>
+    <t>2 sigma</t>
+  </si>
+  <si>
+    <t>3 sigma</t>
+  </si>
+  <si>
+    <t>(-)1 sigma</t>
+  </si>
+  <si>
+    <t>(-)2 sigma</t>
+  </si>
+  <si>
+    <t>(-)3 sigma</t>
+  </si>
+  <si>
+    <t>non-LINEST</t>
+  </si>
+  <si>
+    <t>LINEST</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1345,7 +1382,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="242">
+  <cellStyleXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1588,8 +1625,36 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2026,8 +2091,14 @@
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="9" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="242">
+  <cellStyles count="270">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2149,6 +2220,20 @@
     <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2269,6 +2354,20 @@
     <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2624,43 +2723,43 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.0321786816547358</c:v>
+                  <c:v>0.0321779832178224</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0573178452365171</c:v>
+                  <c:v>0.0573172176151192</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0824570088182983</c:v>
+                  <c:v>0.082456452012416</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10759617240008</c:v>
+                  <c:v>0.107595686409713</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.132735335981861</c:v>
+                  <c:v>0.13273492080701</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.157874499563642</c:v>
+                  <c:v>0.157874155204306</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.183013663145423</c:v>
+                  <c:v>0.183013389601603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.208152826727204</c:v>
+                  <c:v>0.2081526239989</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.233291990308986</c:v>
+                  <c:v>0.233291858396197</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.258431153890767</c:v>
+                  <c:v>0.258431092793494</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.283570317472548</c:v>
+                  <c:v>0.283570327190791</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.333848644636111</c:v>
+                  <c:v>0.333848795985384</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.384126971799673</c:v>
+                  <c:v>0.384127264779978</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3448,40 +3547,40 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0100435405674864</c:v>
+                  <c:v>0.0100442390043998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0204599325412607</c:v>
+                  <c:v>0.0204605601626586</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00309854673725726</c:v>
+                  <c:v>0.00309910354313951</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.0053739501778573</c:v>
+                  <c:v>-0.00537346418749064</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0182908915374163</c:v>
+                  <c:v>-0.0182904763625652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0132366115474691</c:v>
+                  <c:v>0.0132369559068046</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00365300352124348</c:v>
+                  <c:v>0.00365327706506335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.0114861600605378</c:v>
+                  <c:v>-0.0114859573322335</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0355142125312079</c:v>
+                  <c:v>-0.0355140806184192</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.0228755983352113</c:v>
+                  <c:v>-0.0228755372379382</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.00420746030522961</c:v>
+                  <c:v>0.00420745058698707</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0161513553638894</c:v>
+                  <c:v>0.0161512040146157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7302,8 +7401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8917,19 +9016,19 @@
       </c>
       <c r="C20" s="35">
         <f>$A$102*B20+$B$102</f>
-        <v>3.2178681654735836E-2</v>
+        <v>3.2177983217822392E-2</v>
       </c>
       <c r="D20" s="36">
         <f>D4-C20</f>
-        <v>1.0043540567486388E-2</v>
+        <v>1.0044239004399831E-2</v>
       </c>
       <c r="E20" s="38">
         <f t="shared" ref="E20:E30" si="20">D20/E4</f>
-        <v>1.8062457327625761</v>
+        <v>1.8063713407278184</v>
       </c>
       <c r="F20" s="40">
         <f>E20^2</f>
-        <v>3.2625236471230155</v>
+        <v>3.2629774206028159</v>
       </c>
       <c r="G20" s="1">
         <v>4.0483057814126255E-2</v>
@@ -9009,19 +9108,19 @@
       </c>
       <c r="C21" s="35">
         <f t="shared" ref="C21:C30" si="25">$A$102*B21+$B$102</f>
-        <v>5.7317845236517062E-2</v>
+        <v>5.7317217615119223E-2</v>
       </c>
       <c r="D21" s="37">
         <f t="shared" ref="D21:D30" si="26">D5-C21</f>
-        <v>2.0459932541260717E-2</v>
+        <v>2.0460560162658556E-2</v>
       </c>
       <c r="E21" s="39">
         <f t="shared" si="20"/>
-        <v>3.6718204935211189</v>
+        <v>3.6719331289418911</v>
       </c>
       <c r="F21" s="41">
         <f t="shared" ref="F21:F30" si="27">E21^2</f>
-        <v>13.482265736641674</v>
+        <v>13.483092903420987</v>
       </c>
       <c r="G21" s="1">
         <v>6.0724586721189383E-2</v>
@@ -9101,19 +9200,19 @@
       </c>
       <c r="C22" s="35">
         <f t="shared" si="25"/>
-        <v>8.2457008818298289E-2</v>
+        <v>8.245645201241604E-2</v>
       </c>
       <c r="D22" s="37">
         <f t="shared" si="26"/>
-        <v>3.0985467372572628E-3</v>
+        <v>3.0991035431395114E-3</v>
       </c>
       <c r="E22" s="39">
         <f t="shared" si="20"/>
-        <v>0.55573054675190792</v>
+        <v>0.55583041099912289</v>
       </c>
       <c r="F22" s="41">
         <f t="shared" si="27"/>
-        <v>0.3088364405931745</v>
+        <v>0.30894744579145389</v>
       </c>
       <c r="G22" s="1">
         <v>8.0966115628252511E-2</v>
@@ -9193,19 +9292,19 @@
       </c>
       <c r="C23" s="35">
         <f t="shared" si="25"/>
-        <v>0.10759617240007951</v>
+        <v>0.10759568640971286</v>
       </c>
       <c r="D23" s="37">
         <f t="shared" si="26"/>
-        <v>-5.3739501778573007E-3</v>
+        <v>-5.3734641874906425E-3</v>
       </c>
       <c r="E23" s="39">
         <f t="shared" si="20"/>
-        <v>-0.9623512292795624</v>
+        <v>-0.96226419955072373</v>
       </c>
       <c r="F23" s="41">
         <f t="shared" si="27"/>
-        <v>0.92611988849588489</v>
+        <v>0.92595238973699501</v>
       </c>
       <c r="G23" s="1">
         <v>0.10120764453531564</v>
@@ -9287,19 +9386,19 @@
       </c>
       <c r="C24" s="35">
         <f t="shared" si="25"/>
-        <v>0.13273533598186074</v>
+        <v>0.13273492080700969</v>
       </c>
       <c r="D24" s="37">
         <f t="shared" si="26"/>
-        <v>-1.8290891537416296E-2</v>
+        <v>-1.8290476362565242E-2</v>
       </c>
       <c r="E24" s="39">
         <f t="shared" si="20"/>
-        <v>-3.2712421069949928</v>
+        <v>-3.2711678548760212</v>
       </c>
       <c r="F24" s="41">
         <f t="shared" si="27"/>
-        <v>10.701024922577041</v>
+        <v>10.700539134774191</v>
       </c>
       <c r="G24" s="1">
         <v>0.12144917344237877</v>
@@ -9395,19 +9494,19 @@
       </c>
       <c r="C25" s="35">
         <f t="shared" si="25"/>
-        <v>0.15787449956364197</v>
+        <v>0.1578741552043065</v>
       </c>
       <c r="D25" s="37">
         <f t="shared" si="26"/>
-        <v>1.3236611547469135E-2</v>
+        <v>1.3236955906804598E-2</v>
       </c>
       <c r="E25" s="39">
         <f t="shared" si="20"/>
-        <v>2.3488260052325303</v>
+        <v>2.3488871115178798</v>
       </c>
       <c r="F25" s="41">
         <f t="shared" si="27"/>
-        <v>5.5169836028566062</v>
+        <v>5.5172706626548083</v>
       </c>
       <c r="G25" s="1">
         <v>0.14169070234944187</v>
@@ -9501,19 +9600,19 @@
       </c>
       <c r="C26" s="35">
         <f t="shared" si="25"/>
-        <v>0.18301366314542319</v>
+        <v>0.18301338960160332</v>
       </c>
       <c r="D26" s="37">
         <f t="shared" si="26"/>
-        <v>3.6530035212434808E-3</v>
+        <v>3.6532770650633539E-3</v>
       </c>
       <c r="E26" s="39">
         <f t="shared" si="20"/>
-        <v>0.64649570307346571</v>
+        <v>0.64654411389571698</v>
       </c>
       <c r="F26" s="41">
         <f t="shared" si="27"/>
-        <v>0.41795669409245473</v>
+        <v>0.41801929121319786</v>
       </c>
       <c r="G26" s="1">
         <v>0.16193223125650502</v>
@@ -9606,19 +9705,19 @@
       </c>
       <c r="C27" s="35">
         <f t="shared" si="25"/>
-        <v>0.20815282672720442</v>
+        <v>0.20815262399890014</v>
       </c>
       <c r="D27" s="100">
         <f t="shared" si="26"/>
-        <v>-1.1486160060537765E-2</v>
+        <v>-1.1485957332233482E-2</v>
       </c>
       <c r="E27" s="39">
         <f t="shared" si="20"/>
-        <v>-2.0290655097657981</v>
+        <v>-2.0290296971871902</v>
       </c>
       <c r="F27" s="41">
         <f t="shared" si="27"/>
-        <v>4.1171068429211379</v>
+        <v>4.1169615120675402</v>
       </c>
       <c r="G27" s="1">
         <v>0.18217376016356815</v>
@@ -9711,19 +9810,19 @@
       </c>
       <c r="C28" s="35">
         <f t="shared" si="25"/>
-        <v>0.23329199030898565</v>
+        <v>0.23329185839619695</v>
       </c>
       <c r="D28" s="37">
         <f t="shared" si="26"/>
-        <v>-3.5514212531207873E-2</v>
+        <v>-3.551408061841918E-2</v>
       </c>
       <c r="E28" s="39">
         <f t="shared" si="20"/>
-        <v>-6.2723857567828825</v>
+        <v>-6.2723624588455795</v>
       </c>
       <c r="F28" s="41">
         <f t="shared" si="27"/>
-        <v>39.342823081892774</v>
+        <v>39.342530815135362</v>
       </c>
       <c r="G28" s="1">
         <v>0.20241528907063128</v>
@@ -9781,19 +9880,19 @@
       </c>
       <c r="C29" s="35">
         <f t="shared" si="25"/>
-        <v>0.25843115389076687</v>
+        <v>0.2584310927934938</v>
       </c>
       <c r="D29" s="37">
         <f t="shared" si="26"/>
-        <v>-2.2875598335211328E-2</v>
+        <v>-2.2875537237938254E-2</v>
       </c>
       <c r="E29" s="39">
         <f t="shared" si="20"/>
-        <v>-4.0090776380084083</v>
+        <v>-4.009066930366683</v>
       </c>
       <c r="F29" s="41">
         <f t="shared" si="27"/>
-        <v>16.072703507579078</v>
+        <v>16.072617652159739</v>
       </c>
       <c r="G29" s="1">
         <v>0.22265681797769438</v>
@@ -9851,19 +9950,19 @@
       </c>
       <c r="C30" s="35">
         <f t="shared" si="25"/>
-        <v>0.28357031747254813</v>
+        <v>0.28357032719079067</v>
       </c>
       <c r="D30" s="37">
         <f t="shared" si="26"/>
-        <v>4.2074603052296156E-3</v>
+        <v>4.2074505869870715E-3</v>
       </c>
       <c r="E30" s="39">
         <f t="shared" si="20"/>
-        <v>0.72811214139465985</v>
+        <v>0.728110459627067</v>
       </c>
       <c r="F30" s="41">
         <f t="shared" si="27"/>
-        <v>0.53014729044631714</v>
+        <v>0.53014484141833873</v>
       </c>
       <c r="G30" s="1">
         <v>0.24289834688475753</v>
@@ -9916,19 +10015,19 @@
       </c>
       <c r="C31" s="35">
         <f>$A$102*B31+$B$102</f>
-        <v>0.33384864463611058</v>
+        <v>0.33384879598538431</v>
       </c>
       <c r="D31" s="37">
         <f>D15-C31</f>
-        <v>1.6151355363889397E-2</v>
+        <v>1.6151204014615672E-2</v>
       </c>
       <c r="E31" s="39">
         <f>D31/E15</f>
-        <v>2.7456779021882052</v>
+        <v>2.7456521733037236</v>
       </c>
       <c r="F31" s="41">
         <f>E31^2</f>
-        <v>7.5387471425646231</v>
+        <v>7.5386058567674601</v>
       </c>
       <c r="G31" s="1">
         <v>0.28338140469888373</v>
@@ -9952,7 +10051,7 @@
         <v>4</v>
       </c>
       <c r="X31" s="12">
-        <v>1.2359999999999999E-3</v>
+        <v>1.307E-3</v>
       </c>
       <c r="Y31" s="8" t="s">
         <v>8</v>
@@ -9991,19 +10090,19 @@
       </c>
       <c r="C32" s="113">
         <f>$A$102*B32+$B$102</f>
-        <v>0.38412697179967303</v>
+        <v>0.38412726477997794</v>
       </c>
       <c r="D32" s="114">
         <f>D16-C32</f>
-        <v>2.5873028200326942E-2</v>
+        <v>2.5872735220022036E-2</v>
       </c>
       <c r="E32" s="115">
         <f>D32/E16</f>
-        <v>4.3124529710022985</v>
+        <v>4.3124041377626581</v>
       </c>
       <c r="F32" s="116">
         <f>E32^2</f>
-        <v>18.597250627106551</v>
+        <v>18.596829447392494</v>
       </c>
       <c r="G32" s="1">
         <v>0.32386446251301004</v>
@@ -10132,7 +10231,7 @@
       <c r="F35" s="121"/>
       <c r="G35" s="94">
         <f>SUM(F20:F33)</f>
-        <v>120.81448942489034</v>
+        <v>120.81448937313539</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -10172,18 +10271,18 @@
       </c>
       <c r="D36" s="126">
         <f>SUM(F20:F33)</f>
-        <v>120.81448942489034</v>
+        <v>120.81448937313539</v>
       </c>
       <c r="E36" s="125" t="s">
         <v>20</v>
       </c>
       <c r="F36" s="29">
         <f>SUM(F20:F33)/11</f>
-        <v>10.983135402262759</v>
+        <v>10.983135397557762</v>
       </c>
       <c r="G36" s="124">
         <f>D36/11</f>
-        <v>10.983135402262759</v>
+        <v>10.983135397557762</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -10503,7 +10602,9 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
+      <c r="P41" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="Q41" s="63" t="s">
         <v>56</v>
       </c>
@@ -10721,7 +10822,7 @@
       </c>
       <c r="B45" s="97">
         <f>(PI()*$X$21*$X$22*($X$27)^4)*10^-2/(8*$X$30*$A$102)*10^6</f>
-        <v>9.9520135774371489E-4</v>
+        <v>9.9519855432909378E-4</v>
       </c>
       <c r="C45" s="97">
         <f>(PI()*$X$21*$X$22*($X$26)^4)*10^-2/(8*$X$29*$D$102)*10^6</f>
@@ -10781,9 +10882,11 @@
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="B46" s="147">
+        <v>1</v>
+      </c>
+      <c r="C46" s="147"/>
+      <c r="D46" s="147"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -10896,18 +10999,26 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="P48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q48" s="63" t="s">
+        <v>56</v>
+      </c>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
+      <c r="V48" s="63" t="s">
+        <v>60</v>
+      </c>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
-      <c r="AA48" s="1"/>
+      <c r="AA48" s="63" t="s">
+        <v>61</v>
+      </c>
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
@@ -10937,20 +11048,35 @@
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="Q49" s="110" t="s">
+        <v>59</v>
+      </c>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
+      <c r="T49" s="146">
+        <f>B45*SQRT((T42/(X21*X22))^2+(T43/(B37*10^-2*X27^4))^2+(Y30/X30)^2+(A103/A102)^2)</f>
+        <v>2.3365869480949361E-4</v>
+      </c>
       <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
+      <c r="V49" s="110" t="s">
+        <v>59</v>
+      </c>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
+      <c r="Y49" s="146">
+        <f>C45*SQRT((Y42/(X21*X22))^2+(Y43/(I37*10^-2*X26^4))^2+(Y29/X29)^2+(D103/D102)^2)</f>
+        <v>2.9088877216567856E-4</v>
+      </c>
       <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
+      <c r="AA49" s="110" t="s">
+        <v>59</v>
+      </c>
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
+      <c r="AD49" s="146">
+        <f>D45*SQRT((AD42/(X21*X22))^2 + (AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(G103/G102)^2)</f>
+        <v>2.8200689959286018E-4</v>
+      </c>
       <c r="AE49" s="1"/>
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
@@ -10997,10 +11123,18 @@
       <c r="AJ50" s="1"/>
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -11036,9 +11170,18 @@
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
+      <c r="B52" s="97">
+        <f>SUM(B45:D45)/3</f>
+        <v>1.0046843613693648E-3</v>
+      </c>
+      <c r="C52" s="97">
+        <f>STDEV(B45:D45)/SQRT(3)</f>
+        <v>2.5496907024070581E-5</v>
+      </c>
+      <c r="D52" s="1">
+        <f>STDEV(B45:D45)</f>
+        <v>4.4161938401550028E-5</v>
+      </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -11074,7 +11217,10 @@
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="B53" s="97">
+        <f>ABS(B44-$X$31)/D52</f>
+        <v>4.9321147602154092</v>
+      </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -11150,9 +11296,15 @@
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+      <c r="B55" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="99" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="99" t="s">
+        <v>78</v>
+      </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -11188,9 +11340,18 @@
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+      <c r="B56" s="97">
+        <f>$B$52+1*$C$52</f>
+        <v>1.0301812683934353E-3</v>
+      </c>
+      <c r="C56" s="97">
+        <f>$B$52+2*$C$52</f>
+        <v>1.055678175417506E-3</v>
+      </c>
+      <c r="D56" s="97">
+        <f>$B$52+3*$C$52</f>
+        <v>1.0811750824415765E-3</v>
+      </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -11226,9 +11387,15 @@
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="B57" s="99" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="99" t="s">
+        <v>81</v>
+      </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -11263,6 +11430,18 @@
       <c r="AJ57" s="1"/>
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B58" s="97">
+        <f>$B$52-1*$C$52</f>
+        <v>9.7918745434529431E-4</v>
+      </c>
+      <c r="C58" s="97">
+        <f>$B$52-2*$C$52</f>
+        <v>9.536905473212237E-4</v>
+      </c>
+      <c r="D58" s="97">
+        <f>$B$52-3*$C$52</f>
+        <v>9.2819364029715309E-4</v>
+      </c>
       <c r="F58" s="74"/>
       <c r="G58" s="74"/>
       <c r="H58" s="74"/>
@@ -11379,7 +11558,7 @@
       </c>
       <c r="C64" s="85">
         <f>D20</f>
-        <v>1.0043540567486388E-2</v>
+        <v>1.0044239004399831E-2</v>
       </c>
       <c r="F64" s="84">
         <v>2</v>
@@ -11410,7 +11589,7 @@
       </c>
       <c r="C65" s="85">
         <f t="shared" ref="C65:C74" si="35">D21</f>
-        <v>2.0459932541260717E-2</v>
+        <v>2.0460560162658556E-2</v>
       </c>
       <c r="F65" s="84">
         <v>4</v>
@@ -11441,7 +11620,7 @@
       </c>
       <c r="C66" s="85">
         <f t="shared" si="35"/>
-        <v>3.0985467372572628E-3</v>
+        <v>3.0991035431395114E-3</v>
       </c>
       <c r="F66" s="84">
         <v>6</v>
@@ -11472,7 +11651,7 @@
       </c>
       <c r="C67" s="85">
         <f t="shared" si="35"/>
-        <v>-5.3739501778573007E-3</v>
+        <v>-5.3734641874906425E-3</v>
       </c>
       <c r="F67" s="84">
         <v>8</v>
@@ -11503,7 +11682,7 @@
       </c>
       <c r="C68" s="85">
         <f t="shared" si="35"/>
-        <v>-1.8290891537416296E-2</v>
+        <v>-1.8290476362565242E-2</v>
       </c>
       <c r="F68" s="84">
         <v>10</v>
@@ -11534,7 +11713,7 @@
       </c>
       <c r="C69" s="85">
         <f t="shared" si="35"/>
-        <v>1.3236611547469135E-2</v>
+        <v>1.3236955906804598E-2</v>
       </c>
       <c r="F69" s="84">
         <v>12</v>
@@ -11565,7 +11744,7 @@
       </c>
       <c r="C70" s="85">
         <f t="shared" si="35"/>
-        <v>3.6530035212434808E-3</v>
+        <v>3.6532770650633539E-3</v>
       </c>
       <c r="F70" s="84">
         <v>14</v>
@@ -11596,7 +11775,7 @@
       </c>
       <c r="C71" s="85">
         <f t="shared" si="35"/>
-        <v>-1.1486160060537765E-2</v>
+        <v>-1.1485957332233482E-2</v>
       </c>
       <c r="F71" s="84">
         <v>16</v>
@@ -11627,7 +11806,7 @@
       </c>
       <c r="C72" s="85">
         <f t="shared" si="35"/>
-        <v>-3.5514212531207873E-2</v>
+        <v>-3.551408061841918E-2</v>
       </c>
       <c r="H72" s="76"/>
       <c r="I72" s="78"/>
@@ -11644,7 +11823,7 @@
       </c>
       <c r="C73" s="85">
         <f t="shared" si="35"/>
-        <v>-2.2875598335211328E-2</v>
+        <v>-2.2875537237938254E-2</v>
       </c>
       <c r="F73" s="76"/>
       <c r="G73" s="78"/>
@@ -11665,7 +11844,7 @@
       </c>
       <c r="C74" s="85">
         <f t="shared" si="35"/>
-        <v>4.2074603052296156E-3</v>
+        <v>4.2074505869870715E-3</v>
       </c>
       <c r="F74" s="74"/>
       <c r="H74" s="76"/>
@@ -11684,7 +11863,7 @@
       </c>
       <c r="C75" s="85">
         <f>D31</f>
-        <v>1.6151355363889397E-2</v>
+        <v>1.6151204014615672E-2</v>
       </c>
       <c r="F75" s="76"/>
       <c r="G75" s="78"/>
@@ -11705,7 +11884,7 @@
       </c>
       <c r="C76" s="85">
         <f>D32</f>
-        <v>2.5873028200326942E-2</v>
+        <v>2.5872735220022036E-2</v>
       </c>
       <c r="F76" s="74"/>
       <c r="H76" s="75"/>
@@ -11867,10 +12046,10 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>2.5139163581781226E-2</v>
+        <v>2.5139234397296824E-2</v>
       </c>
       <c r="B102" s="2">
-        <v>-1.8099645508826614E-2</v>
+        <v>-1.8100485576771259E-2</v>
       </c>
       <c r="D102" s="2">
         <v>1.1832898866262154E-2</v>

</xml_diff>

<commit_message>
more lab report and cp7 cp7: - commented on a few things - renamed a few variables
lab report:
- more discussion
- rejiggled the intro and method a bit
- started on diagram for method
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -1382,7 +1382,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="270">
+  <cellStyleXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1653,8 +1653,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2097,8 +2101,11 @@
     <xf numFmtId="168" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="16" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="270">
+  <cellStyles count="274">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2234,6 +2241,8 @@
     <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2368,6 +2377,8 @@
     <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7401,8 +7412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10883,10 +10894,16 @@
     <row r="46" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="147">
-        <v>1</v>
-      </c>
-      <c r="C46" s="147"/>
-      <c r="D46" s="147"/>
+        <f>1*10^-3</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C46" s="147">
+        <f>1.1*10^-3</f>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D46" s="148">
+        <v>1E-3</v>
+      </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -11175,8 +11192,8 @@
         <v>1.0046843613693648E-3</v>
       </c>
       <c r="C52" s="97">
-        <f>STDEV(B45:D45)/SQRT(3)</f>
-        <v>2.5496907024070581E-5</v>
+        <f>STDEV(B46:D46)/SQRT(3)</f>
+        <v>3.3333333333333348E-5</v>
       </c>
       <c r="D52" s="1">
         <f>STDEV(B45:D45)</f>
@@ -11218,8 +11235,8 @@
     <row r="53" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="97">
-        <f>ABS(B44-$X$31)/D52</f>
-        <v>4.9321147602154092</v>
+        <f>ABS(B52-$X$31)/C52</f>
+        <v>9.0694691589190519</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -11342,15 +11359,15 @@
       <c r="A56" s="1"/>
       <c r="B56" s="97">
         <f>$B$52+1*$C$52</f>
-        <v>1.0301812683934353E-3</v>
+        <v>1.0380176947026982E-3</v>
       </c>
       <c r="C56" s="97">
         <f>$B$52+2*$C$52</f>
-        <v>1.055678175417506E-3</v>
+        <v>1.0713510280360315E-3</v>
       </c>
       <c r="D56" s="97">
         <f>$B$52+3*$C$52</f>
-        <v>1.0811750824415765E-3</v>
+        <v>1.1046843613693649E-3</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -11432,15 +11449,15 @@
     <row r="58" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B58" s="97">
         <f>$B$52-1*$C$52</f>
-        <v>9.7918745434529431E-4</v>
+        <v>9.7135102803603147E-4</v>
       </c>
       <c r="C58" s="97">
         <f>$B$52-2*$C$52</f>
-        <v>9.536905473212237E-4</v>
+        <v>9.3801769470269812E-4</v>
       </c>
       <c r="D58" s="97">
         <f>$B$52-3*$C$52</f>
-        <v>9.2819364029715309E-4</v>
+        <v>9.0468436136936477E-4</v>
       </c>
       <c r="F58" s="74"/>
       <c r="G58" s="74"/>

</xml_diff>

<commit_message>
hate programming, hate labreport
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/data/viscosity_of_water.xlsx
@@ -7455,8 +7455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64:D76"/>
+    <sheetView tabSelected="1" topLeftCell="Q31" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25:Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9624,7 +9624,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Z25" s="1">
-        <v>3.0000000000000001E-5</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="AA25" s="1"/>
       <c r="AB25" s="54">
@@ -9729,7 +9729,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Z26" s="1">
-        <v>3.0000000000000001E-5</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="AA26" s="1"/>
       <c r="AB26" s="54">
@@ -9834,7 +9834,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Z27" s="1">
-        <v>3.0000000000000001E-5</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="AA27" s="1"/>
       <c r="AB27" s="54">
@@ -10779,7 +10779,7 @@
       </c>
       <c r="T43" s="63">
         <f>B37*10^-2*(X27^4)*SQRT((0.5/B37)^2+(S44/X27^4)^2)</f>
-        <v>1.705778781104631E-15</v>
+        <v>1.6439098983178802E-14</v>
       </c>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
@@ -10791,7 +10791,7 @@
       </c>
       <c r="Y43" s="66">
         <f>I37*10^-2*X26^4*SQRT((0.5/I37)^2+(X44/X26^4)^2)</f>
-        <v>1.1475259877793456E-15</v>
+        <v>1.1215538141975641E-14</v>
       </c>
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
@@ -10803,7 +10803,7 @@
       </c>
       <c r="AD43" s="66">
         <f>P37*10^-2*X25^4*SQRT((0.5/P37)^2+(AC44/X25^4)^2)</f>
-        <v>1.0748027821555357E-15</v>
+        <v>1.0514671560515991E-14</v>
       </c>
       <c r="AE43" s="1"/>
       <c r="AF43" s="1"/>
@@ -10844,7 +10844,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1">
         <f>X27^4*ABS(4*Z27/X27)</f>
-        <v>1.9965000000000003E-14</v>
+        <v>1.9965000000000001E-13</v>
       </c>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
@@ -10852,7 +10852,7 @@
       <c r="W44" s="1"/>
       <c r="X44" s="110">
         <f>X26^4*ABS(4*Z26/X26)</f>
-        <v>1.2458760000000002E-14</v>
+        <v>1.2458760000000001E-13</v>
       </c>
       <c r="Y44" s="110"/>
       <c r="Z44" s="1"/>
@@ -10860,7 +10860,7 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="110">
         <f>X25^4*ABS(4*Z25/X25)</f>
-        <v>1.1680320000000001E-14</v>
+        <v>1.168032E-13</v>
       </c>
       <c r="AD44" s="110"/>
       <c r="AE44" s="1"/>
@@ -10966,7 +10966,7 @@
       <c r="S46" s="1"/>
       <c r="T46" s="97">
         <f>B44*SQRT((T42/(X21*X22))^2+(T43/(B37*10^-2*X27^4))^2+(Y30/X30)^2+(D37/C37)^2)</f>
-        <v>3.0522491032608002E-4</v>
+        <v>2.3841176416662803E-3</v>
       </c>
       <c r="U46" s="1"/>
       <c r="V46" s="1" t="s">
@@ -10976,7 +10976,7 @@
       <c r="X46" s="1"/>
       <c r="Y46" s="97">
         <f>C44*SQRT((Y42/(X21*X22))^2+(Y43/(I37*10^-2*X26^4))^2+(Y29/X29)^2+(K37/J37)^2)</f>
-        <v>3.9486222382218242E-4</v>
+        <v>2.947914257418379E-3</v>
       </c>
       <c r="Z46" s="1"/>
       <c r="AA46" s="1" t="s">
@@ -10986,15 +10986,15 @@
       <c r="AC46" s="1"/>
       <c r="AD46" s="97">
         <f>D44*SQRT((AD42/(X21*X22))^2 + (AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(R37/Q37)^2)</f>
-        <v>4.2318461798020342E-4</v>
+        <v>3.3487796964455311E-3</v>
       </c>
       <c r="AE46" s="97">
         <f>T38*SQRT((AD42/(X21*X22))^2+(AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(R37/Q37)^2)</f>
-        <v>5.9597827784945454E-4</v>
+        <v>4.7161448492870081E-3</v>
       </c>
       <c r="AF46" s="1">
         <f>T38*SQRT((AD42/(X21*X22))^2+(AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(R37/Q37)^2)</f>
-        <v>5.9597827784945454E-4</v>
+        <v>4.7161448492870081E-3</v>
       </c>
       <c r="AG46" s="1"/>
       <c r="AH46" s="1"/>
@@ -11115,7 +11115,7 @@
       <c r="S49" s="1"/>
       <c r="T49" s="146">
         <f>B45*SQRT((T42/(X21*X22))^2+(T43/(B37*10^-2*X27^4))^2+(Y30/X30)^2+(A103/A102)^2)</f>
-        <v>2.3365869480949361E-4</v>
+        <v>2.1730569475085712E-3</v>
       </c>
       <c r="U49" s="1"/>
       <c r="V49" s="110" t="s">
@@ -11125,7 +11125,7 @@
       <c r="X49" s="1"/>
       <c r="Y49" s="146">
         <f>C45*SQRT((Y42/(X21*X22))^2+(Y43/(I37*10^-2*X26^4))^2+(Y29/X29)^2+(D103/D102)^2)</f>
-        <v>2.9088877216567856E-4</v>
+        <v>2.6903451445138972E-3</v>
       </c>
       <c r="Z49" s="1"/>
       <c r="AA49" s="110" t="s">
@@ -11135,7 +11135,7 @@
       <c r="AC49" s="1"/>
       <c r="AD49" s="146">
         <f>D45*SQRT((AD42/(X21*X22))^2 + (AD43/(P37*10^-2*X25^4))^2+(Y28/X28)^2+(G103/G102)^2)</f>
-        <v>2.8200689959286018E-4</v>
+        <v>2.5232705084111376E-3</v>
       </c>
       <c r="AE49" s="1"/>
       <c r="AF49" s="1"/>

</xml_diff>